<commit_message>
floor change + other things
</commit_message>
<xml_diff>
--- a/01_doc/Planning.xlsx
+++ b/01_doc/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naily\Documents\01_HEIG\01_TB\01_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074598B6-1C47-4757-A296-8A3BD9E0174E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E537B2C-EDC9-4061-BA05-523CA82A7EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22236" windowHeight="13176" xr2:uid="{F59D9D10-3A89-4134-8555-53CD5E65A538}"/>
   </bookViews>
@@ -1080,6 +1080,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1120,42 +1156,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1477,8 +1477,8 @@
   </sheetPr>
   <dimension ref="A1:BQ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD47" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BO28" sqref="BO28"/>
+    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG46" sqref="AG46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1525,280 +1525,280 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:68" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="90" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="82"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
-      <c r="AM1" s="82"/>
-      <c r="AN1" s="82"/>
-      <c r="AO1" s="82"/>
-      <c r="AP1" s="82"/>
-      <c r="AQ1" s="82"/>
-      <c r="AR1" s="82"/>
-      <c r="AS1" s="82"/>
-      <c r="AT1" s="82"/>
-      <c r="AU1" s="82"/>
-      <c r="AV1" s="82"/>
-      <c r="AW1" s="82"/>
-      <c r="AX1" s="82"/>
-      <c r="AY1" s="82"/>
-      <c r="AZ1" s="82"/>
-      <c r="BA1" s="82"/>
-      <c r="BB1" s="82"/>
-      <c r="BC1" s="82"/>
-      <c r="BD1" s="82"/>
-      <c r="BE1" s="82"/>
-      <c r="BF1" s="82"/>
-      <c r="BG1" s="82"/>
-      <c r="BH1" s="82"/>
-      <c r="BI1" s="82"/>
-      <c r="BJ1" s="82"/>
-      <c r="BK1" s="82"/>
-      <c r="BL1" s="82"/>
-      <c r="BM1" s="82"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="94"/>
+      <c r="U1" s="94"/>
+      <c r="V1" s="94"/>
+      <c r="W1" s="94"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="94"/>
+      <c r="Z1" s="94"/>
+      <c r="AA1" s="94"/>
+      <c r="AB1" s="94"/>
+      <c r="AC1" s="94"/>
+      <c r="AD1" s="94"/>
+      <c r="AE1" s="94"/>
+      <c r="AF1" s="94"/>
+      <c r="AG1" s="94"/>
+      <c r="AH1" s="94"/>
+      <c r="AI1" s="94"/>
+      <c r="AJ1" s="94"/>
+      <c r="AK1" s="94"/>
+      <c r="AL1" s="94"/>
+      <c r="AM1" s="94"/>
+      <c r="AN1" s="94"/>
+      <c r="AO1" s="94"/>
+      <c r="AP1" s="94"/>
+      <c r="AQ1" s="94"/>
+      <c r="AR1" s="94"/>
+      <c r="AS1" s="94"/>
+      <c r="AT1" s="94"/>
+      <c r="AU1" s="94"/>
+      <c r="AV1" s="94"/>
+      <c r="AW1" s="94"/>
+      <c r="AX1" s="94"/>
+      <c r="AY1" s="94"/>
+      <c r="AZ1" s="94"/>
+      <c r="BA1" s="94"/>
+      <c r="BB1" s="94"/>
+      <c r="BC1" s="94"/>
+      <c r="BD1" s="94"/>
+      <c r="BE1" s="94"/>
+      <c r="BF1" s="94"/>
+      <c r="BG1" s="94"/>
+      <c r="BH1" s="94"/>
+      <c r="BI1" s="94"/>
+      <c r="BJ1" s="94"/>
+      <c r="BK1" s="94"/>
+      <c r="BL1" s="94"/>
+      <c r="BM1" s="94"/>
       <c r="BN1" s="47" t="s">
         <v>4</v>
       </c>
       <c r="BO1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="BP1" s="83" t="s">
+      <c r="BP1" s="95" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:68" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
-      <c r="B2" s="79"/>
+      <c r="A2" s="88"/>
+      <c r="B2" s="91"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="87"/>
-      <c r="T2" s="87"/>
-      <c r="U2" s="87"/>
-      <c r="V2" s="87"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="87"/>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="87"/>
-      <c r="AF2" s="87"/>
-      <c r="AG2" s="87"/>
-      <c r="AH2" s="87"/>
-      <c r="AI2" s="87"/>
-      <c r="AJ2" s="87"/>
-      <c r="AK2" s="87"/>
-      <c r="AL2" s="87"/>
-      <c r="AM2" s="87"/>
-      <c r="AN2" s="87"/>
-      <c r="AO2" s="87"/>
-      <c r="AP2" s="87"/>
-      <c r="AQ2" s="87"/>
-      <c r="AR2" s="87"/>
-      <c r="AS2" s="87"/>
-      <c r="AT2" s="87"/>
-      <c r="AU2" s="87"/>
-      <c r="AV2" s="87"/>
-      <c r="AW2" s="87"/>
-      <c r="AX2" s="87"/>
-      <c r="AY2" s="87"/>
-      <c r="AZ2" s="87"/>
-      <c r="BA2" s="87"/>
-      <c r="BB2" s="87"/>
-      <c r="BC2" s="87"/>
-      <c r="BD2" s="87"/>
-      <c r="BE2" s="87"/>
-      <c r="BF2" s="87"/>
-      <c r="BG2" s="87"/>
-      <c r="BH2" s="87"/>
-      <c r="BI2" s="87"/>
-      <c r="BJ2" s="87"/>
-      <c r="BK2" s="87"/>
-      <c r="BL2" s="87"/>
-      <c r="BM2" s="87"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="99"/>
+      <c r="AA2" s="99"/>
+      <c r="AB2" s="99"/>
+      <c r="AC2" s="99"/>
+      <c r="AD2" s="99"/>
+      <c r="AE2" s="99"/>
+      <c r="AF2" s="99"/>
+      <c r="AG2" s="99"/>
+      <c r="AH2" s="99"/>
+      <c r="AI2" s="99"/>
+      <c r="AJ2" s="99"/>
+      <c r="AK2" s="99"/>
+      <c r="AL2" s="99"/>
+      <c r="AM2" s="99"/>
+      <c r="AN2" s="99"/>
+      <c r="AO2" s="99"/>
+      <c r="AP2" s="99"/>
+      <c r="AQ2" s="99"/>
+      <c r="AR2" s="99"/>
+      <c r="AS2" s="99"/>
+      <c r="AT2" s="99"/>
+      <c r="AU2" s="99"/>
+      <c r="AV2" s="99"/>
+      <c r="AW2" s="99"/>
+      <c r="AX2" s="99"/>
+      <c r="AY2" s="99"/>
+      <c r="AZ2" s="99"/>
+      <c r="BA2" s="99"/>
+      <c r="BB2" s="99"/>
+      <c r="BC2" s="99"/>
+      <c r="BD2" s="99"/>
+      <c r="BE2" s="99"/>
+      <c r="BF2" s="99"/>
+      <c r="BG2" s="99"/>
+      <c r="BH2" s="99"/>
+      <c r="BI2" s="99"/>
+      <c r="BJ2" s="99"/>
+      <c r="BK2" s="99"/>
+      <c r="BL2" s="99"/>
+      <c r="BM2" s="99"/>
       <c r="BN2" s="3"/>
       <c r="BO2" s="3"/>
-      <c r="BP2" s="84"/>
+      <c r="BP2" s="96"/>
     </row>
     <row r="3" spans="1:68" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="80"/>
+      <c r="A3" s="89"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="88">
+      <c r="D3" s="100">
         <v>1</v>
       </c>
-      <c r="E3" s="89"/>
-      <c r="F3" s="90">
+      <c r="E3" s="82"/>
+      <c r="F3" s="80">
         <v>2</v>
       </c>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90">
+      <c r="G3" s="82"/>
+      <c r="H3" s="80">
         <v>3</v>
       </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="90">
+      <c r="I3" s="82"/>
+      <c r="J3" s="80">
         <v>4</v>
       </c>
-      <c r="K3" s="89"/>
-      <c r="L3" s="90">
+      <c r="K3" s="82"/>
+      <c r="L3" s="80">
         <v>5</v>
       </c>
-      <c r="M3" s="89"/>
-      <c r="N3" s="90">
+      <c r="M3" s="82"/>
+      <c r="N3" s="80">
         <v>6</v>
       </c>
-      <c r="O3" s="89"/>
-      <c r="P3" s="90">
+      <c r="O3" s="82"/>
+      <c r="P3" s="80">
         <v>7</v>
       </c>
-      <c r="Q3" s="89"/>
-      <c r="R3" s="90">
+      <c r="Q3" s="82"/>
+      <c r="R3" s="80">
         <v>8</v>
       </c>
-      <c r="S3" s="89"/>
-      <c r="T3" s="90">
+      <c r="S3" s="82"/>
+      <c r="T3" s="80">
         <v>9</v>
       </c>
-      <c r="U3" s="89"/>
-      <c r="V3" s="90">
+      <c r="U3" s="82"/>
+      <c r="V3" s="80">
         <v>10</v>
       </c>
-      <c r="W3" s="89"/>
-      <c r="X3" s="90">
+      <c r="W3" s="82"/>
+      <c r="X3" s="80">
         <v>11</v>
       </c>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="90">
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="80">
         <v>12</v>
       </c>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="90">
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="80">
         <v>13</v>
       </c>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="90">
+      <c r="AC3" s="82"/>
+      <c r="AD3" s="80">
         <v>14</v>
       </c>
-      <c r="AE3" s="89"/>
-      <c r="AF3" s="90">
+      <c r="AE3" s="82"/>
+      <c r="AF3" s="80">
         <v>15</v>
       </c>
-      <c r="AG3" s="89"/>
-      <c r="AH3" s="90">
+      <c r="AG3" s="82"/>
+      <c r="AH3" s="80">
         <v>16</v>
       </c>
-      <c r="AI3" s="89"/>
-      <c r="AJ3" s="90">
+      <c r="AI3" s="82"/>
+      <c r="AJ3" s="80">
         <v>17</v>
       </c>
-      <c r="AK3" s="91"/>
-      <c r="AL3" s="91"/>
-      <c r="AM3" s="91"/>
-      <c r="AN3" s="89"/>
-      <c r="AO3" s="90">
+      <c r="AK3" s="81"/>
+      <c r="AL3" s="81"/>
+      <c r="AM3" s="81"/>
+      <c r="AN3" s="82"/>
+      <c r="AO3" s="80">
         <v>18</v>
       </c>
-      <c r="AP3" s="91"/>
-      <c r="AQ3" s="91"/>
-      <c r="AR3" s="91"/>
-      <c r="AS3" s="89"/>
-      <c r="AT3" s="90">
+      <c r="AP3" s="81"/>
+      <c r="AQ3" s="81"/>
+      <c r="AR3" s="81"/>
+      <c r="AS3" s="82"/>
+      <c r="AT3" s="80">
         <v>19</v>
       </c>
-      <c r="AU3" s="95"/>
-      <c r="AV3" s="91"/>
-      <c r="AW3" s="95"/>
-      <c r="AX3" s="96"/>
-      <c r="AY3" s="97">
+      <c r="AU3" s="83"/>
+      <c r="AV3" s="81"/>
+      <c r="AW3" s="83"/>
+      <c r="AX3" s="84"/>
+      <c r="AY3" s="85">
         <v>20</v>
       </c>
-      <c r="AZ3" s="95"/>
-      <c r="BA3" s="95"/>
-      <c r="BB3" s="95"/>
-      <c r="BC3" s="96"/>
-      <c r="BD3" s="97">
+      <c r="AZ3" s="83"/>
+      <c r="BA3" s="83"/>
+      <c r="BB3" s="83"/>
+      <c r="BC3" s="84"/>
+      <c r="BD3" s="85">
         <v>21</v>
       </c>
-      <c r="BE3" s="95"/>
-      <c r="BF3" s="95"/>
-      <c r="BG3" s="95"/>
-      <c r="BH3" s="96"/>
-      <c r="BI3" s="97">
+      <c r="BE3" s="83"/>
+      <c r="BF3" s="83"/>
+      <c r="BG3" s="83"/>
+      <c r="BH3" s="84"/>
+      <c r="BI3" s="85">
         <v>22</v>
       </c>
-      <c r="BJ3" s="95"/>
-      <c r="BK3" s="95"/>
-      <c r="BL3" s="95"/>
-      <c r="BM3" s="91"/>
+      <c r="BJ3" s="83"/>
+      <c r="BK3" s="83"/>
+      <c r="BL3" s="83"/>
+      <c r="BM3" s="81"/>
       <c r="BN3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="BO3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="BP3" s="85"/>
+      <c r="BP3" s="97"/>
     </row>
     <row r="4" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -4242,10 +4242,18 @@
       <c r="Y35" s="33"/>
       <c r="Z35" s="59"/>
       <c r="AA35" s="33"/>
-      <c r="AB35" s="59"/>
-      <c r="AC35" s="33"/>
-      <c r="AD35" s="38"/>
-      <c r="AE35" s="39"/>
+      <c r="AB35" s="59">
+        <v>6</v>
+      </c>
+      <c r="AC35" s="33">
+        <v>4</v>
+      </c>
+      <c r="AD35" s="38">
+        <v>8</v>
+      </c>
+      <c r="AE35" s="39">
+        <v>2</v>
+      </c>
       <c r="AF35" s="59"/>
       <c r="AG35" s="33"/>
       <c r="AH35" s="59"/>
@@ -4282,7 +4290,7 @@
       <c r="BM35" s="44"/>
       <c r="BN35" s="8">
         <f>SUM(D35:BM35)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="BO35" s="8">
         <v>20</v>
@@ -4469,7 +4477,9 @@
       <c r="AC38" s="33"/>
       <c r="AD38" s="59"/>
       <c r="AE38" s="33"/>
-      <c r="AF38" s="38"/>
+      <c r="AF38" s="38">
+        <v>2</v>
+      </c>
       <c r="AG38" s="39"/>
       <c r="AH38" s="38"/>
       <c r="AI38" s="39"/>
@@ -4505,11 +4515,11 @@
       <c r="BM38" s="44"/>
       <c r="BN38" s="8">
         <f>SUM(D38:BM38)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BO38" s="8">
         <f t="shared" ref="BO38" si="7">C38-BN38</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="BP38" s="10">
         <f t="shared" ref="BP38" si="8">C38-BN38-BO38</f>
@@ -4555,10 +4565,14 @@
       <c r="AD39" s="59"/>
       <c r="AE39" s="33"/>
       <c r="AF39" s="38"/>
-      <c r="AG39" s="39"/>
+      <c r="AG39" s="39">
+        <v>4</v>
+      </c>
       <c r="AH39" s="38"/>
       <c r="AI39" s="39"/>
-      <c r="AJ39" s="40"/>
+      <c r="AJ39" s="40">
+        <v>5</v>
+      </c>
       <c r="AK39" s="42"/>
       <c r="AL39" s="40"/>
       <c r="AM39" s="42"/>
@@ -4590,11 +4604,11 @@
       <c r="BM39" s="46"/>
       <c r="BN39" s="8">
         <f>SUM(D39:BM39)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="BO39" s="8">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="BP39" s="10">
         <f t="shared" si="0"/>
@@ -4861,10 +4875,14 @@
       <c r="Z43" s="59"/>
       <c r="AA43" s="33"/>
       <c r="AB43" s="59"/>
-      <c r="AC43" s="33"/>
+      <c r="AC43" s="33">
+        <v>3</v>
+      </c>
       <c r="AD43" s="59"/>
       <c r="AE43" s="33"/>
-      <c r="AF43" s="59"/>
+      <c r="AF43" s="59">
+        <v>4</v>
+      </c>
       <c r="AG43" s="33"/>
       <c r="AH43" s="59"/>
       <c r="AI43" s="33"/>
@@ -4900,11 +4918,11 @@
       <c r="BM43" s="46"/>
       <c r="BN43" s="8">
         <f>SUM(D43:BM43)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="BO43" s="8">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>-2</v>
       </c>
       <c r="BP43" s="10">
         <f t="shared" si="0"/>
@@ -5165,7 +5183,9 @@
       <c r="AD47" s="70"/>
       <c r="AE47" s="35"/>
       <c r="AF47" s="70"/>
-      <c r="AG47" s="35"/>
+      <c r="AG47" s="35">
+        <v>3</v>
+      </c>
       <c r="AH47" s="59"/>
       <c r="AI47" s="33"/>
       <c r="AJ47" s="59"/>
@@ -5200,11 +5220,11 @@
       <c r="BM47" s="73"/>
       <c r="BN47" s="8">
         <f>SUM(D47:BM47)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BO47" s="8">
         <f t="shared" ref="BO47" si="11">C47-BN47</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="BP47" s="10">
         <f t="shared" ref="BP47" si="12">C47-BN47-BO47</f>
@@ -5251,7 +5271,9 @@
       <c r="AD48" s="59"/>
       <c r="AE48" s="33"/>
       <c r="AF48" s="59"/>
-      <c r="AG48" s="33"/>
+      <c r="AG48" s="33">
+        <v>3</v>
+      </c>
       <c r="AH48" s="59"/>
       <c r="AI48" s="33"/>
       <c r="AJ48" s="46"/>
@@ -5286,11 +5308,11 @@
       <c r="BM48" s="46"/>
       <c r="BN48" s="8">
         <f>SUM(D48:BM48)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BO48" s="8">
         <f t="shared" ref="BO48:BO50" si="13">C48-BN48</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="BP48" s="10">
         <f t="shared" ref="BP48:BP50" si="14">C48-BN48-BO48</f>
@@ -6434,7 +6456,9 @@
       <c r="AB63" s="59"/>
       <c r="AC63" s="33"/>
       <c r="AD63" s="59"/>
-      <c r="AE63" s="33"/>
+      <c r="AE63" s="33">
+        <v>6</v>
+      </c>
       <c r="AF63" s="59"/>
       <c r="AG63" s="33"/>
       <c r="AH63" s="59"/>
@@ -6471,11 +6495,11 @@
       <c r="BM63" s="46"/>
       <c r="BN63" s="8">
         <f>SUM(D63:BM63)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BO63" s="8">
         <f>C63-BN63</f>
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="BP63" s="10">
         <f>C63-BN63-BO63</f>
@@ -6773,141 +6797,141 @@
         <f>SUM(C5:C13)+SUM(C16:C33)+SUM(C36:C56)+SUM(C58:C67)</f>
         <v>466</v>
       </c>
-      <c r="D68" s="92">
+      <c r="D68" s="86">
         <f>SUM(D4:E67)</f>
         <v>10</v>
       </c>
-      <c r="E68" s="93"/>
-      <c r="F68" s="94">
+      <c r="E68" s="78"/>
+      <c r="F68" s="75">
         <f>SUM(F4:G67)</f>
         <v>7</v>
       </c>
-      <c r="G68" s="93"/>
-      <c r="H68" s="94">
+      <c r="G68" s="78"/>
+      <c r="H68" s="75">
         <f>SUM(H4:I67)</f>
         <v>4</v>
       </c>
-      <c r="I68" s="93"/>
-      <c r="J68" s="94">
+      <c r="I68" s="78"/>
+      <c r="J68" s="75">
         <f>SUM(J4:K67)</f>
         <v>0</v>
       </c>
-      <c r="K68" s="93"/>
-      <c r="L68" s="94">
+      <c r="K68" s="78"/>
+      <c r="L68" s="75">
         <f>SUM(L4:M67)</f>
         <v>18</v>
       </c>
-      <c r="M68" s="93"/>
-      <c r="N68" s="94">
+      <c r="M68" s="78"/>
+      <c r="N68" s="75">
         <f>SUM(N4:O67)</f>
         <v>11</v>
       </c>
-      <c r="O68" s="93"/>
-      <c r="P68" s="94">
+      <c r="O68" s="78"/>
+      <c r="P68" s="75">
         <f>SUM(P4:Q67)</f>
         <v>11</v>
       </c>
-      <c r="Q68" s="93"/>
-      <c r="R68" s="94">
+      <c r="Q68" s="78"/>
+      <c r="R68" s="75">
         <f>SUM(R4:S67)</f>
         <v>4</v>
       </c>
-      <c r="S68" s="93"/>
-      <c r="T68" s="94">
+      <c r="S68" s="78"/>
+      <c r="T68" s="75">
         <f>SUM(T4:U67)</f>
         <v>7</v>
       </c>
-      <c r="U68" s="93"/>
-      <c r="V68" s="94">
+      <c r="U68" s="78"/>
+      <c r="V68" s="75">
         <f>SUM(V4:W67)</f>
         <v>9</v>
       </c>
-      <c r="W68" s="93"/>
-      <c r="X68" s="94">
+      <c r="W68" s="78"/>
+      <c r="X68" s="75">
         <f>SUM(X4:Y67)</f>
         <v>11</v>
       </c>
-      <c r="Y68" s="93"/>
-      <c r="Z68" s="94">
+      <c r="Y68" s="78"/>
+      <c r="Z68" s="75">
         <f>SUM(Z4:AA67)</f>
         <v>17</v>
       </c>
-      <c r="AA68" s="93"/>
-      <c r="AB68" s="94">
+      <c r="AA68" s="78"/>
+      <c r="AB68" s="75">
         <f>SUM(AB4:AC67)</f>
-        <v>0</v>
-      </c>
-      <c r="AC68" s="93"/>
-      <c r="AD68" s="94">
+        <v>13</v>
+      </c>
+      <c r="AC68" s="78"/>
+      <c r="AD68" s="75">
         <f>SUM(AD4:AE67)</f>
-        <v>0</v>
-      </c>
-      <c r="AE68" s="93"/>
-      <c r="AF68" s="94">
+        <v>16</v>
+      </c>
+      <c r="AE68" s="78"/>
+      <c r="AF68" s="75">
         <f>SUM(AF4:AG67)</f>
-        <v>0</v>
-      </c>
-      <c r="AG68" s="100"/>
-      <c r="AH68" s="94">
+        <v>16</v>
+      </c>
+      <c r="AG68" s="79"/>
+      <c r="AH68" s="75">
         <f>SUM(AH4:AI67)</f>
         <v>0</v>
       </c>
-      <c r="AI68" s="100"/>
-      <c r="AJ68" s="94">
+      <c r="AI68" s="79"/>
+      <c r="AJ68" s="75">
         <f>SUM(AJ4:AN67)</f>
-        <v>0</v>
-      </c>
-      <c r="AK68" s="98"/>
-      <c r="AL68" s="98"/>
-      <c r="AM68" s="98"/>
-      <c r="AN68" s="99"/>
-      <c r="AO68" s="94">
+        <v>5</v>
+      </c>
+      <c r="AK68" s="76"/>
+      <c r="AL68" s="76"/>
+      <c r="AM68" s="76"/>
+      <c r="AN68" s="77"/>
+      <c r="AO68" s="75">
         <f>SUM(AO4:AS67)</f>
         <v>0</v>
       </c>
-      <c r="AP68" s="98"/>
-      <c r="AQ68" s="98"/>
-      <c r="AR68" s="98"/>
-      <c r="AS68" s="99"/>
-      <c r="AT68" s="94">
+      <c r="AP68" s="76"/>
+      <c r="AQ68" s="76"/>
+      <c r="AR68" s="76"/>
+      <c r="AS68" s="77"/>
+      <c r="AT68" s="75">
         <f>SUM(AT4:AX67)</f>
         <v>0</v>
       </c>
-      <c r="AU68" s="98"/>
-      <c r="AV68" s="98"/>
-      <c r="AW68" s="98"/>
-      <c r="AX68" s="99"/>
-      <c r="AY68" s="94">
+      <c r="AU68" s="76"/>
+      <c r="AV68" s="76"/>
+      <c r="AW68" s="76"/>
+      <c r="AX68" s="77"/>
+      <c r="AY68" s="75">
         <f>SUM(AY4:BC67)</f>
         <v>0</v>
       </c>
-      <c r="AZ68" s="98"/>
-      <c r="BA68" s="98"/>
-      <c r="BB68" s="98"/>
-      <c r="BC68" s="99"/>
-      <c r="BD68" s="94">
+      <c r="AZ68" s="76"/>
+      <c r="BA68" s="76"/>
+      <c r="BB68" s="76"/>
+      <c r="BC68" s="77"/>
+      <c r="BD68" s="75">
         <f>SUM(BD4:BH67)</f>
         <v>0</v>
       </c>
-      <c r="BE68" s="98"/>
-      <c r="BF68" s="98"/>
-      <c r="BG68" s="98"/>
-      <c r="BH68" s="99"/>
-      <c r="BI68" s="94">
+      <c r="BE68" s="76"/>
+      <c r="BF68" s="76"/>
+      <c r="BG68" s="76"/>
+      <c r="BH68" s="77"/>
+      <c r="BI68" s="75">
         <f>SUM(BI4:BM67)</f>
         <v>0</v>
       </c>
-      <c r="BJ68" s="98"/>
-      <c r="BK68" s="98"/>
-      <c r="BL68" s="98"/>
-      <c r="BM68" s="99"/>
+      <c r="BJ68" s="76"/>
+      <c r="BK68" s="76"/>
+      <c r="BL68" s="76"/>
+      <c r="BM68" s="77"/>
       <c r="BN68" s="21">
         <f>SUM(BN4:BN67)</f>
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="BO68" s="21">
         <f>SUM(BO4:BO67)</f>
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="BP68" s="22">
         <f>SUM(BP4:BP67)</f>
@@ -6919,39 +6943,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="AO68:AS68"/>
-    <mergeCell ref="AT68:AX68"/>
-    <mergeCell ref="AY68:BC68"/>
-    <mergeCell ref="BD68:BH68"/>
-    <mergeCell ref="BI68:BM68"/>
-    <mergeCell ref="AJ68:AN68"/>
-    <mergeCell ref="N68:O68"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="R68:S68"/>
-    <mergeCell ref="T68:U68"/>
-    <mergeCell ref="V68:W68"/>
-    <mergeCell ref="X68:Y68"/>
-    <mergeCell ref="Z68:AA68"/>
-    <mergeCell ref="AB68:AC68"/>
-    <mergeCell ref="AD68:AE68"/>
-    <mergeCell ref="AF68:AG68"/>
-    <mergeCell ref="AH68:AI68"/>
-    <mergeCell ref="AO3:AS3"/>
-    <mergeCell ref="AT3:AX3"/>
-    <mergeCell ref="AY3:BC3"/>
-    <mergeCell ref="BD3:BH3"/>
-    <mergeCell ref="BI3:BM3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="L68:M68"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="D1:BM1"/>
@@ -6968,6 +6959,39 @@
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="L68:M68"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AO3:AS3"/>
+    <mergeCell ref="AT3:AX3"/>
+    <mergeCell ref="AY3:BC3"/>
+    <mergeCell ref="BD3:BH3"/>
+    <mergeCell ref="BI3:BM3"/>
+    <mergeCell ref="AJ68:AN68"/>
+    <mergeCell ref="N68:O68"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="R68:S68"/>
+    <mergeCell ref="T68:U68"/>
+    <mergeCell ref="V68:W68"/>
+    <mergeCell ref="X68:Y68"/>
+    <mergeCell ref="Z68:AA68"/>
+    <mergeCell ref="AB68:AC68"/>
+    <mergeCell ref="AD68:AE68"/>
+    <mergeCell ref="AF68:AG68"/>
+    <mergeCell ref="AH68:AI68"/>
+    <mergeCell ref="AO68:AS68"/>
+    <mergeCell ref="AT68:AX68"/>
+    <mergeCell ref="AY68:BC68"/>
+    <mergeCell ref="BD68:BH68"/>
+    <mergeCell ref="BI68:BM68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="63" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Rapport partie 4 data + frontend
</commit_message>
<xml_diff>
--- a/01_doc/Planning.xlsx
+++ b/01_doc/Planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naily\Documents\01_HEIG\01_TB\01_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EC97BC-405F-4912-AE01-F4111D4CDBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E8E780-03C1-495C-B1A9-3CE835731BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22236" windowHeight="13176" xr2:uid="{F59D9D10-3A89-4134-8555-53CD5E65A538}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Tâche</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>30.40.70</t>
+  </si>
+  <si>
+    <t>Outil de recherche</t>
+  </si>
+  <si>
+    <t>30.40.80</t>
   </si>
 </sst>
 </file>
@@ -1169,85 +1175,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1567,10 +1573,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BS76"/>
+  <dimension ref="A1:BS77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AY61" sqref="AY61"/>
+    <sheetView tabSelected="1" topLeftCell="X52" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BR76" sqref="BR76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1619,286 +1625,286 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="87" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="102"/>
-      <c r="X1" s="102"/>
-      <c r="Y1" s="102"/>
-      <c r="Z1" s="102"/>
-      <c r="AA1" s="102"/>
-      <c r="AB1" s="102"/>
-      <c r="AC1" s="102"/>
-      <c r="AD1" s="102"/>
-      <c r="AE1" s="102"/>
-      <c r="AF1" s="102"/>
-      <c r="AG1" s="102"/>
-      <c r="AH1" s="102"/>
-      <c r="AI1" s="102"/>
-      <c r="AJ1" s="102"/>
-      <c r="AK1" s="102"/>
-      <c r="AL1" s="102"/>
-      <c r="AM1" s="102"/>
-      <c r="AN1" s="102"/>
-      <c r="AO1" s="102"/>
-      <c r="AP1" s="102"/>
-      <c r="AQ1" s="102"/>
-      <c r="AR1" s="102"/>
-      <c r="AS1" s="102"/>
-      <c r="AT1" s="102"/>
-      <c r="AU1" s="102"/>
-      <c r="AV1" s="102"/>
-      <c r="AW1" s="102"/>
-      <c r="AX1" s="102"/>
-      <c r="AY1" s="102"/>
-      <c r="AZ1" s="102"/>
-      <c r="BA1" s="102"/>
-      <c r="BB1" s="102"/>
-      <c r="BC1" s="102"/>
-      <c r="BD1" s="102"/>
-      <c r="BE1" s="102"/>
-      <c r="BF1" s="102"/>
-      <c r="BG1" s="102"/>
-      <c r="BH1" s="102"/>
-      <c r="BI1" s="102"/>
-      <c r="BJ1" s="102"/>
-      <c r="BK1" s="102"/>
-      <c r="BL1" s="102"/>
-      <c r="BM1" s="102"/>
-      <c r="BN1" s="102"/>
-      <c r="BO1" s="102"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="91"/>
+      <c r="S1" s="91"/>
+      <c r="T1" s="91"/>
+      <c r="U1" s="91"/>
+      <c r="V1" s="91"/>
+      <c r="W1" s="91"/>
+      <c r="X1" s="91"/>
+      <c r="Y1" s="91"/>
+      <c r="Z1" s="91"/>
+      <c r="AA1" s="91"/>
+      <c r="AB1" s="91"/>
+      <c r="AC1" s="91"/>
+      <c r="AD1" s="91"/>
+      <c r="AE1" s="91"/>
+      <c r="AF1" s="91"/>
+      <c r="AG1" s="91"/>
+      <c r="AH1" s="91"/>
+      <c r="AI1" s="91"/>
+      <c r="AJ1" s="91"/>
+      <c r="AK1" s="91"/>
+      <c r="AL1" s="91"/>
+      <c r="AM1" s="91"/>
+      <c r="AN1" s="91"/>
+      <c r="AO1" s="91"/>
+      <c r="AP1" s="91"/>
+      <c r="AQ1" s="91"/>
+      <c r="AR1" s="91"/>
+      <c r="AS1" s="91"/>
+      <c r="AT1" s="91"/>
+      <c r="AU1" s="91"/>
+      <c r="AV1" s="91"/>
+      <c r="AW1" s="91"/>
+      <c r="AX1" s="91"/>
+      <c r="AY1" s="91"/>
+      <c r="AZ1" s="91"/>
+      <c r="BA1" s="91"/>
+      <c r="BB1" s="91"/>
+      <c r="BC1" s="91"/>
+      <c r="BD1" s="91"/>
+      <c r="BE1" s="91"/>
+      <c r="BF1" s="91"/>
+      <c r="BG1" s="91"/>
+      <c r="BH1" s="91"/>
+      <c r="BI1" s="91"/>
+      <c r="BJ1" s="91"/>
+      <c r="BK1" s="91"/>
+      <c r="BL1" s="91"/>
+      <c r="BM1" s="91"/>
+      <c r="BN1" s="91"/>
+      <c r="BO1" s="91"/>
       <c r="BP1" s="47" t="s">
         <v>4</v>
       </c>
       <c r="BQ1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="BR1" s="103" t="s">
+      <c r="BR1" s="92" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:70" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96"/>
-      <c r="B2" s="99"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="88"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="106" t="s">
+      <c r="D2" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="107"/>
-      <c r="AB2" s="107"/>
-      <c r="AC2" s="107"/>
-      <c r="AD2" s="107"/>
-      <c r="AE2" s="107"/>
-      <c r="AF2" s="107"/>
-      <c r="AG2" s="107"/>
-      <c r="AH2" s="107"/>
-      <c r="AI2" s="107"/>
-      <c r="AJ2" s="107"/>
-      <c r="AK2" s="107"/>
-      <c r="AL2" s="107"/>
-      <c r="AM2" s="107"/>
-      <c r="AN2" s="107"/>
-      <c r="AO2" s="107"/>
-      <c r="AP2" s="107"/>
-      <c r="AQ2" s="107"/>
-      <c r="AR2" s="107"/>
-      <c r="AS2" s="107"/>
-      <c r="AT2" s="107"/>
-      <c r="AU2" s="107"/>
-      <c r="AV2" s="107"/>
-      <c r="AW2" s="107"/>
-      <c r="AX2" s="107"/>
-      <c r="AY2" s="107"/>
-      <c r="AZ2" s="107"/>
-      <c r="BA2" s="107"/>
-      <c r="BB2" s="107"/>
-      <c r="BC2" s="107"/>
-      <c r="BD2" s="107"/>
-      <c r="BE2" s="107"/>
-      <c r="BF2" s="107"/>
-      <c r="BG2" s="107"/>
-      <c r="BH2" s="107"/>
-      <c r="BI2" s="107"/>
-      <c r="BJ2" s="107"/>
-      <c r="BK2" s="107"/>
-      <c r="BL2" s="107"/>
-      <c r="BM2" s="107"/>
-      <c r="BN2" s="107"/>
-      <c r="BO2" s="107"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
+      <c r="Q2" s="96"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="96"/>
+      <c r="T2" s="96"/>
+      <c r="U2" s="96"/>
+      <c r="V2" s="96"/>
+      <c r="W2" s="96"/>
+      <c r="X2" s="96"/>
+      <c r="Y2" s="96"/>
+      <c r="Z2" s="96"/>
+      <c r="AA2" s="96"/>
+      <c r="AB2" s="96"/>
+      <c r="AC2" s="96"/>
+      <c r="AD2" s="96"/>
+      <c r="AE2" s="96"/>
+      <c r="AF2" s="96"/>
+      <c r="AG2" s="96"/>
+      <c r="AH2" s="96"/>
+      <c r="AI2" s="96"/>
+      <c r="AJ2" s="96"/>
+      <c r="AK2" s="96"/>
+      <c r="AL2" s="96"/>
+      <c r="AM2" s="96"/>
+      <c r="AN2" s="96"/>
+      <c r="AO2" s="96"/>
+      <c r="AP2" s="96"/>
+      <c r="AQ2" s="96"/>
+      <c r="AR2" s="96"/>
+      <c r="AS2" s="96"/>
+      <c r="AT2" s="96"/>
+      <c r="AU2" s="96"/>
+      <c r="AV2" s="96"/>
+      <c r="AW2" s="96"/>
+      <c r="AX2" s="96"/>
+      <c r="AY2" s="96"/>
+      <c r="AZ2" s="96"/>
+      <c r="BA2" s="96"/>
+      <c r="BB2" s="96"/>
+      <c r="BC2" s="96"/>
+      <c r="BD2" s="96"/>
+      <c r="BE2" s="96"/>
+      <c r="BF2" s="96"/>
+      <c r="BG2" s="96"/>
+      <c r="BH2" s="96"/>
+      <c r="BI2" s="96"/>
+      <c r="BJ2" s="96"/>
+      <c r="BK2" s="96"/>
+      <c r="BL2" s="96"/>
+      <c r="BM2" s="96"/>
+      <c r="BN2" s="96"/>
+      <c r="BO2" s="96"/>
       <c r="BP2" s="3"/>
       <c r="BQ2" s="3"/>
-      <c r="BR2" s="104"/>
+      <c r="BR2" s="93"/>
     </row>
     <row r="3" spans="1:70" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="97"/>
-      <c r="B3" s="100"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="89"/>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="108">
+      <c r="D3" s="97">
         <v>1</v>
       </c>
-      <c r="E3" s="90"/>
-      <c r="F3" s="88">
+      <c r="E3" s="98"/>
+      <c r="F3" s="99">
         <v>2</v>
       </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="88">
+      <c r="G3" s="98"/>
+      <c r="H3" s="99">
         <v>3</v>
       </c>
-      <c r="I3" s="90"/>
-      <c r="J3" s="88">
+      <c r="I3" s="98"/>
+      <c r="J3" s="99">
         <v>4</v>
       </c>
-      <c r="K3" s="90"/>
-      <c r="L3" s="88">
+      <c r="K3" s="98"/>
+      <c r="L3" s="99">
         <v>5</v>
       </c>
-      <c r="M3" s="90"/>
-      <c r="N3" s="88">
+      <c r="M3" s="98"/>
+      <c r="N3" s="99">
         <v>6</v>
       </c>
-      <c r="O3" s="90"/>
-      <c r="P3" s="88">
+      <c r="O3" s="98"/>
+      <c r="P3" s="99">
         <v>7</v>
       </c>
-      <c r="Q3" s="90"/>
-      <c r="R3" s="88">
+      <c r="Q3" s="98"/>
+      <c r="R3" s="99">
         <v>8</v>
       </c>
-      <c r="S3" s="90"/>
-      <c r="T3" s="88">
+      <c r="S3" s="98"/>
+      <c r="T3" s="99">
         <v>9</v>
       </c>
-      <c r="U3" s="90"/>
-      <c r="V3" s="88">
+      <c r="U3" s="98"/>
+      <c r="V3" s="99">
         <v>10</v>
       </c>
-      <c r="W3" s="90"/>
-      <c r="X3" s="88">
+      <c r="W3" s="98"/>
+      <c r="X3" s="99">
         <v>11</v>
       </c>
-      <c r="Y3" s="90"/>
-      <c r="Z3" s="88">
+      <c r="Y3" s="98"/>
+      <c r="Z3" s="99">
         <v>12</v>
       </c>
-      <c r="AA3" s="90"/>
-      <c r="AB3" s="88">
+      <c r="AA3" s="98"/>
+      <c r="AB3" s="99">
         <v>13</v>
       </c>
-      <c r="AC3" s="90"/>
-      <c r="AD3" s="88">
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="99">
         <v>14</v>
       </c>
-      <c r="AE3" s="90"/>
-      <c r="AF3" s="88">
+      <c r="AE3" s="98"/>
+      <c r="AF3" s="99">
         <v>15</v>
       </c>
-      <c r="AG3" s="90"/>
-      <c r="AH3" s="88">
+      <c r="AG3" s="98"/>
+      <c r="AH3" s="99">
         <v>16</v>
       </c>
-      <c r="AI3" s="90"/>
-      <c r="AJ3" s="88">
+      <c r="AI3" s="98"/>
+      <c r="AJ3" s="99">
         <v>17</v>
       </c>
-      <c r="AK3" s="89"/>
-      <c r="AL3" s="89"/>
-      <c r="AM3" s="89"/>
-      <c r="AN3" s="90"/>
+      <c r="AK3" s="100"/>
+      <c r="AL3" s="100"/>
+      <c r="AM3" s="100"/>
+      <c r="AN3" s="98"/>
       <c r="AO3" s="76"/>
-      <c r="AP3" s="88">
+      <c r="AP3" s="99">
         <v>18</v>
       </c>
-      <c r="AQ3" s="89"/>
-      <c r="AR3" s="89"/>
-      <c r="AS3" s="89"/>
-      <c r="AT3" s="90"/>
+      <c r="AQ3" s="100"/>
+      <c r="AR3" s="100"/>
+      <c r="AS3" s="100"/>
+      <c r="AT3" s="98"/>
       <c r="AU3" s="77"/>
-      <c r="AV3" s="88">
+      <c r="AV3" s="99">
         <v>19</v>
       </c>
-      <c r="AW3" s="91"/>
-      <c r="AX3" s="89"/>
-      <c r="AY3" s="91"/>
-      <c r="AZ3" s="92"/>
-      <c r="BA3" s="93">
+      <c r="AW3" s="104"/>
+      <c r="AX3" s="100"/>
+      <c r="AY3" s="104"/>
+      <c r="AZ3" s="105"/>
+      <c r="BA3" s="106">
         <v>20</v>
       </c>
-      <c r="BB3" s="91"/>
-      <c r="BC3" s="91"/>
-      <c r="BD3" s="91"/>
-      <c r="BE3" s="92"/>
-      <c r="BF3" s="93">
+      <c r="BB3" s="104"/>
+      <c r="BC3" s="104"/>
+      <c r="BD3" s="104"/>
+      <c r="BE3" s="105"/>
+      <c r="BF3" s="106">
         <v>21</v>
       </c>
-      <c r="BG3" s="91"/>
-      <c r="BH3" s="91"/>
-      <c r="BI3" s="91"/>
-      <c r="BJ3" s="92"/>
-      <c r="BK3" s="93">
+      <c r="BG3" s="104"/>
+      <c r="BH3" s="104"/>
+      <c r="BI3" s="104"/>
+      <c r="BJ3" s="105"/>
+      <c r="BK3" s="106">
         <v>22</v>
       </c>
-      <c r="BL3" s="91"/>
-      <c r="BM3" s="91"/>
-      <c r="BN3" s="91"/>
-      <c r="BO3" s="89"/>
+      <c r="BL3" s="104"/>
+      <c r="BM3" s="104"/>
+      <c r="BN3" s="104"/>
+      <c r="BO3" s="100"/>
       <c r="BP3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="BQ3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="BR3" s="105"/>
+      <c r="BR3" s="94"/>
     </row>
     <row r="4" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -4298,7 +4304,7 @@
         <v>61</v>
       </c>
       <c r="C34" s="17">
-        <f>SUM(C39:C58)</f>
+        <f>SUM(C39:C59)</f>
         <v>154</v>
       </c>
       <c r="D34" s="63"/>
@@ -5366,7 +5372,9 @@
       <c r="AY46" s="45"/>
       <c r="AZ46" s="33"/>
       <c r="BA46" s="46"/>
-      <c r="BB46" s="45"/>
+      <c r="BB46" s="45">
+        <v>6</v>
+      </c>
       <c r="BC46" s="46"/>
       <c r="BD46" s="45"/>
       <c r="BE46" s="33"/>
@@ -5589,13 +5597,23 @@
       <c r="AW49" s="45"/>
       <c r="AX49" s="44"/>
       <c r="AY49" s="45"/>
-      <c r="AZ49" s="44"/>
+      <c r="AZ49" s="33">
+        <v>9</v>
+      </c>
       <c r="BA49" s="59"/>
-      <c r="BB49" s="32"/>
+      <c r="BB49" s="32">
+        <v>2</v>
+      </c>
       <c r="BC49" s="32"/>
-      <c r="BD49" s="32"/>
-      <c r="BE49" s="44"/>
-      <c r="BF49" s="70"/>
+      <c r="BD49" s="32">
+        <v>6</v>
+      </c>
+      <c r="BE49" s="44">
+        <v>6</v>
+      </c>
+      <c r="BF49" s="70">
+        <v>2</v>
+      </c>
       <c r="BG49" s="45"/>
       <c r="BH49" s="44"/>
       <c r="BI49" s="45"/>
@@ -5606,12 +5624,12 @@
       <c r="BN49" s="45"/>
       <c r="BO49" s="73"/>
       <c r="BP49" s="8">
-        <f t="shared" ref="BP49:BP54" si="0">SUM(D49:BO49)</f>
-        <v>5</v>
+        <f t="shared" ref="BP49:BP56" si="0">SUM(D49:BO49)</f>
+        <v>30</v>
       </c>
       <c r="BQ49" s="8">
         <f t="shared" ref="BQ49:BQ54" si="1">C49-BP49</f>
-        <v>11</v>
+        <v>-14</v>
       </c>
       <c r="BR49" s="10">
         <f t="shared" ref="BR49:BR54" si="2">C49-BP49-BQ49</f>
@@ -5685,7 +5703,6 @@
       <c r="AW50" s="42"/>
       <c r="AX50" s="40"/>
       <c r="AY50" s="45"/>
-      <c r="AZ50" s="33"/>
       <c r="BA50" s="46"/>
       <c r="BB50" s="45"/>
       <c r="BC50" s="46"/>
@@ -5871,7 +5888,9 @@
       <c r="BA52" s="40"/>
       <c r="BB52" s="45"/>
       <c r="BC52" s="46"/>
-      <c r="BD52" s="45"/>
+      <c r="BD52" s="45">
+        <v>2</v>
+      </c>
       <c r="BE52" s="33"/>
       <c r="BF52" s="46"/>
       <c r="BG52" s="45"/>
@@ -5885,11 +5904,11 @@
       <c r="BO52" s="46"/>
       <c r="BP52" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BQ52" s="8">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="BR52" s="10">
         <f t="shared" si="2"/>
@@ -6157,11 +6176,19 @@
       <c r="BM55" s="46"/>
       <c r="BN55" s="45"/>
       <c r="BO55" s="46"/>
+      <c r="BP55" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="BR55" s="10"/>
     </row>
     <row r="56" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A56" s="27"/>
-      <c r="B56" s="16"/>
+      <c r="A56" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>102</v>
+      </c>
       <c r="D56" s="34"/>
       <c r="E56" s="35"/>
       <c r="F56" s="59"/>
@@ -6210,10 +6237,14 @@
       <c r="AW56" s="45"/>
       <c r="AX56" s="46"/>
       <c r="AY56" s="45"/>
-      <c r="AZ56" s="33"/>
-      <c r="BA56" s="46"/>
+      <c r="AZ56" s="39"/>
+      <c r="BA56" s="40">
+        <v>8</v>
+      </c>
       <c r="BB56" s="45"/>
-      <c r="BC56" s="46"/>
+      <c r="BC56" s="46">
+        <v>8</v>
+      </c>
       <c r="BD56" s="45"/>
       <c r="BE56" s="33"/>
       <c r="BF56" s="46"/>
@@ -6226,16 +6257,15 @@
       <c r="BM56" s="46"/>
       <c r="BN56" s="45"/>
       <c r="BO56" s="46"/>
-      <c r="BP56" s="28"/>
+      <c r="BP56" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="BR56" s="10"/>
     </row>
     <row r="57" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A57" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="B57" s="51" t="s">
-        <v>57</v>
-      </c>
+      <c r="A57" s="27"/>
+      <c r="B57" s="16"/>
       <c r="D57" s="34"/>
       <c r="E57" s="35"/>
       <c r="F57" s="59"/>
@@ -6304,14 +6334,11 @@
       <c r="BR57" s="10"/>
     </row>
     <row r="58" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A58" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B58" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" s="8">
-        <v>20</v>
+      <c r="A58" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="51" t="s">
+        <v>57</v>
       </c>
       <c r="D58" s="34"/>
       <c r="E58" s="35"/>
@@ -6353,16 +6380,16 @@
       <c r="AO58" s="33"/>
       <c r="AP58" s="46"/>
       <c r="AQ58" s="45"/>
-      <c r="AR58" s="40"/>
-      <c r="AS58" s="42"/>
-      <c r="AT58" s="39"/>
-      <c r="AU58" s="39"/>
-      <c r="AV58" s="40"/>
-      <c r="AW58" s="42"/>
-      <c r="AX58" s="40"/>
-      <c r="AY58" s="42"/>
-      <c r="AZ58" s="39"/>
-      <c r="BA58" s="40"/>
+      <c r="AR58" s="46"/>
+      <c r="AS58" s="45"/>
+      <c r="AT58" s="33"/>
+      <c r="AU58" s="33"/>
+      <c r="AV58" s="46"/>
+      <c r="AW58" s="45"/>
+      <c r="AX58" s="46"/>
+      <c r="AY58" s="45"/>
+      <c r="AZ58" s="33"/>
+      <c r="BA58" s="46"/>
       <c r="BB58" s="45"/>
       <c r="BC58" s="46"/>
       <c r="BD58" s="45"/>
@@ -6377,22 +6404,19 @@
       <c r="BM58" s="46"/>
       <c r="BN58" s="45"/>
       <c r="BO58" s="46"/>
-      <c r="BP58" s="8">
-        <f>SUM(D58:BO58)</f>
-        <v>0</v>
-      </c>
-      <c r="BQ58" s="8">
-        <f>C58-BP58</f>
-        <v>20</v>
-      </c>
-      <c r="BR58" s="10">
-        <f>C58-BP58-BQ58</f>
-        <v>0</v>
-      </c>
+      <c r="BP58" s="28"/>
+      <c r="BR58" s="10"/>
     </row>
     <row r="59" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A59" s="6"/>
-      <c r="B59" s="16"/>
+      <c r="A59" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="8">
+        <v>20</v>
+      </c>
       <c r="D59" s="34"/>
       <c r="E59" s="35"/>
       <c r="F59" s="59"/>
@@ -6433,16 +6457,16 @@
       <c r="AO59" s="33"/>
       <c r="AP59" s="46"/>
       <c r="AQ59" s="45"/>
-      <c r="AR59" s="46"/>
-      <c r="AS59" s="45"/>
-      <c r="AT59" s="33"/>
-      <c r="AU59" s="33"/>
-      <c r="AV59" s="46"/>
-      <c r="AW59" s="45"/>
-      <c r="AX59" s="46"/>
-      <c r="AY59" s="45"/>
-      <c r="AZ59" s="33"/>
-      <c r="BA59" s="46"/>
+      <c r="AR59" s="40"/>
+      <c r="AS59" s="42"/>
+      <c r="AT59" s="39"/>
+      <c r="AU59" s="39"/>
+      <c r="AV59" s="40"/>
+      <c r="AW59" s="42"/>
+      <c r="AX59" s="40"/>
+      <c r="AY59" s="42"/>
+      <c r="AZ59" s="39"/>
+      <c r="BA59" s="40"/>
       <c r="BB59" s="45"/>
       <c r="BC59" s="46"/>
       <c r="BD59" s="45"/>
@@ -6457,19 +6481,22 @@
       <c r="BM59" s="46"/>
       <c r="BN59" s="45"/>
       <c r="BO59" s="46"/>
-      <c r="BP59" s="28"/>
-      <c r="BR59" s="10"/>
+      <c r="BP59" s="8">
+        <f>SUM(D59:BO59)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ59" s="8">
+        <f>C59-BP59</f>
+        <v>20</v>
+      </c>
+      <c r="BR59" s="10">
+        <f>C59-BP59-BQ59</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B60" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" s="8">
-        <v>30</v>
-      </c>
+      <c r="A60" s="6"/>
+      <c r="B60" s="16"/>
       <c r="D60" s="34"/>
       <c r="E60" s="35"/>
       <c r="F60" s="59"/>
@@ -6497,9 +6524,7 @@
       <c r="AB60" s="59"/>
       <c r="AC60" s="33"/>
       <c r="AD60" s="59"/>
-      <c r="AE60" s="33">
-        <v>2</v>
-      </c>
+      <c r="AE60" s="33"/>
       <c r="AF60" s="59"/>
       <c r="AG60" s="33"/>
       <c r="AH60" s="59"/>
@@ -6513,25 +6538,19 @@
       <c r="AP60" s="46"/>
       <c r="AQ60" s="45"/>
       <c r="AR60" s="46"/>
-      <c r="AS60" s="45">
-        <v>3</v>
-      </c>
+      <c r="AS60" s="45"/>
       <c r="AT60" s="33"/>
       <c r="AU60" s="33"/>
       <c r="AV60" s="46"/>
       <c r="AW60" s="45"/>
-      <c r="AX60" s="46">
-        <v>1</v>
-      </c>
-      <c r="AY60" s="45">
-        <v>8</v>
-      </c>
+      <c r="AX60" s="46"/>
+      <c r="AY60" s="45"/>
       <c r="AZ60" s="33"/>
       <c r="BA60" s="46"/>
-      <c r="BB60" s="42"/>
-      <c r="BC60" s="40"/>
-      <c r="BD60" s="42"/>
-      <c r="BE60" s="39"/>
+      <c r="BB60" s="45"/>
+      <c r="BC60" s="46"/>
+      <c r="BD60" s="45"/>
+      <c r="BE60" s="33"/>
       <c r="BF60" s="46"/>
       <c r="BG60" s="45"/>
       <c r="BH60" s="46"/>
@@ -6542,22 +6561,19 @@
       <c r="BM60" s="46"/>
       <c r="BN60" s="45"/>
       <c r="BO60" s="46"/>
-      <c r="BP60" s="8">
-        <f>SUM(D60:BO60)</f>
-        <v>14</v>
-      </c>
-      <c r="BQ60" s="8">
-        <f>C60-BP60</f>
-        <v>16</v>
-      </c>
-      <c r="BR60" s="10">
-        <f>C60-BP60-BQ60</f>
-        <v>0</v>
-      </c>
+      <c r="BP60" s="28"/>
+      <c r="BR60" s="10"/>
     </row>
     <row r="61" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A61" s="6"/>
-      <c r="B61" s="16"/>
+      <c r="A61" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B61" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="8">
+        <v>30</v>
+      </c>
       <c r="D61" s="34"/>
       <c r="E61" s="35"/>
       <c r="F61" s="59"/>
@@ -6585,7 +6601,9 @@
       <c r="AB61" s="59"/>
       <c r="AC61" s="33"/>
       <c r="AD61" s="59"/>
-      <c r="AE61" s="33"/>
+      <c r="AE61" s="33">
+        <v>2</v>
+      </c>
       <c r="AF61" s="59"/>
       <c r="AG61" s="33"/>
       <c r="AH61" s="59"/>
@@ -6599,19 +6617,27 @@
       <c r="AP61" s="46"/>
       <c r="AQ61" s="45"/>
       <c r="AR61" s="46"/>
-      <c r="AS61" s="45"/>
+      <c r="AS61" s="45">
+        <v>3</v>
+      </c>
       <c r="AT61" s="33"/>
       <c r="AU61" s="33"/>
       <c r="AV61" s="46"/>
       <c r="AW61" s="45"/>
-      <c r="AX61" s="46"/>
-      <c r="AY61" s="45"/>
+      <c r="AX61" s="46">
+        <v>1</v>
+      </c>
+      <c r="AY61" s="45">
+        <v>8</v>
+      </c>
       <c r="AZ61" s="33"/>
       <c r="BA61" s="46"/>
-      <c r="BB61" s="45"/>
-      <c r="BC61" s="46"/>
-      <c r="BD61" s="45"/>
-      <c r="BE61" s="33"/>
+      <c r="BB61" s="42"/>
+      <c r="BC61" s="40"/>
+      <c r="BD61" s="42"/>
+      <c r="BE61" s="39">
+        <v>2</v>
+      </c>
       <c r="BF61" s="46"/>
       <c r="BG61" s="45"/>
       <c r="BH61" s="46"/>
@@ -6622,182 +6648,173 @@
       <c r="BM61" s="46"/>
       <c r="BN61" s="45"/>
       <c r="BO61" s="46"/>
-      <c r="BP61" s="28"/>
-      <c r="BR61" s="10"/>
+      <c r="BP61" s="8">
+        <f>SUM(D61:BO61)</f>
+        <v>16</v>
+      </c>
+      <c r="BQ61" s="8">
+        <f>C61-BP61</f>
+        <v>14</v>
+      </c>
+      <c r="BR61" s="10">
+        <f>C61-BP61-BQ61</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="11" t="s">
+    <row r="62" spans="1:71" x14ac:dyDescent="0.3">
+      <c r="A62" s="6"/>
+      <c r="B62" s="16"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="59"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="32"/>
+      <c r="M62" s="33"/>
+      <c r="N62" s="59"/>
+      <c r="O62" s="33"/>
+      <c r="P62" s="59"/>
+      <c r="Q62" s="33"/>
+      <c r="R62" s="59"/>
+      <c r="S62" s="33"/>
+      <c r="T62" s="59"/>
+      <c r="U62" s="33"/>
+      <c r="V62" s="59"/>
+      <c r="W62" s="33"/>
+      <c r="X62" s="59"/>
+      <c r="Y62" s="33"/>
+      <c r="Z62" s="59"/>
+      <c r="AA62" s="33"/>
+      <c r="AB62" s="59"/>
+      <c r="AC62" s="33"/>
+      <c r="AD62" s="59"/>
+      <c r="AE62" s="33"/>
+      <c r="AF62" s="59"/>
+      <c r="AG62" s="33"/>
+      <c r="AH62" s="59"/>
+      <c r="AI62" s="33"/>
+      <c r="AJ62" s="46"/>
+      <c r="AK62" s="45"/>
+      <c r="AL62" s="46"/>
+      <c r="AM62" s="45"/>
+      <c r="AN62" s="33"/>
+      <c r="AO62" s="33"/>
+      <c r="AP62" s="46"/>
+      <c r="AQ62" s="45"/>
+      <c r="AR62" s="46"/>
+      <c r="AS62" s="45"/>
+      <c r="AT62" s="33"/>
+      <c r="AU62" s="33"/>
+      <c r="AV62" s="46"/>
+      <c r="AW62" s="45"/>
+      <c r="AX62" s="46"/>
+      <c r="AY62" s="45"/>
+      <c r="AZ62" s="33"/>
+      <c r="BA62" s="46"/>
+      <c r="BB62" s="45"/>
+      <c r="BC62" s="46"/>
+      <c r="BD62" s="45"/>
+      <c r="BE62" s="33"/>
+      <c r="BF62" s="46"/>
+      <c r="BG62" s="45"/>
+      <c r="BH62" s="46"/>
+      <c r="BI62" s="45"/>
+      <c r="BJ62" s="33"/>
+      <c r="BK62" s="46"/>
+      <c r="BL62" s="45"/>
+      <c r="BM62" s="46"/>
+      <c r="BN62" s="45"/>
+      <c r="BO62" s="46"/>
+      <c r="BP62" s="28"/>
+      <c r="BR62" s="10"/>
+    </row>
+    <row r="63" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B63" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="65"/>
-      <c r="G62" s="66"/>
-      <c r="H62" s="65"/>
-      <c r="I62" s="66"/>
-      <c r="J62" s="67"/>
-      <c r="K62" s="64"/>
-      <c r="L62" s="68"/>
-      <c r="M62" s="66"/>
-      <c r="N62" s="65"/>
-      <c r="O62" s="66"/>
-      <c r="P62" s="65"/>
-      <c r="Q62" s="66"/>
-      <c r="R62" s="65"/>
-      <c r="S62" s="66"/>
-      <c r="T62" s="65"/>
-      <c r="U62" s="66"/>
-      <c r="V62" s="65"/>
-      <c r="W62" s="66"/>
-      <c r="X62" s="65"/>
-      <c r="Y62" s="66"/>
-      <c r="Z62" s="65"/>
-      <c r="AA62" s="66"/>
-      <c r="AB62" s="65"/>
-      <c r="AC62" s="66"/>
-      <c r="AD62" s="65"/>
-      <c r="AE62" s="66"/>
-      <c r="AF62" s="65"/>
-      <c r="AG62" s="66"/>
-      <c r="AH62" s="65"/>
-      <c r="AI62" s="66"/>
-      <c r="AJ62" s="67"/>
-      <c r="AK62" s="69"/>
-      <c r="AL62" s="67"/>
-      <c r="AM62" s="69"/>
-      <c r="AN62" s="66"/>
-      <c r="AO62" s="66"/>
-      <c r="AP62" s="67"/>
-      <c r="AQ62" s="69"/>
-      <c r="AR62" s="67"/>
-      <c r="AS62" s="69"/>
-      <c r="AT62" s="66"/>
-      <c r="AU62" s="66"/>
-      <c r="AV62" s="67"/>
-      <c r="AW62" s="69"/>
-      <c r="AX62" s="67"/>
-      <c r="AY62" s="69"/>
-      <c r="AZ62" s="66"/>
-      <c r="BA62" s="67"/>
-      <c r="BB62" s="69"/>
-      <c r="BC62" s="67"/>
-      <c r="BD62" s="69"/>
-      <c r="BE62" s="66"/>
-      <c r="BF62" s="67"/>
-      <c r="BG62" s="69"/>
-      <c r="BH62" s="67"/>
-      <c r="BI62" s="69"/>
-      <c r="BJ62" s="66"/>
-      <c r="BK62" s="67"/>
-      <c r="BL62" s="69"/>
-      <c r="BM62" s="67"/>
-      <c r="BN62" s="69"/>
-      <c r="BO62" s="67"/>
-      <c r="BP62" s="17"/>
-      <c r="BR62" s="13"/>
-    </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A63" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" s="8">
-        <v>20</v>
-      </c>
-      <c r="D63" s="34"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="59"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="32"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="59"/>
-      <c r="O63" s="33"/>
-      <c r="P63" s="59"/>
-      <c r="Q63" s="33"/>
-      <c r="R63" s="59"/>
-      <c r="S63" s="33"/>
-      <c r="T63" s="59"/>
-      <c r="U63" s="33"/>
-      <c r="V63" s="59"/>
-      <c r="W63" s="33"/>
-      <c r="X63" s="59"/>
-      <c r="Y63" s="33"/>
-      <c r="Z63" s="59"/>
-      <c r="AA63" s="33"/>
-      <c r="AB63" s="59"/>
-      <c r="AC63" s="33"/>
-      <c r="AD63" s="38"/>
-      <c r="AE63" s="39"/>
-      <c r="AF63" s="59"/>
-      <c r="AG63" s="33"/>
-      <c r="AH63" s="59"/>
-      <c r="AI63" s="33"/>
-      <c r="AJ63" s="46"/>
-      <c r="AK63" s="45"/>
-      <c r="AL63" s="46"/>
-      <c r="AM63" s="45"/>
-      <c r="AN63" s="39"/>
-      <c r="AO63" s="39"/>
-      <c r="AP63" s="46"/>
-      <c r="AQ63" s="45"/>
-      <c r="AR63" s="46"/>
-      <c r="AS63" s="45"/>
-      <c r="AT63" s="39">
-        <v>1.5</v>
-      </c>
-      <c r="AU63" s="39"/>
-      <c r="AV63" s="46"/>
-      <c r="AW63" s="45"/>
-      <c r="AX63" s="46"/>
-      <c r="AY63" s="45"/>
-      <c r="AZ63" s="39"/>
-      <c r="BA63" s="46"/>
-      <c r="BB63" s="45"/>
-      <c r="BC63" s="46"/>
-      <c r="BD63" s="45"/>
-      <c r="BE63" s="39"/>
-      <c r="BF63" s="46"/>
-      <c r="BG63" s="45"/>
-      <c r="BH63" s="46"/>
-      <c r="BI63" s="45"/>
-      <c r="BJ63" s="33"/>
-      <c r="BK63" s="46"/>
-      <c r="BL63" s="45"/>
-      <c r="BM63" s="46"/>
-      <c r="BN63" s="45"/>
-      <c r="BO63" s="46"/>
-      <c r="BP63" s="8">
-        <f>SUM(D63:BO63)</f>
-        <v>1.5</v>
-      </c>
-      <c r="BQ63" s="31">
-        <f>C63-BP63</f>
-        <v>18.5</v>
-      </c>
-      <c r="BR63" s="10">
-        <f>C63-BP63-BQ63</f>
-        <v>0</v>
-      </c>
+      <c r="C63" s="12"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="65"/>
+      <c r="G63" s="66"/>
+      <c r="H63" s="65"/>
+      <c r="I63" s="66"/>
+      <c r="J63" s="67"/>
+      <c r="K63" s="64"/>
+      <c r="L63" s="68"/>
+      <c r="M63" s="66"/>
+      <c r="N63" s="65"/>
+      <c r="O63" s="66"/>
+      <c r="P63" s="65"/>
+      <c r="Q63" s="66"/>
+      <c r="R63" s="65"/>
+      <c r="S63" s="66"/>
+      <c r="T63" s="65"/>
+      <c r="U63" s="66"/>
+      <c r="V63" s="65"/>
+      <c r="W63" s="66"/>
+      <c r="X63" s="65"/>
+      <c r="Y63" s="66"/>
+      <c r="Z63" s="65"/>
+      <c r="AA63" s="66"/>
+      <c r="AB63" s="65"/>
+      <c r="AC63" s="66"/>
+      <c r="AD63" s="65"/>
+      <c r="AE63" s="66"/>
+      <c r="AF63" s="65"/>
+      <c r="AG63" s="66"/>
+      <c r="AH63" s="65"/>
+      <c r="AI63" s="66"/>
+      <c r="AJ63" s="67"/>
+      <c r="AK63" s="69"/>
+      <c r="AL63" s="67"/>
+      <c r="AM63" s="69"/>
+      <c r="AN63" s="66"/>
+      <c r="AO63" s="66"/>
+      <c r="AP63" s="67"/>
+      <c r="AQ63" s="69"/>
+      <c r="AR63" s="67"/>
+      <c r="AS63" s="69"/>
+      <c r="AT63" s="66"/>
+      <c r="AU63" s="66"/>
+      <c r="AV63" s="67"/>
+      <c r="AW63" s="69"/>
+      <c r="AX63" s="67"/>
+      <c r="AY63" s="69"/>
+      <c r="AZ63" s="66"/>
+      <c r="BA63" s="67"/>
+      <c r="BB63" s="69"/>
+      <c r="BC63" s="67"/>
+      <c r="BD63" s="69"/>
+      <c r="BE63" s="66"/>
+      <c r="BF63" s="67"/>
+      <c r="BG63" s="69"/>
+      <c r="BH63" s="67"/>
+      <c r="BI63" s="69"/>
+      <c r="BJ63" s="66"/>
+      <c r="BK63" s="67"/>
+      <c r="BL63" s="69"/>
+      <c r="BM63" s="67"/>
+      <c r="BN63" s="69"/>
+      <c r="BO63" s="67"/>
+      <c r="BP63" s="17"/>
+      <c r="BR63" s="13"/>
     </row>
     <row r="64" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="8">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D64" s="34"/>
       <c r="E64" s="35"/>
@@ -6819,20 +6836,14 @@
       <c r="U64" s="33"/>
       <c r="V64" s="59"/>
       <c r="W64" s="33"/>
-      <c r="X64" s="38">
-        <v>8</v>
-      </c>
-      <c r="Y64" s="39">
-        <v>3</v>
-      </c>
-      <c r="Z64" s="59">
-        <v>3</v>
-      </c>
+      <c r="X64" s="59"/>
+      <c r="Y64" s="33"/>
+      <c r="Z64" s="59"/>
       <c r="AA64" s="33"/>
       <c r="AB64" s="59"/>
       <c r="AC64" s="33"/>
-      <c r="AD64" s="59"/>
-      <c r="AE64" s="33"/>
+      <c r="AD64" s="38"/>
+      <c r="AE64" s="39"/>
       <c r="AF64" s="59"/>
       <c r="AG64" s="33"/>
       <c r="AH64" s="59"/>
@@ -6841,24 +6852,26 @@
       <c r="AK64" s="45"/>
       <c r="AL64" s="46"/>
       <c r="AM64" s="45"/>
-      <c r="AN64" s="33"/>
-      <c r="AO64" s="33"/>
+      <c r="AN64" s="39"/>
+      <c r="AO64" s="39"/>
       <c r="AP64" s="46"/>
       <c r="AQ64" s="45"/>
       <c r="AR64" s="46"/>
       <c r="AS64" s="45"/>
-      <c r="AT64" s="33"/>
-      <c r="AU64" s="33"/>
+      <c r="AT64" s="39">
+        <v>1.5</v>
+      </c>
+      <c r="AU64" s="39"/>
       <c r="AV64" s="46"/>
       <c r="AW64" s="45"/>
       <c r="AX64" s="46"/>
       <c r="AY64" s="45"/>
-      <c r="AZ64" s="33"/>
+      <c r="AZ64" s="39"/>
       <c r="BA64" s="46"/>
       <c r="BB64" s="45"/>
       <c r="BC64" s="46"/>
       <c r="BD64" s="45"/>
-      <c r="BE64" s="33"/>
+      <c r="BE64" s="39"/>
       <c r="BF64" s="46"/>
       <c r="BG64" s="45"/>
       <c r="BH64" s="46"/>
@@ -6871,25 +6884,26 @@
       <c r="BO64" s="46"/>
       <c r="BP64" s="8">
         <f>SUM(D64:BO64)</f>
-        <v>14</v>
-      </c>
-      <c r="BQ64" s="8">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="BQ64" s="31">
+        <f>C64-BP64</f>
+        <v>18.5</v>
       </c>
       <c r="BR64" s="10">
         <f>C64-BP64-BQ64</f>
-        <v>-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C65" s="8">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D65" s="34"/>
       <c r="E65" s="35"/>
@@ -6911,9 +6925,15 @@
       <c r="U65" s="33"/>
       <c r="V65" s="59"/>
       <c r="W65" s="33"/>
-      <c r="X65" s="59"/>
-      <c r="Y65" s="33"/>
-      <c r="Z65" s="59"/>
+      <c r="X65" s="38">
+        <v>8</v>
+      </c>
+      <c r="Y65" s="39">
+        <v>3</v>
+      </c>
+      <c r="Z65" s="59">
+        <v>3</v>
+      </c>
       <c r="AA65" s="33"/>
       <c r="AB65" s="59"/>
       <c r="AC65" s="33"/>
@@ -6945,11 +6965,11 @@
       <c r="BC65" s="46"/>
       <c r="BD65" s="45"/>
       <c r="BE65" s="33"/>
-      <c r="BF65" s="40"/>
-      <c r="BG65" s="42"/>
-      <c r="BH65" s="40"/>
-      <c r="BI65" s="42"/>
-      <c r="BJ65" s="39"/>
+      <c r="BF65" s="46"/>
+      <c r="BG65" s="45"/>
+      <c r="BH65" s="46"/>
+      <c r="BI65" s="45"/>
+      <c r="BJ65" s="33"/>
       <c r="BK65" s="46"/>
       <c r="BL65" s="45"/>
       <c r="BM65" s="46"/>
@@ -6957,26 +6977,25 @@
       <c r="BO65" s="46"/>
       <c r="BP65" s="8">
         <f>SUM(D65:BO65)</f>
+        <v>14</v>
+      </c>
+      <c r="BQ65" s="8">
         <v>0</v>
-      </c>
-      <c r="BQ65" s="8">
-        <f>C65-BP65</f>
-        <v>40</v>
       </c>
       <c r="BR65" s="10">
         <f>C65-BP65-BQ65</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="66" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C66" s="8">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="D66" s="34"/>
       <c r="E66" s="35"/>
@@ -7032,23 +7051,31 @@
       <c r="BC66" s="46"/>
       <c r="BD66" s="45"/>
       <c r="BE66" s="33"/>
-      <c r="BF66" s="46"/>
-      <c r="BG66" s="45"/>
-      <c r="BH66" s="46"/>
-      <c r="BI66" s="45"/>
+      <c r="BF66" s="40">
+        <v>6</v>
+      </c>
+      <c r="BG66" s="42">
+        <v>8</v>
+      </c>
+      <c r="BH66" s="40">
+        <v>8</v>
+      </c>
+      <c r="BI66" s="42">
+        <v>3</v>
+      </c>
       <c r="BJ66" s="39"/>
-      <c r="BK66" s="40"/>
+      <c r="BK66" s="46"/>
       <c r="BL66" s="45"/>
       <c r="BM66" s="46"/>
       <c r="BN66" s="45"/>
       <c r="BO66" s="46"/>
       <c r="BP66" s="8">
         <f>SUM(D66:BO66)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="BQ66" s="8">
         <f>C66-BP66</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="BR66" s="10">
         <f>C66-BP66-BQ66</f>
@@ -7056,8 +7083,15 @@
       </c>
     </row>
     <row r="67" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A67" s="6"/>
-      <c r="B67" s="14"/>
+      <c r="A67" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="8">
+        <v>5</v>
+      </c>
       <c r="D67" s="34"/>
       <c r="E67" s="35"/>
       <c r="F67" s="59"/>
@@ -7122,86 +7156,65 @@
       <c r="BM67" s="46"/>
       <c r="BN67" s="45"/>
       <c r="BO67" s="46"/>
-      <c r="BR67" s="10"/>
+      <c r="BP67" s="8">
+        <f>SUM(D67:BO67)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ67" s="8">
+        <f>C67-BP67</f>
+        <v>5</v>
+      </c>
+      <c r="BR67" s="10">
+        <f>C67-BP67-BQ67</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
-      <c r="B68" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="B68" s="14"/>
+      <c r="D68" s="34"/>
       <c r="E68" s="35"/>
-      <c r="F68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="F68" s="59"/>
       <c r="G68" s="33"/>
-      <c r="H68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="H68" s="59"/>
       <c r="I68" s="33"/>
       <c r="J68" s="46"/>
       <c r="K68" s="35"/>
-      <c r="L68" s="34"/>
+      <c r="L68" s="32"/>
       <c r="M68" s="33"/>
-      <c r="N68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="N68" s="59"/>
       <c r="O68" s="33"/>
-      <c r="P68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="P68" s="59"/>
       <c r="Q68" s="33"/>
-      <c r="R68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="R68" s="59"/>
       <c r="S68" s="33"/>
-      <c r="T68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="T68" s="59"/>
       <c r="U68" s="33"/>
-      <c r="V68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="V68" s="59"/>
       <c r="W68" s="33"/>
-      <c r="X68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="X68" s="59"/>
       <c r="Y68" s="33"/>
-      <c r="Z68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="Z68" s="59"/>
       <c r="AA68" s="33"/>
-      <c r="AB68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="AB68" s="59"/>
       <c r="AC68" s="33"/>
-      <c r="AD68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="AD68" s="59"/>
       <c r="AE68" s="33"/>
-      <c r="AF68" s="34"/>
+      <c r="AF68" s="59"/>
       <c r="AG68" s="33"/>
-      <c r="AH68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="AH68" s="59"/>
       <c r="AI68" s="33"/>
       <c r="AJ68" s="46"/>
       <c r="AK68" s="45"/>
       <c r="AL68" s="46"/>
       <c r="AM68" s="45"/>
-      <c r="AN68" s="81">
-        <v>0.5</v>
-      </c>
-      <c r="AO68" s="79"/>
+      <c r="AN68" s="33"/>
+      <c r="AO68" s="33"/>
       <c r="AP68" s="46"/>
       <c r="AQ68" s="45"/>
       <c r="AR68" s="46"/>
       <c r="AS68" s="45"/>
-      <c r="AT68" s="34">
-        <v>0.5</v>
-      </c>
+      <c r="AT68" s="33"/>
       <c r="AU68" s="33"/>
       <c r="AV68" s="46"/>
       <c r="AW68" s="45"/>
@@ -7223,64 +7236,86 @@
       <c r="BM68" s="46"/>
       <c r="BN68" s="45"/>
       <c r="BO68" s="46"/>
-      <c r="BP68" s="8">
-        <f>SUM(D68:BO68)</f>
-        <v>7.5</v>
-      </c>
-      <c r="BQ68" s="8">
-        <f>C68-BP68</f>
-        <v>-7.5</v>
-      </c>
-      <c r="BR68" s="10">
-        <f>C68-BP68-BQ68</f>
-        <v>0</v>
-      </c>
+      <c r="BR68" s="10"/>
     </row>
     <row r="69" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
-      <c r="D69" s="34"/>
+      <c r="B69" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="E69" s="35"/>
-      <c r="F69" s="59"/>
+      <c r="F69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="G69" s="33"/>
-      <c r="H69" s="59"/>
+      <c r="H69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="I69" s="33"/>
       <c r="J69" s="46"/>
       <c r="K69" s="35"/>
-      <c r="L69" s="32"/>
+      <c r="L69" s="34"/>
       <c r="M69" s="33"/>
-      <c r="N69" s="59"/>
+      <c r="N69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="O69" s="33"/>
-      <c r="P69" s="59"/>
+      <c r="P69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="Q69" s="33"/>
-      <c r="R69" s="59"/>
+      <c r="R69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="S69" s="33"/>
-      <c r="T69" s="59"/>
+      <c r="T69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="U69" s="33"/>
-      <c r="V69" s="59"/>
+      <c r="V69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="W69" s="33"/>
-      <c r="X69" s="59"/>
+      <c r="X69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="Y69" s="33"/>
-      <c r="Z69" s="59"/>
+      <c r="Z69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AA69" s="33"/>
-      <c r="AB69" s="59"/>
+      <c r="AB69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AC69" s="33"/>
-      <c r="AD69" s="59"/>
+      <c r="AD69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AE69" s="33"/>
-      <c r="AF69" s="59"/>
+      <c r="AF69" s="34"/>
       <c r="AG69" s="33"/>
-      <c r="AH69" s="59"/>
+      <c r="AH69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AI69" s="33"/>
       <c r="AJ69" s="46"/>
       <c r="AK69" s="45"/>
       <c r="AL69" s="46"/>
       <c r="AM69" s="45"/>
-      <c r="AN69" s="33"/>
-      <c r="AO69" s="33"/>
+      <c r="AN69" s="81">
+        <v>0.5</v>
+      </c>
+      <c r="AO69" s="79"/>
       <c r="AP69" s="46"/>
       <c r="AQ69" s="45"/>
       <c r="AR69" s="46"/>
       <c r="AS69" s="45"/>
-      <c r="AT69" s="33"/>
+      <c r="AT69" s="34">
+        <v>0.5</v>
+      </c>
       <c r="AU69" s="33"/>
       <c r="AV69" s="46"/>
       <c r="AW69" s="45"/>
@@ -7296,24 +7331,27 @@
       <c r="BG69" s="45"/>
       <c r="BH69" s="46"/>
       <c r="BI69" s="45"/>
-      <c r="BJ69" s="33"/>
-      <c r="BK69" s="46"/>
+      <c r="BJ69" s="39"/>
+      <c r="BK69" s="40"/>
       <c r="BL69" s="45"/>
       <c r="BM69" s="46"/>
       <c r="BN69" s="45"/>
       <c r="BO69" s="46"/>
-      <c r="BR69" s="10"/>
+      <c r="BP69" s="8">
+        <f>SUM(D69:BO69)</f>
+        <v>7.5</v>
+      </c>
+      <c r="BQ69" s="8">
+        <f>C69-BP69</f>
+        <v>-7.5</v>
+      </c>
+      <c r="BR69" s="10">
+        <f>C69-BP69-BQ69</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A70" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C70" s="8">
-        <v>90</v>
-      </c>
+      <c r="A70" s="6"/>
       <c r="D70" s="34"/>
       <c r="E70" s="35"/>
       <c r="F70" s="59"/>
@@ -7339,9 +7377,7 @@
       <c r="Z70" s="59"/>
       <c r="AA70" s="33"/>
       <c r="AB70" s="59"/>
-      <c r="AC70" s="33">
-        <v>6</v>
-      </c>
+      <c r="AC70" s="33"/>
       <c r="AD70" s="59"/>
       <c r="AE70" s="33"/>
       <c r="AF70" s="59"/>
@@ -7353,7 +7389,7 @@
       <c r="AL70" s="46"/>
       <c r="AM70" s="45"/>
       <c r="AN70" s="33"/>
-      <c r="AO70" s="79"/>
+      <c r="AO70" s="33"/>
       <c r="AP70" s="46"/>
       <c r="AQ70" s="45"/>
       <c r="AR70" s="46"/>
@@ -7380,22 +7416,18 @@
       <c r="BM70" s="46"/>
       <c r="BN70" s="45"/>
       <c r="BO70" s="46"/>
-      <c r="BP70" s="8">
-        <f>SUM(D70:BO70)</f>
-        <v>6</v>
-      </c>
-      <c r="BQ70" s="8">
-        <f>C70-BP70</f>
-        <v>84</v>
-      </c>
-      <c r="BR70" s="10">
-        <f>C70-BP70-BQ70</f>
-        <v>0</v>
-      </c>
+      <c r="BR70" s="10"/>
     </row>
     <row r="71" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A71" s="6"/>
-      <c r="C71" s="18"/>
+      <c r="A71" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="8">
+        <v>90</v>
+      </c>
       <c r="D71" s="34"/>
       <c r="E71" s="35"/>
       <c r="F71" s="59"/>
@@ -7421,7 +7453,9 @@
       <c r="Z71" s="59"/>
       <c r="AA71" s="33"/>
       <c r="AB71" s="59"/>
-      <c r="AC71" s="33"/>
+      <c r="AC71" s="33">
+        <v>6</v>
+      </c>
       <c r="AD71" s="59"/>
       <c r="AE71" s="33"/>
       <c r="AF71" s="59"/>
@@ -7460,6 +7494,18 @@
       <c r="BM71" s="46"/>
       <c r="BN71" s="45"/>
       <c r="BO71" s="46"/>
+      <c r="BP71" s="8">
+        <f>SUM(D71:BO71)</f>
+        <v>6</v>
+      </c>
+      <c r="BQ71" s="8">
+        <f>C71-BP71</f>
+        <v>84</v>
+      </c>
+      <c r="BR71" s="10">
+        <f>C71-BP71-BQ71</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
@@ -7528,11 +7574,9 @@
       <c r="BM72" s="46"/>
       <c r="BN72" s="45"/>
       <c r="BO72" s="46"/>
-      <c r="BR72" s="10"/>
     </row>
     <row r="73" spans="1:70" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
-      <c r="B73" s="14"/>
       <c r="C73" s="18"/>
       <c r="D73" s="34"/>
       <c r="E73" s="35"/>
@@ -7598,248 +7642,351 @@
       <c r="BM73" s="46"/>
       <c r="BN73" s="45"/>
       <c r="BO73" s="46"/>
-      <c r="BP73" s="8">
-        <f>SUM(D73:BO73)</f>
+      <c r="BR73" s="10"/>
+    </row>
+    <row r="74" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="A74" s="6"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="46"/>
+      <c r="K74" s="35"/>
+      <c r="L74" s="32"/>
+      <c r="M74" s="33"/>
+      <c r="N74" s="59"/>
+      <c r="O74" s="33"/>
+      <c r="P74" s="59"/>
+      <c r="Q74" s="33"/>
+      <c r="R74" s="59"/>
+      <c r="S74" s="33"/>
+      <c r="T74" s="59"/>
+      <c r="U74" s="33"/>
+      <c r="V74" s="59"/>
+      <c r="W74" s="33"/>
+      <c r="X74" s="59"/>
+      <c r="Y74" s="33"/>
+      <c r="Z74" s="59"/>
+      <c r="AA74" s="33"/>
+      <c r="AB74" s="59"/>
+      <c r="AC74" s="33"/>
+      <c r="AD74" s="59"/>
+      <c r="AE74" s="33"/>
+      <c r="AF74" s="59"/>
+      <c r="AG74" s="33"/>
+      <c r="AH74" s="59"/>
+      <c r="AI74" s="33"/>
+      <c r="AJ74" s="46"/>
+      <c r="AK74" s="45"/>
+      <c r="AL74" s="46"/>
+      <c r="AM74" s="45"/>
+      <c r="AN74" s="33"/>
+      <c r="AO74" s="79"/>
+      <c r="AP74" s="46"/>
+      <c r="AQ74" s="45"/>
+      <c r="AR74" s="46"/>
+      <c r="AS74" s="45"/>
+      <c r="AT74" s="33"/>
+      <c r="AU74" s="33"/>
+      <c r="AV74" s="46"/>
+      <c r="AW74" s="45"/>
+      <c r="AX74" s="46"/>
+      <c r="AY74" s="45"/>
+      <c r="AZ74" s="33"/>
+      <c r="BA74" s="46"/>
+      <c r="BB74" s="45"/>
+      <c r="BC74" s="46"/>
+      <c r="BD74" s="45"/>
+      <c r="BE74" s="33"/>
+      <c r="BF74" s="46"/>
+      <c r="BG74" s="45"/>
+      <c r="BH74" s="46"/>
+      <c r="BI74" s="45"/>
+      <c r="BJ74" s="33"/>
+      <c r="BK74" s="46"/>
+      <c r="BL74" s="45"/>
+      <c r="BM74" s="46"/>
+      <c r="BN74" s="45"/>
+      <c r="BO74" s="46"/>
+      <c r="BP74" s="8">
+        <f>SUM(D74:BO74)</f>
         <v>0</v>
       </c>
-      <c r="BQ73" s="8">
-        <f>C73-BP73</f>
+      <c r="BQ74" s="8">
+        <f>C74-BP74</f>
         <v>0</v>
       </c>
-      <c r="BR73" s="10">
-        <f>C73-BP73-BQ73</f>
+      <c r="BR74" s="10">
+        <f>C74-BP74-BQ74</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="11"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="63"/>
-      <c r="E74" s="64"/>
-      <c r="F74" s="65"/>
-      <c r="G74" s="66"/>
-      <c r="H74" s="65"/>
-      <c r="I74" s="66"/>
-      <c r="J74" s="67"/>
-      <c r="K74" s="35"/>
-      <c r="L74" s="65"/>
-      <c r="M74" s="66"/>
-      <c r="N74" s="65"/>
-      <c r="O74" s="66"/>
-      <c r="P74" s="65"/>
-      <c r="Q74" s="66"/>
-      <c r="R74" s="65"/>
-      <c r="S74" s="66"/>
-      <c r="T74" s="65"/>
-      <c r="U74" s="66"/>
-      <c r="V74" s="65"/>
-      <c r="W74" s="66"/>
-      <c r="X74" s="65"/>
-      <c r="Y74" s="66"/>
-      <c r="Z74" s="65"/>
-      <c r="AA74" s="66"/>
-      <c r="AB74" s="65"/>
-      <c r="AC74" s="66"/>
-      <c r="AD74" s="65"/>
-      <c r="AE74" s="66"/>
-      <c r="AF74" s="65"/>
-      <c r="AG74" s="66"/>
-      <c r="AH74" s="65"/>
-      <c r="AI74" s="66"/>
-      <c r="AJ74" s="67"/>
-      <c r="AK74" s="69"/>
-      <c r="AL74" s="67"/>
-      <c r="AM74" s="69"/>
-      <c r="AN74" s="66"/>
-      <c r="AO74" s="80"/>
-      <c r="AP74" s="67"/>
-      <c r="AQ74" s="69"/>
-      <c r="AR74" s="67"/>
-      <c r="AS74" s="69"/>
-      <c r="AT74" s="66"/>
-      <c r="AU74" s="109"/>
-      <c r="AV74" s="67"/>
-      <c r="AW74" s="69"/>
-      <c r="AX74" s="67"/>
-      <c r="AY74" s="69"/>
-      <c r="AZ74" s="66"/>
-      <c r="BA74" s="67"/>
-      <c r="BB74" s="69"/>
-      <c r="BC74" s="67"/>
-      <c r="BD74" s="69"/>
-      <c r="BE74" s="66"/>
-      <c r="BF74" s="67"/>
-      <c r="BG74" s="69"/>
-      <c r="BH74" s="67"/>
-      <c r="BI74" s="69"/>
-      <c r="BJ74" s="66"/>
-      <c r="BK74" s="67"/>
-      <c r="BL74" s="69"/>
-      <c r="BM74" s="67"/>
-      <c r="BN74" s="69"/>
-      <c r="BO74" s="67"/>
-      <c r="BP74" s="12"/>
-      <c r="BQ74" s="12"/>
-      <c r="BR74" s="13"/>
-    </row>
-    <row r="75" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A75" s="19"/>
-      <c r="B75" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C75" s="21">
-        <f>SUM(C5:C13)+SUM(C16:C33)+SUM(C37:C61)+SUM(C63:C74)</f>
-        <v>466</v>
-      </c>
-      <c r="D75" s="94">
-        <f>SUM(D4:E74)</f>
-        <v>10.5</v>
-      </c>
-      <c r="E75" s="86"/>
-      <c r="F75" s="83">
-        <f>SUM(F4:G74)</f>
-        <v>7.5</v>
-      </c>
-      <c r="G75" s="86"/>
-      <c r="H75" s="83">
-        <f>SUM(H4:I74)</f>
-        <v>4.5</v>
-      </c>
-      <c r="I75" s="86"/>
-      <c r="J75" s="83">
-        <f>SUM(J4:K74)</f>
-        <v>0</v>
-      </c>
-      <c r="K75" s="86"/>
-      <c r="L75" s="83">
-        <f>SUM(L4:M74)</f>
-        <v>18</v>
-      </c>
-      <c r="M75" s="86"/>
-      <c r="N75" s="83">
-        <f>SUM(N4:O74)</f>
-        <v>11.5</v>
-      </c>
-      <c r="O75" s="86"/>
-      <c r="P75" s="83">
-        <f>SUM(P4:Q74)</f>
-        <v>11.5</v>
-      </c>
-      <c r="Q75" s="86"/>
-      <c r="R75" s="83">
-        <f>SUM(R4:S74)</f>
-        <v>4.5</v>
-      </c>
-      <c r="S75" s="86"/>
-      <c r="T75" s="83">
-        <f>SUM(T4:U74)</f>
-        <v>7.5</v>
-      </c>
-      <c r="U75" s="86"/>
-      <c r="V75" s="83">
-        <f>SUM(V4:W74)</f>
-        <v>9.5</v>
-      </c>
-      <c r="W75" s="86"/>
-      <c r="X75" s="83">
-        <f>SUM(X4:Y74)</f>
-        <v>11.5</v>
-      </c>
-      <c r="Y75" s="86"/>
-      <c r="Z75" s="83">
-        <f>SUM(Z4:AA74)</f>
-        <v>17.5</v>
-      </c>
-      <c r="AA75" s="86"/>
-      <c r="AB75" s="83">
-        <f>SUM(AB4:AC74)</f>
-        <v>19.5</v>
-      </c>
-      <c r="AC75" s="86"/>
-      <c r="AD75" s="83">
-        <f>SUM(AD4:AE74)</f>
-        <v>12.5</v>
-      </c>
-      <c r="AE75" s="86"/>
-      <c r="AF75" s="83">
-        <f>SUM(AF4:AG74)</f>
-        <v>16</v>
-      </c>
-      <c r="AG75" s="87"/>
-      <c r="AH75" s="83">
-        <f>SUM(AH4:AI74)</f>
-        <v>0.5</v>
-      </c>
-      <c r="AI75" s="87"/>
-      <c r="AJ75" s="83">
-        <f>SUM(AJ4:AO74)</f>
-        <v>48</v>
-      </c>
-      <c r="AK75" s="84"/>
-      <c r="AL75" s="84"/>
-      <c r="AM75" s="84"/>
-      <c r="AN75" s="85"/>
-      <c r="AO75" s="75"/>
-      <c r="AP75" s="83">
-        <f>SUM(AP4:AU74)</f>
-        <v>44</v>
-      </c>
-      <c r="AQ75" s="84"/>
-      <c r="AR75" s="84"/>
-      <c r="AS75" s="84"/>
-      <c r="AT75" s="85"/>
-      <c r="AU75" s="78"/>
-      <c r="AV75" s="83">
-        <f>SUM(AV4:AZ74)</f>
-        <v>34</v>
-      </c>
-      <c r="AW75" s="84"/>
-      <c r="AX75" s="84"/>
-      <c r="AY75" s="84"/>
-      <c r="AZ75" s="85"/>
-      <c r="BA75" s="83">
-        <f>SUM(BA4:BE74)</f>
-        <v>0</v>
-      </c>
-      <c r="BB75" s="84"/>
-      <c r="BC75" s="84"/>
-      <c r="BD75" s="84"/>
-      <c r="BE75" s="85"/>
-      <c r="BF75" s="83">
-        <f>SUM(BF4:BJ74)</f>
-        <v>0</v>
-      </c>
-      <c r="BG75" s="84"/>
-      <c r="BH75" s="84"/>
-      <c r="BI75" s="84"/>
-      <c r="BJ75" s="85"/>
-      <c r="BK75" s="83">
-        <f>SUM(BK4:BO74)</f>
-        <v>0</v>
-      </c>
-      <c r="BL75" s="84"/>
-      <c r="BM75" s="84"/>
-      <c r="BN75" s="84"/>
-      <c r="BO75" s="85"/>
-      <c r="BP75" s="21">
-        <f>SUM(BP4:BP74)</f>
-        <v>285.5</v>
-      </c>
-      <c r="BQ75" s="21">
-        <f>SUM(BQ4:BQ74)</f>
-        <v>206.5</v>
-      </c>
-      <c r="BR75" s="22">
-        <f>SUM(BR4:BR74)</f>
-        <v>18</v>
-      </c>
+    <row r="75" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="11"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="63"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="65"/>
+      <c r="G75" s="66"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="66"/>
+      <c r="J75" s="67"/>
+      <c r="K75" s="35"/>
+      <c r="L75" s="65"/>
+      <c r="M75" s="66"/>
+      <c r="N75" s="65"/>
+      <c r="O75" s="66"/>
+      <c r="P75" s="65"/>
+      <c r="Q75" s="66"/>
+      <c r="R75" s="65"/>
+      <c r="S75" s="66"/>
+      <c r="T75" s="65"/>
+      <c r="U75" s="66"/>
+      <c r="V75" s="65"/>
+      <c r="W75" s="66"/>
+      <c r="X75" s="65"/>
+      <c r="Y75" s="66"/>
+      <c r="Z75" s="65"/>
+      <c r="AA75" s="66"/>
+      <c r="AB75" s="65"/>
+      <c r="AC75" s="66"/>
+      <c r="AD75" s="65"/>
+      <c r="AE75" s="66"/>
+      <c r="AF75" s="65"/>
+      <c r="AG75" s="66"/>
+      <c r="AH75" s="65"/>
+      <c r="AI75" s="66"/>
+      <c r="AJ75" s="67"/>
+      <c r="AK75" s="69"/>
+      <c r="AL75" s="67"/>
+      <c r="AM75" s="69"/>
+      <c r="AN75" s="66"/>
+      <c r="AO75" s="80"/>
+      <c r="AP75" s="67"/>
+      <c r="AQ75" s="69"/>
+      <c r="AR75" s="67"/>
+      <c r="AS75" s="69"/>
+      <c r="AT75" s="66"/>
+      <c r="AU75" s="83"/>
+      <c r="AV75" s="67"/>
+      <c r="AW75" s="69"/>
+      <c r="AX75" s="67"/>
+      <c r="AY75" s="69"/>
+      <c r="AZ75" s="66"/>
+      <c r="BA75" s="67"/>
+      <c r="BB75" s="69"/>
+      <c r="BC75" s="67"/>
+      <c r="BD75" s="69"/>
+      <c r="BE75" s="66"/>
+      <c r="BF75" s="67"/>
+      <c r="BG75" s="69"/>
+      <c r="BH75" s="67"/>
+      <c r="BI75" s="69"/>
+      <c r="BJ75" s="66"/>
+      <c r="BK75" s="67"/>
+      <c r="BL75" s="69"/>
+      <c r="BM75" s="67"/>
+      <c r="BN75" s="69"/>
+      <c r="BO75" s="67"/>
+      <c r="BP75" s="12"/>
+      <c r="BQ75" s="12"/>
+      <c r="BR75" s="13"/>
     </row>
     <row r="76" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="I76" s="24"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76" s="21">
+        <f>SUM(C5:C13)+SUM(C16:C33)+SUM(C37:C62)+SUM(C64:C75)</f>
+        <v>466</v>
+      </c>
+      <c r="D76" s="101">
+        <f>SUM(D4:E75)</f>
+        <v>10.5</v>
+      </c>
+      <c r="E76" s="102"/>
+      <c r="F76" s="103">
+        <f>SUM(F4:G75)</f>
+        <v>7.5</v>
+      </c>
+      <c r="G76" s="102"/>
+      <c r="H76" s="103">
+        <f>SUM(H4:I75)</f>
+        <v>4.5</v>
+      </c>
+      <c r="I76" s="102"/>
+      <c r="J76" s="103">
+        <f>SUM(J4:K75)</f>
+        <v>0</v>
+      </c>
+      <c r="K76" s="102"/>
+      <c r="L76" s="103">
+        <f>SUM(L4:M75)</f>
+        <v>18</v>
+      </c>
+      <c r="M76" s="102"/>
+      <c r="N76" s="103">
+        <f>SUM(N4:O75)</f>
+        <v>11.5</v>
+      </c>
+      <c r="O76" s="102"/>
+      <c r="P76" s="103">
+        <f>SUM(P4:Q75)</f>
+        <v>11.5</v>
+      </c>
+      <c r="Q76" s="102"/>
+      <c r="R76" s="103">
+        <f>SUM(R4:S75)</f>
+        <v>4.5</v>
+      </c>
+      <c r="S76" s="102"/>
+      <c r="T76" s="103">
+        <f>SUM(T4:U75)</f>
+        <v>7.5</v>
+      </c>
+      <c r="U76" s="102"/>
+      <c r="V76" s="103">
+        <f>SUM(V4:W75)</f>
+        <v>9.5</v>
+      </c>
+      <c r="W76" s="102"/>
+      <c r="X76" s="103">
+        <f>SUM(X4:Y75)</f>
+        <v>11.5</v>
+      </c>
+      <c r="Y76" s="102"/>
+      <c r="Z76" s="103">
+        <f>SUM(Z4:AA75)</f>
+        <v>17.5</v>
+      </c>
+      <c r="AA76" s="102"/>
+      <c r="AB76" s="103">
+        <f>SUM(AB4:AC75)</f>
+        <v>19.5</v>
+      </c>
+      <c r="AC76" s="102"/>
+      <c r="AD76" s="103">
+        <f>SUM(AD4:AE75)</f>
+        <v>12.5</v>
+      </c>
+      <c r="AE76" s="102"/>
+      <c r="AF76" s="103">
+        <f>SUM(AF4:AG75)</f>
+        <v>16</v>
+      </c>
+      <c r="AG76" s="109"/>
+      <c r="AH76" s="103">
+        <f>SUM(AH4:AI75)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AI76" s="109"/>
+      <c r="AJ76" s="103">
+        <f>SUM(AJ4:AO75)</f>
+        <v>48</v>
+      </c>
+      <c r="AK76" s="107"/>
+      <c r="AL76" s="107"/>
+      <c r="AM76" s="107"/>
+      <c r="AN76" s="108"/>
+      <c r="AO76" s="75"/>
+      <c r="AP76" s="103">
+        <f>SUM(AP4:AU75)</f>
+        <v>44</v>
+      </c>
+      <c r="AQ76" s="107"/>
+      <c r="AR76" s="107"/>
+      <c r="AS76" s="107"/>
+      <c r="AT76" s="108"/>
+      <c r="AU76" s="78"/>
+      <c r="AV76" s="103">
+        <f>SUM(AV4:AZ75)</f>
+        <v>43</v>
+      </c>
+      <c r="AW76" s="107"/>
+      <c r="AX76" s="107"/>
+      <c r="AY76" s="107"/>
+      <c r="AZ76" s="108"/>
+      <c r="BA76" s="103">
+        <f>SUM(BA4:BE75)</f>
+        <v>40</v>
+      </c>
+      <c r="BB76" s="107"/>
+      <c r="BC76" s="107"/>
+      <c r="BD76" s="107"/>
+      <c r="BE76" s="108"/>
+      <c r="BF76" s="103">
+        <f>SUM(BF4:BJ75)</f>
+        <v>27</v>
+      </c>
+      <c r="BG76" s="107"/>
+      <c r="BH76" s="107"/>
+      <c r="BI76" s="107"/>
+      <c r="BJ76" s="108"/>
+      <c r="BK76" s="103">
+        <f>SUM(BK4:BO75)</f>
+        <v>0</v>
+      </c>
+      <c r="BL76" s="107"/>
+      <c r="BM76" s="107"/>
+      <c r="BN76" s="107"/>
+      <c r="BO76" s="108"/>
+      <c r="BP76" s="21">
+        <f>SUM(BP4:BP75)</f>
+        <v>358.5</v>
+      </c>
+      <c r="BQ76" s="21">
+        <f>SUM(BQ4:BQ75)</f>
+        <v>152.5</v>
+      </c>
+      <c r="BR76" s="22">
+        <f>SUM(BR4:BR75)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:70" x14ac:dyDescent="0.3">
+      <c r="I77" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="AP76:AT76"/>
+    <mergeCell ref="AV76:AZ76"/>
+    <mergeCell ref="BA76:BE76"/>
+    <mergeCell ref="BF76:BJ76"/>
+    <mergeCell ref="BK76:BO76"/>
+    <mergeCell ref="AJ76:AN76"/>
+    <mergeCell ref="N76:O76"/>
+    <mergeCell ref="P76:Q76"/>
+    <mergeCell ref="R76:S76"/>
+    <mergeCell ref="T76:U76"/>
+    <mergeCell ref="V76:W76"/>
+    <mergeCell ref="X76:Y76"/>
+    <mergeCell ref="Z76:AA76"/>
+    <mergeCell ref="AB76:AC76"/>
+    <mergeCell ref="AD76:AE76"/>
+    <mergeCell ref="AF76:AG76"/>
+    <mergeCell ref="AH76:AI76"/>
+    <mergeCell ref="AP3:AT3"/>
+    <mergeCell ref="AV3:AZ3"/>
+    <mergeCell ref="BA3:BE3"/>
+    <mergeCell ref="BF3:BJ3"/>
+    <mergeCell ref="BK3:BO3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="L76:M76"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="D1:BO1"/>
@@ -7856,39 +8003,6 @@
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H75:I75"/>
-    <mergeCell ref="J75:K75"/>
-    <mergeCell ref="L75:M75"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AV3:AZ3"/>
-    <mergeCell ref="BA3:BE3"/>
-    <mergeCell ref="BF3:BJ3"/>
-    <mergeCell ref="BK3:BO3"/>
-    <mergeCell ref="AJ75:AN75"/>
-    <mergeCell ref="N75:O75"/>
-    <mergeCell ref="P75:Q75"/>
-    <mergeCell ref="R75:S75"/>
-    <mergeCell ref="T75:U75"/>
-    <mergeCell ref="V75:W75"/>
-    <mergeCell ref="X75:Y75"/>
-    <mergeCell ref="Z75:AA75"/>
-    <mergeCell ref="AB75:AC75"/>
-    <mergeCell ref="AD75:AE75"/>
-    <mergeCell ref="AF75:AG75"/>
-    <mergeCell ref="AH75:AI75"/>
-    <mergeCell ref="AP75:AT75"/>
-    <mergeCell ref="AV75:AZ75"/>
-    <mergeCell ref="BA75:BE75"/>
-    <mergeCell ref="BF75:BJ75"/>
-    <mergeCell ref="BK75:BO75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="63" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fin rapport + dernières corrections
</commit_message>
<xml_diff>
--- a/01_doc/Planning.xlsx
+++ b/01_doc/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naily\Documents\01_HEIG\01_TB\01_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E8E780-03C1-495C-B1A9-3CE835731BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E151C5-1DC1-4162-9A7B-E3550045D259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22236" windowHeight="13176" xr2:uid="{F59D9D10-3A89-4134-8555-53CD5E65A538}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>Tâche</t>
   </si>
@@ -162,33 +162,18 @@
     <t>Planning</t>
   </si>
   <si>
-    <t>Recherche système existants</t>
-  </si>
-  <si>
     <t>Recherche informative</t>
   </si>
   <si>
-    <t>Recherche Technologies</t>
-  </si>
-  <si>
     <t>Elaboration et vérification du projet</t>
   </si>
   <si>
     <t>Traitement d'un plan</t>
   </si>
   <si>
-    <t>Conversion format compatible GeoMapFish</t>
-  </si>
-  <si>
-    <t>Géoréférençage du plan</t>
-  </si>
-  <si>
     <t>Design du site</t>
   </si>
   <si>
-    <t>PipelinCI/CD</t>
-  </si>
-  <si>
     <t>Définition du projet</t>
   </si>
   <si>
@@ -201,9 +186,6 @@
     <t>Frontend</t>
   </si>
   <si>
-    <t xml:space="preserve">Creation projet basique </t>
-  </si>
-  <si>
     <t>20.50.20</t>
   </si>
   <si>
@@ -216,9 +198,6 @@
     <t>20.60.10</t>
   </si>
   <si>
-    <t xml:space="preserve">Envoi des données géographqiue </t>
-  </si>
-  <si>
     <t>V0.2 - Affichage des plans</t>
   </si>
   <si>
@@ -240,9 +219,6 @@
     <t>Outil changement d'étage</t>
   </si>
   <si>
-    <t>Outil changement de site</t>
-  </si>
-  <si>
     <t>Adaptation selon zoom</t>
   </si>
   <si>
@@ -273,15 +249,9 @@
     <t>Déploiement serveur</t>
   </si>
   <si>
-    <t>Conversion format geojson + shapefile</t>
-  </si>
-  <si>
     <t>30.20.20</t>
   </si>
   <si>
-    <t>Intégraition des données géographique dans la BDD</t>
-  </si>
-  <si>
     <t>Mise en place complète du serveur API</t>
   </si>
   <si>
@@ -333,12 +303,6 @@
     <t>30.40.60</t>
   </si>
   <si>
-    <t>création test</t>
-  </si>
-  <si>
-    <t>refactoring</t>
-  </si>
-  <si>
     <t>30.40.70</t>
   </si>
   <si>
@@ -346,6 +310,51 @@
   </si>
   <si>
     <t>30.40.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conversion format compatible </t>
+  </si>
+  <si>
+    <t>Pipeline CI/CD</t>
+  </si>
+  <si>
+    <t>Géoréférencement du plan</t>
+  </si>
+  <si>
+    <t>Conversion format GeoJson + shapefile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Envoi des données géographiques </t>
+  </si>
+  <si>
+    <t>Pipelinw CI/CD</t>
+  </si>
+  <si>
+    <t>Géoréférencement des plans</t>
+  </si>
+  <si>
+    <t>Intégration des données géographiques dans la BDD</t>
+  </si>
+  <si>
+    <t>Outil changement de bâtiments</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Recherche de systèmes existants</t>
+  </si>
+  <si>
+    <t>Recherche technologique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création projet basique </t>
+  </si>
+  <si>
+    <t>Création test</t>
   </si>
 </sst>
 </file>
@@ -403,7 +412,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -937,12 +946,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="double">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="double">
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -951,7 +984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1151,109 +1184,106 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1573,16 +1603,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BS77"/>
+  <dimension ref="A1:BT74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X52" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BR76" sqref="BR76"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="86" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="8" customWidth="1"/>
     <col min="4" max="4" width="3.6640625" style="8" customWidth="1"/>
     <col min="5" max="5" width="1.88671875" style="9" customWidth="1"/>
@@ -1617,301 +1647,304 @@
     <col min="34" max="34" width="3.6640625" style="9" customWidth="1"/>
     <col min="35" max="35" width="2" style="9" customWidth="1"/>
     <col min="36" max="40" width="3.6640625" style="9" customWidth="1"/>
-    <col min="41" max="41" width="3.6640625" style="82" customWidth="1"/>
-    <col min="42" max="67" width="3.6640625" style="9" customWidth="1"/>
-    <col min="68" max="68" width="12" style="8" customWidth="1"/>
-    <col min="69" max="69" width="12.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.44140625" style="25"/>
+    <col min="41" max="41" width="3.6640625" style="78" customWidth="1"/>
+    <col min="42" max="68" width="3.6640625" style="9" customWidth="1"/>
+    <col min="69" max="69" width="12" style="8" customWidth="1"/>
+    <col min="70" max="70" width="12.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="11.44140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="84" t="s">
+    <row r="1" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="93" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="91"/>
-      <c r="AD1" s="91"/>
-      <c r="AE1" s="91"/>
-      <c r="AF1" s="91"/>
-      <c r="AG1" s="91"/>
-      <c r="AH1" s="91"/>
-      <c r="AI1" s="91"/>
-      <c r="AJ1" s="91"/>
-      <c r="AK1" s="91"/>
-      <c r="AL1" s="91"/>
-      <c r="AM1" s="91"/>
-      <c r="AN1" s="91"/>
-      <c r="AO1" s="91"/>
-      <c r="AP1" s="91"/>
-      <c r="AQ1" s="91"/>
-      <c r="AR1" s="91"/>
-      <c r="AS1" s="91"/>
-      <c r="AT1" s="91"/>
-      <c r="AU1" s="91"/>
-      <c r="AV1" s="91"/>
-      <c r="AW1" s="91"/>
-      <c r="AX1" s="91"/>
-      <c r="AY1" s="91"/>
-      <c r="AZ1" s="91"/>
-      <c r="BA1" s="91"/>
-      <c r="BB1" s="91"/>
-      <c r="BC1" s="91"/>
-      <c r="BD1" s="91"/>
-      <c r="BE1" s="91"/>
-      <c r="BF1" s="91"/>
-      <c r="BG1" s="91"/>
-      <c r="BH1" s="91"/>
-      <c r="BI1" s="91"/>
-      <c r="BJ1" s="91"/>
-      <c r="BK1" s="91"/>
-      <c r="BL1" s="91"/>
-      <c r="BM1" s="91"/>
-      <c r="BN1" s="91"/>
-      <c r="BO1" s="91"/>
-      <c r="BP1" s="47" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="97"/>
+      <c r="N1" s="97"/>
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="97"/>
+      <c r="U1" s="97"/>
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97"/>
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97"/>
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97"/>
+      <c r="AL1" s="97"/>
+      <c r="AM1" s="97"/>
+      <c r="AN1" s="97"/>
+      <c r="AO1" s="97"/>
+      <c r="AP1" s="97"/>
+      <c r="AQ1" s="97"/>
+      <c r="AR1" s="97"/>
+      <c r="AS1" s="97"/>
+      <c r="AT1" s="97"/>
+      <c r="AU1" s="97"/>
+      <c r="AV1" s="97"/>
+      <c r="AW1" s="97"/>
+      <c r="AX1" s="97"/>
+      <c r="AY1" s="97"/>
+      <c r="AZ1" s="97"/>
+      <c r="BA1" s="97"/>
+      <c r="BB1" s="97"/>
+      <c r="BC1" s="97"/>
+      <c r="BD1" s="97"/>
+      <c r="BE1" s="97"/>
+      <c r="BF1" s="97"/>
+      <c r="BG1" s="97"/>
+      <c r="BH1" s="97"/>
+      <c r="BI1" s="97"/>
+      <c r="BJ1" s="97"/>
+      <c r="BK1" s="97"/>
+      <c r="BL1" s="97"/>
+      <c r="BM1" s="97"/>
+      <c r="BN1" s="97"/>
+      <c r="BO1" s="97"/>
+      <c r="BP1" s="97"/>
       <c r="BQ1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="BR1" s="92" t="s">
+      <c r="BR1" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS1" s="98" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:70" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="85"/>
-      <c r="B2" s="88"/>
+    <row r="2" spans="1:71" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="91"/>
+      <c r="B2" s="94"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="95" t="s">
+      <c r="D2" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="96"/>
-      <c r="U2" s="96"/>
-      <c r="V2" s="96"/>
-      <c r="W2" s="96"/>
-      <c r="X2" s="96"/>
-      <c r="Y2" s="96"/>
-      <c r="Z2" s="96"/>
-      <c r="AA2" s="96"/>
-      <c r="AB2" s="96"/>
-      <c r="AC2" s="96"/>
-      <c r="AD2" s="96"/>
-      <c r="AE2" s="96"/>
-      <c r="AF2" s="96"/>
-      <c r="AG2" s="96"/>
-      <c r="AH2" s="96"/>
-      <c r="AI2" s="96"/>
-      <c r="AJ2" s="96"/>
-      <c r="AK2" s="96"/>
-      <c r="AL2" s="96"/>
-      <c r="AM2" s="96"/>
-      <c r="AN2" s="96"/>
-      <c r="AO2" s="96"/>
-      <c r="AP2" s="96"/>
-      <c r="AQ2" s="96"/>
-      <c r="AR2" s="96"/>
-      <c r="AS2" s="96"/>
-      <c r="AT2" s="96"/>
-      <c r="AU2" s="96"/>
-      <c r="AV2" s="96"/>
-      <c r="AW2" s="96"/>
-      <c r="AX2" s="96"/>
-      <c r="AY2" s="96"/>
-      <c r="AZ2" s="96"/>
-      <c r="BA2" s="96"/>
-      <c r="BB2" s="96"/>
-      <c r="BC2" s="96"/>
-      <c r="BD2" s="96"/>
-      <c r="BE2" s="96"/>
-      <c r="BF2" s="96"/>
-      <c r="BG2" s="96"/>
-      <c r="BH2" s="96"/>
-      <c r="BI2" s="96"/>
-      <c r="BJ2" s="96"/>
-      <c r="BK2" s="96"/>
-      <c r="BL2" s="96"/>
-      <c r="BM2" s="96"/>
-      <c r="BN2" s="96"/>
-      <c r="BO2" s="96"/>
-      <c r="BP2" s="3"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="102"/>
+      <c r="Y2" s="102"/>
+      <c r="Z2" s="102"/>
+      <c r="AA2" s="102"/>
+      <c r="AB2" s="102"/>
+      <c r="AC2" s="102"/>
+      <c r="AD2" s="102"/>
+      <c r="AE2" s="102"/>
+      <c r="AF2" s="102"/>
+      <c r="AG2" s="102"/>
+      <c r="AH2" s="102"/>
+      <c r="AI2" s="102"/>
+      <c r="AJ2" s="102"/>
+      <c r="AK2" s="102"/>
+      <c r="AL2" s="102"/>
+      <c r="AM2" s="102"/>
+      <c r="AN2" s="102"/>
+      <c r="AO2" s="102"/>
+      <c r="AP2" s="102"/>
+      <c r="AQ2" s="102"/>
+      <c r="AR2" s="102"/>
+      <c r="AS2" s="102"/>
+      <c r="AT2" s="102"/>
+      <c r="AU2" s="102"/>
+      <c r="AV2" s="102"/>
+      <c r="AW2" s="102"/>
+      <c r="AX2" s="102"/>
+      <c r="AY2" s="102"/>
+      <c r="AZ2" s="102"/>
+      <c r="BA2" s="102"/>
+      <c r="BB2" s="102"/>
+      <c r="BC2" s="102"/>
+      <c r="BD2" s="102"/>
+      <c r="BE2" s="102"/>
+      <c r="BF2" s="102"/>
+      <c r="BG2" s="102"/>
+      <c r="BH2" s="102"/>
+      <c r="BI2" s="102"/>
+      <c r="BJ2" s="102"/>
+      <c r="BK2" s="102"/>
+      <c r="BL2" s="102"/>
+      <c r="BM2" s="102"/>
+      <c r="BN2" s="102"/>
+      <c r="BO2" s="102"/>
+      <c r="BP2" s="102"/>
       <c r="BQ2" s="3"/>
-      <c r="BR2" s="93"/>
+      <c r="BR2" s="3"/>
+      <c r="BS2" s="99"/>
     </row>
-    <row r="3" spans="1:70" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86"/>
-      <c r="B3" s="89"/>
+    <row r="3" spans="1:71" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="92"/>
+      <c r="B3" s="95"/>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="97">
+      <c r="D3" s="103">
         <v>1</v>
       </c>
-      <c r="E3" s="98"/>
-      <c r="F3" s="99">
+      <c r="E3" s="88"/>
+      <c r="F3" s="87">
         <v>2</v>
       </c>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99">
+      <c r="G3" s="88"/>
+      <c r="H3" s="87">
         <v>3</v>
       </c>
-      <c r="I3" s="98"/>
-      <c r="J3" s="99">
+      <c r="I3" s="88"/>
+      <c r="J3" s="87">
         <v>4</v>
       </c>
-      <c r="K3" s="98"/>
-      <c r="L3" s="99">
+      <c r="K3" s="88"/>
+      <c r="L3" s="87">
         <v>5</v>
       </c>
-      <c r="M3" s="98"/>
-      <c r="N3" s="99">
+      <c r="M3" s="88"/>
+      <c r="N3" s="87">
         <v>6</v>
       </c>
-      <c r="O3" s="98"/>
-      <c r="P3" s="99">
+      <c r="O3" s="88"/>
+      <c r="P3" s="87">
         <v>7</v>
       </c>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="99">
+      <c r="Q3" s="88"/>
+      <c r="R3" s="87">
         <v>8</v>
       </c>
-      <c r="S3" s="98"/>
-      <c r="T3" s="99">
+      <c r="S3" s="88"/>
+      <c r="T3" s="87">
         <v>9</v>
       </c>
-      <c r="U3" s="98"/>
-      <c r="V3" s="99">
+      <c r="U3" s="88"/>
+      <c r="V3" s="87">
         <v>10</v>
       </c>
-      <c r="W3" s="98"/>
-      <c r="X3" s="99">
+      <c r="W3" s="88"/>
+      <c r="X3" s="87">
         <v>11</v>
       </c>
-      <c r="Y3" s="98"/>
-      <c r="Z3" s="99">
+      <c r="Y3" s="88"/>
+      <c r="Z3" s="87">
         <v>12</v>
       </c>
-      <c r="AA3" s="98"/>
-      <c r="AB3" s="99">
+      <c r="AA3" s="88"/>
+      <c r="AB3" s="87">
         <v>13</v>
       </c>
-      <c r="AC3" s="98"/>
-      <c r="AD3" s="99">
+      <c r="AC3" s="88"/>
+      <c r="AD3" s="87">
         <v>14</v>
       </c>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="99">
+      <c r="AE3" s="88"/>
+      <c r="AF3" s="87">
         <v>15</v>
       </c>
-      <c r="AG3" s="98"/>
-      <c r="AH3" s="99">
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="87">
         <v>16</v>
       </c>
-      <c r="AI3" s="98"/>
-      <c r="AJ3" s="99">
+      <c r="AI3" s="88"/>
+      <c r="AJ3" s="87">
         <v>17</v>
       </c>
-      <c r="AK3" s="100"/>
-      <c r="AL3" s="100"/>
-      <c r="AM3" s="100"/>
-      <c r="AN3" s="98"/>
-      <c r="AO3" s="76"/>
-      <c r="AP3" s="99">
+      <c r="AK3" s="104"/>
+      <c r="AL3" s="104"/>
+      <c r="AM3" s="104"/>
+      <c r="AN3" s="88"/>
+      <c r="AO3" s="87">
         <v>18</v>
       </c>
-      <c r="AQ3" s="100"/>
-      <c r="AR3" s="100"/>
-      <c r="AS3" s="100"/>
-      <c r="AT3" s="98"/>
-      <c r="AU3" s="77"/>
-      <c r="AV3" s="99">
+      <c r="AP3" s="104"/>
+      <c r="AQ3" s="104"/>
+      <c r="AR3" s="104"/>
+      <c r="AS3" s="104"/>
+      <c r="AT3" s="88"/>
+      <c r="AU3" s="87">
         <v>19</v>
       </c>
+      <c r="AV3" s="104"/>
       <c r="AW3" s="104"/>
-      <c r="AX3" s="100"/>
+      <c r="AX3" s="104"/>
       <c r="AY3" s="104"/>
-      <c r="AZ3" s="105"/>
+      <c r="AZ3" s="88"/>
       <c r="BA3" s="106">
         <v>20</v>
       </c>
-      <c r="BB3" s="104"/>
-      <c r="BC3" s="104"/>
-      <c r="BD3" s="104"/>
-      <c r="BE3" s="105"/>
+      <c r="BB3" s="107"/>
+      <c r="BC3" s="107"/>
+      <c r="BD3" s="107"/>
+      <c r="BE3" s="108"/>
       <c r="BF3" s="106">
         <v>21</v>
       </c>
-      <c r="BG3" s="104"/>
-      <c r="BH3" s="104"/>
-      <c r="BI3" s="104"/>
-      <c r="BJ3" s="105"/>
-      <c r="BK3" s="106">
+      <c r="BG3" s="107"/>
+      <c r="BH3" s="107"/>
+      <c r="BI3" s="107"/>
+      <c r="BJ3" s="108"/>
+      <c r="BK3" s="87">
         <v>22</v>
       </c>
       <c r="BL3" s="104"/>
       <c r="BM3" s="104"/>
       <c r="BN3" s="104"/>
-      <c r="BO3" s="100"/>
-      <c r="BP3" s="4" t="s">
+      <c r="BO3" s="104"/>
+      <c r="BP3" s="105"/>
+      <c r="BQ3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="BQ3" s="4" t="s">
+      <c r="BR3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="BR3" s="94"/>
+      <c r="BS3" s="100"/>
     </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" s="8">
         <f>SUM(C7:C13)</f>
@@ -1976,14 +2009,15 @@
       <c r="BH4" s="62"/>
       <c r="BI4" s="60"/>
       <c r="BJ4" s="61"/>
-      <c r="BK4" s="62"/>
-      <c r="BL4" s="60"/>
-      <c r="BM4" s="62"/>
-      <c r="BN4" s="60"/>
-      <c r="BO4" s="46"/>
-      <c r="BR4" s="10"/>
+      <c r="BK4" s="61"/>
+      <c r="BL4" s="62"/>
+      <c r="BM4" s="60"/>
+      <c r="BN4" s="62"/>
+      <c r="BO4" s="60"/>
+      <c r="BP4" s="46"/>
+      <c r="BS4" s="10"/>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="D5" s="34"/>
       <c r="E5" s="35"/>
@@ -2044,19 +2078,20 @@
       <c r="BH5" s="46"/>
       <c r="BI5" s="45"/>
       <c r="BJ5" s="33"/>
-      <c r="BK5" s="46"/>
-      <c r="BL5" s="45"/>
-      <c r="BM5" s="46"/>
-      <c r="BN5" s="45"/>
-      <c r="BO5" s="46"/>
-      <c r="BR5" s="10"/>
+      <c r="BK5" s="33"/>
+      <c r="BL5" s="46"/>
+      <c r="BM5" s="45"/>
+      <c r="BN5" s="46"/>
+      <c r="BO5" s="45"/>
+      <c r="BP5" s="46"/>
+      <c r="BS5" s="10"/>
     </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="35"/>
@@ -2117,25 +2152,26 @@
       <c r="BH6" s="44"/>
       <c r="BI6" s="45"/>
       <c r="BJ6" s="33"/>
-      <c r="BK6" s="44"/>
-      <c r="BL6" s="45"/>
-      <c r="BM6" s="44"/>
-      <c r="BN6" s="45"/>
-      <c r="BO6" s="44"/>
-      <c r="BR6" s="10"/>
+      <c r="BK6" s="33"/>
+      <c r="BL6" s="44"/>
+      <c r="BM6" s="45"/>
+      <c r="BN6" s="44"/>
+      <c r="BO6" s="45"/>
+      <c r="BP6" s="44"/>
+      <c r="BS6" s="10"/>
     </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="C7" s="8">
         <v>8</v>
       </c>
       <c r="D7" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="38"/>
@@ -2197,29 +2233,30 @@
       <c r="BH7" s="46"/>
       <c r="BI7" s="45"/>
       <c r="BJ7" s="33"/>
-      <c r="BK7" s="46"/>
-      <c r="BL7" s="45"/>
-      <c r="BM7" s="46"/>
-      <c r="BN7" s="45"/>
-      <c r="BO7" s="46"/>
-      <c r="BP7" s="8">
-        <f>SUM(D7:BO7)</f>
-        <v>7</v>
-      </c>
+      <c r="BK7" s="33"/>
+      <c r="BL7" s="46"/>
+      <c r="BM7" s="45"/>
+      <c r="BN7" s="46"/>
+      <c r="BO7" s="45"/>
+      <c r="BP7" s="46"/>
       <c r="BQ7" s="8">
+        <f>SUM(D7:BP7)</f>
+        <v>9</v>
+      </c>
+      <c r="BR7" s="8">
         <v>0</v>
       </c>
-      <c r="BR7" s="10">
-        <f>C7-BP7-BQ7</f>
-        <v>1</v>
+      <c r="BS7" s="10">
+        <f>C7-BQ7-BR7</f>
+        <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C8" s="8">
         <v>8</v>
@@ -2291,24 +2328,25 @@
       <c r="BH8" s="46"/>
       <c r="BI8" s="45"/>
       <c r="BJ8" s="33"/>
-      <c r="BK8" s="46"/>
-      <c r="BL8" s="45"/>
-      <c r="BM8" s="46"/>
-      <c r="BN8" s="45"/>
-      <c r="BO8" s="46"/>
-      <c r="BP8" s="8">
-        <f>SUM(D8:BO8)</f>
+      <c r="BK8" s="33"/>
+      <c r="BL8" s="46"/>
+      <c r="BM8" s="45"/>
+      <c r="BN8" s="46"/>
+      <c r="BO8" s="45"/>
+      <c r="BP8" s="46"/>
+      <c r="BQ8" s="8">
+        <f>SUM(D8:BP8)</f>
         <v>7</v>
       </c>
-      <c r="BQ8" s="8">
+      <c r="BR8" s="8">
         <v>0</v>
       </c>
-      <c r="BR8" s="10">
-        <f>C8-BP8-BQ8</f>
+      <c r="BS8" s="10">
+        <f>C8-BQ8-BR8</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="15"/>
       <c r="D9" s="34"/>
@@ -2370,19 +2408,20 @@
       <c r="BH9" s="46"/>
       <c r="BI9" s="45"/>
       <c r="BJ9" s="33"/>
-      <c r="BK9" s="46"/>
-      <c r="BL9" s="45"/>
-      <c r="BM9" s="46"/>
-      <c r="BN9" s="45"/>
-      <c r="BO9" s="46"/>
-      <c r="BR9" s="10"/>
+      <c r="BK9" s="33"/>
+      <c r="BL9" s="46"/>
+      <c r="BM9" s="45"/>
+      <c r="BN9" s="46"/>
+      <c r="BO9" s="45"/>
+      <c r="BP9" s="46"/>
+      <c r="BS9" s="10"/>
     </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="35"/>
@@ -2443,14 +2482,15 @@
       <c r="BH10" s="46"/>
       <c r="BI10" s="45"/>
       <c r="BJ10" s="33"/>
-      <c r="BK10" s="46"/>
-      <c r="BL10" s="45"/>
-      <c r="BM10" s="46"/>
-      <c r="BN10" s="45"/>
-      <c r="BO10" s="46"/>
-      <c r="BR10" s="10"/>
+      <c r="BK10" s="33"/>
+      <c r="BL10" s="46"/>
+      <c r="BM10" s="45"/>
+      <c r="BN10" s="46"/>
+      <c r="BO10" s="45"/>
+      <c r="BP10" s="46"/>
+      <c r="BS10" s="10"/>
     </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -2529,24 +2569,25 @@
       <c r="BH11" s="46"/>
       <c r="BI11" s="45"/>
       <c r="BJ11" s="33"/>
-      <c r="BK11" s="46"/>
-      <c r="BL11" s="45"/>
-      <c r="BM11" s="46"/>
-      <c r="BN11" s="45"/>
-      <c r="BO11" s="46"/>
-      <c r="BP11" s="8">
-        <f>SUM(D11:BO11)</f>
+      <c r="BK11" s="33"/>
+      <c r="BL11" s="46"/>
+      <c r="BM11" s="45"/>
+      <c r="BN11" s="46"/>
+      <c r="BO11" s="45"/>
+      <c r="BP11" s="46"/>
+      <c r="BQ11" s="8">
+        <f>SUM(D11:BP11)</f>
         <v>21</v>
       </c>
-      <c r="BQ11" s="8">
+      <c r="BR11" s="8">
         <v>0</v>
       </c>
-      <c r="BR11" s="10">
-        <f>C11-BP11-BQ11</f>
+      <c r="BS11" s="10">
+        <f>C11-BQ11-BR11</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -2617,24 +2658,25 @@
       <c r="BH12" s="46"/>
       <c r="BI12" s="45"/>
       <c r="BJ12" s="33"/>
-      <c r="BK12" s="46"/>
-      <c r="BL12" s="45"/>
-      <c r="BM12" s="46"/>
-      <c r="BN12" s="45"/>
-      <c r="BO12" s="46"/>
-      <c r="BP12" s="8">
-        <f>SUM(D12:BO12)</f>
+      <c r="BK12" s="33"/>
+      <c r="BL12" s="46"/>
+      <c r="BM12" s="45"/>
+      <c r="BN12" s="46"/>
+      <c r="BO12" s="45"/>
+      <c r="BP12" s="46"/>
+      <c r="BQ12" s="8">
+        <f>SUM(D12:BP12)</f>
         <v>4</v>
       </c>
-      <c r="BQ12" s="8">
+      <c r="BR12" s="8">
         <v>0</v>
       </c>
-      <c r="BR12" s="10">
-        <f>C12-BP12-BQ12</f>
+      <c r="BS12" s="10">
+        <f>C12-BQ12-BR12</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="D13" s="34"/>
       <c r="E13" s="35"/>
@@ -2695,19 +2737,20 @@
       <c r="BH13" s="46"/>
       <c r="BI13" s="45"/>
       <c r="BJ13" s="33"/>
-      <c r="BK13" s="46"/>
-      <c r="BL13" s="45"/>
-      <c r="BM13" s="46"/>
-      <c r="BN13" s="45"/>
-      <c r="BO13" s="46"/>
-      <c r="BR13" s="10"/>
+      <c r="BK13" s="33"/>
+      <c r="BL13" s="46"/>
+      <c r="BM13" s="45"/>
+      <c r="BN13" s="46"/>
+      <c r="BO13" s="45"/>
+      <c r="BP13" s="46"/>
+      <c r="BS13" s="10"/>
     </row>
-    <row r="14" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C14" s="12">
         <f>SUM(C15:C33)</f>
@@ -2772,21 +2815,22 @@
       <c r="BH14" s="67"/>
       <c r="BI14" s="69"/>
       <c r="BJ14" s="66"/>
-      <c r="BK14" s="67"/>
-      <c r="BL14" s="69"/>
-      <c r="BM14" s="67"/>
-      <c r="BN14" s="69"/>
-      <c r="BO14" s="67"/>
-      <c r="BP14" s="12"/>
+      <c r="BK14" s="66"/>
+      <c r="BL14" s="67"/>
+      <c r="BM14" s="69"/>
+      <c r="BN14" s="67"/>
+      <c r="BO14" s="69"/>
+      <c r="BP14" s="67"/>
       <c r="BQ14" s="12"/>
-      <c r="BR14" s="13"/>
+      <c r="BR14" s="12"/>
+      <c r="BS14" s="13"/>
     </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="35"/>
@@ -2847,19 +2891,20 @@
       <c r="BH15" s="46"/>
       <c r="BI15" s="45"/>
       <c r="BJ15" s="33"/>
-      <c r="BK15" s="46"/>
-      <c r="BL15" s="45"/>
-      <c r="BM15" s="46"/>
-      <c r="BN15" s="45"/>
-      <c r="BO15" s="46"/>
-      <c r="BR15" s="10"/>
+      <c r="BK15" s="33"/>
+      <c r="BL15" s="46"/>
+      <c r="BM15" s="45"/>
+      <c r="BN15" s="46"/>
+      <c r="BO15" s="45"/>
+      <c r="BP15" s="46"/>
+      <c r="BS15" s="10"/>
     </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="C16" s="8">
         <v>20</v>
@@ -2875,7 +2920,7 @@
       <c r="L16" s="32"/>
       <c r="M16" s="33"/>
       <c r="N16" s="38">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O16" s="39">
         <v>4</v>
@@ -2884,7 +2929,7 @@
         <v>7</v>
       </c>
       <c r="Q16" s="39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="33"/>
@@ -2931,30 +2976,31 @@
       <c r="BH16" s="46"/>
       <c r="BI16" s="45"/>
       <c r="BJ16" s="33"/>
-      <c r="BK16" s="46"/>
-      <c r="BL16" s="45"/>
-      <c r="BM16" s="46"/>
-      <c r="BN16" s="45"/>
-      <c r="BO16" s="46"/>
-      <c r="BP16" s="8">
-        <f>SUM(D16:BO16)</f>
-        <v>20</v>
-      </c>
+      <c r="BK16" s="33"/>
+      <c r="BL16" s="46"/>
+      <c r="BM16" s="45"/>
+      <c r="BN16" s="46"/>
+      <c r="BO16" s="45"/>
+      <c r="BP16" s="46"/>
       <c r="BQ16" s="8">
-        <f>C16-BP16</f>
+        <f>SUM(D16:BP16)</f>
+        <v>23</v>
+      </c>
+      <c r="BR16" s="8">
+        <f>C16-BQ16</f>
+        <v>-3</v>
+      </c>
+      <c r="BS16" s="10">
+        <f>C16-BQ16-BR16</f>
         <v>0</v>
       </c>
-      <c r="BR16" s="10">
-        <f>C16-BP16-BQ16</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="C17" s="8">
         <v>4</v>
@@ -3022,24 +3068,25 @@
       <c r="BH17" s="46"/>
       <c r="BI17" s="45"/>
       <c r="BJ17" s="33"/>
-      <c r="BK17" s="46"/>
-      <c r="BL17" s="45"/>
-      <c r="BM17" s="46"/>
-      <c r="BN17" s="45"/>
-      <c r="BO17" s="46"/>
-      <c r="BP17" s="8">
-        <f>SUM(D17:BO17)</f>
+      <c r="BK17" s="33"/>
+      <c r="BL17" s="46"/>
+      <c r="BM17" s="45"/>
+      <c r="BN17" s="46"/>
+      <c r="BO17" s="45"/>
+      <c r="BP17" s="46"/>
+      <c r="BQ17" s="8">
+        <f>SUM(D17:BP17)</f>
         <v>2</v>
       </c>
-      <c r="BQ17" s="8">
+      <c r="BR17" s="8">
         <v>0</v>
       </c>
-      <c r="BR17" s="10">
-        <f>C17-BP17-BQ17</f>
+      <c r="BS17" s="10">
+        <f>C17-BQ17-BR17</f>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="16"/>
       <c r="D18" s="34"/>
@@ -3101,19 +3148,20 @@
       <c r="BH18" s="46"/>
       <c r="BI18" s="45"/>
       <c r="BJ18" s="33"/>
-      <c r="BK18" s="46"/>
-      <c r="BL18" s="45"/>
-      <c r="BM18" s="46"/>
-      <c r="BN18" s="45"/>
-      <c r="BO18" s="46"/>
-      <c r="BR18" s="10"/>
+      <c r="BK18" s="33"/>
+      <c r="BL18" s="46"/>
+      <c r="BM18" s="45"/>
+      <c r="BN18" s="46"/>
+      <c r="BO18" s="45"/>
+      <c r="BP18" s="46"/>
+      <c r="BS18" s="10"/>
     </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C19" s="8">
         <v>8</v>
@@ -3133,7 +3181,7 @@
       <c r="P19" s="59"/>
       <c r="Q19" s="33"/>
       <c r="R19" s="59">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S19" s="39"/>
       <c r="T19" s="38"/>
@@ -3179,24 +3227,25 @@
       <c r="BH19" s="44"/>
       <c r="BI19" s="45"/>
       <c r="BJ19" s="33"/>
-      <c r="BK19" s="44"/>
-      <c r="BL19" s="45"/>
-      <c r="BM19" s="44"/>
-      <c r="BN19" s="45"/>
-      <c r="BO19" s="44"/>
-      <c r="BP19" s="8">
-        <f>SUM(D19:BO19)</f>
-        <v>4</v>
-      </c>
+      <c r="BK19" s="33"/>
+      <c r="BL19" s="44"/>
+      <c r="BM19" s="45"/>
+      <c r="BN19" s="44"/>
+      <c r="BO19" s="45"/>
+      <c r="BP19" s="44"/>
       <c r="BQ19" s="8">
+        <f>SUM(D19:BP19)</f>
+        <v>7</v>
+      </c>
+      <c r="BR19" s="8">
         <v>0</v>
       </c>
-      <c r="BR19" s="10">
-        <f>C19-BP19-BQ19</f>
-        <v>4</v>
+      <c r="BS19" s="10">
+        <f>C19-BQ19-BR19</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="16"/>
       <c r="D20" s="34"/>
@@ -3258,19 +3307,20 @@
       <c r="BH20" s="46"/>
       <c r="BI20" s="45"/>
       <c r="BJ20" s="33"/>
-      <c r="BK20" s="46"/>
-      <c r="BL20" s="45"/>
-      <c r="BM20" s="46"/>
-      <c r="BN20" s="45"/>
-      <c r="BO20" s="46"/>
-      <c r="BR20" s="10"/>
+      <c r="BK20" s="33"/>
+      <c r="BL20" s="46"/>
+      <c r="BM20" s="45"/>
+      <c r="BN20" s="46"/>
+      <c r="BO20" s="45"/>
+      <c r="BP20" s="46"/>
+      <c r="BS20" s="10"/>
     </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="C21" s="8">
         <v>4</v>
@@ -3334,24 +3384,25 @@
       <c r="BH21" s="46"/>
       <c r="BI21" s="45"/>
       <c r="BJ21" s="33"/>
-      <c r="BK21" s="46"/>
-      <c r="BL21" s="45"/>
-      <c r="BM21" s="46"/>
-      <c r="BN21" s="45"/>
-      <c r="BO21" s="46"/>
-      <c r="BP21" s="8">
-        <f>SUM(D21:BO21)</f>
+      <c r="BK21" s="33"/>
+      <c r="BL21" s="46"/>
+      <c r="BM21" s="45"/>
+      <c r="BN21" s="46"/>
+      <c r="BO21" s="45"/>
+      <c r="BP21" s="46"/>
+      <c r="BQ21" s="8">
+        <f>SUM(D21:BP21)</f>
         <v>0</v>
       </c>
-      <c r="BQ21" s="8">
+      <c r="BR21" s="8">
         <v>0</v>
       </c>
-      <c r="BR21" s="10">
-        <f>C21-BP21-BQ21</f>
+      <c r="BS21" s="10">
+        <f>C21-BQ21-BR21</f>
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="16"/>
       <c r="D22" s="34"/>
@@ -3413,19 +3464,20 @@
       <c r="BH22" s="46"/>
       <c r="BI22" s="45"/>
       <c r="BJ22" s="33"/>
-      <c r="BK22" s="46"/>
-      <c r="BL22" s="45"/>
-      <c r="BM22" s="46"/>
-      <c r="BN22" s="45"/>
-      <c r="BO22" s="46"/>
-      <c r="BR22" s="10"/>
+      <c r="BK22" s="33"/>
+      <c r="BL22" s="46"/>
+      <c r="BM22" s="45"/>
+      <c r="BN22" s="46"/>
+      <c r="BO22" s="45"/>
+      <c r="BP22" s="46"/>
+      <c r="BS22" s="10"/>
     </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="35"/>
@@ -3486,19 +3538,20 @@
       <c r="BH23" s="46"/>
       <c r="BI23" s="45"/>
       <c r="BJ23" s="33"/>
-      <c r="BK23" s="46"/>
-      <c r="BL23" s="45"/>
-      <c r="BM23" s="46"/>
-      <c r="BN23" s="45"/>
-      <c r="BO23" s="46"/>
-      <c r="BR23" s="10"/>
+      <c r="BK23" s="33"/>
+      <c r="BL23" s="46"/>
+      <c r="BM23" s="45"/>
+      <c r="BN23" s="46"/>
+      <c r="BO23" s="45"/>
+      <c r="BP23" s="46"/>
+      <c r="BS23" s="10"/>
     </row>
-    <row r="24" spans="1:70" s="52" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:71" s="52" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C24" s="28">
         <v>4</v>
@@ -3566,29 +3619,30 @@
       <c r="BH24" s="72"/>
       <c r="BI24" s="45"/>
       <c r="BJ24" s="44"/>
-      <c r="BK24" s="59"/>
-      <c r="BL24" s="44"/>
-      <c r="BM24" s="45"/>
+      <c r="BK24" s="75"/>
+      <c r="BL24" s="32"/>
+      <c r="BM24" s="44"/>
       <c r="BN24" s="45"/>
-      <c r="BO24" s="44"/>
-      <c r="BP24" s="8">
-        <f>SUM(D24:BO24)</f>
+      <c r="BO24" s="45"/>
+      <c r="BP24" s="44"/>
+      <c r="BQ24" s="8">
+        <f>SUM(D24:BP24)</f>
         <v>3</v>
       </c>
-      <c r="BQ24" s="8">
+      <c r="BR24" s="8">
         <v>0</v>
       </c>
-      <c r="BR24" s="10">
-        <f>C24-BP24-BQ24</f>
+      <c r="BS24" s="10">
+        <f>C24-BQ24-BR24</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C25" s="28">
         <v>12</v>
@@ -3610,7 +3664,7 @@
       <c r="R25" s="59"/>
       <c r="S25" s="33"/>
       <c r="T25" s="59">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U25" s="33">
         <v>3</v>
@@ -3658,24 +3712,25 @@
       <c r="BH25" s="46"/>
       <c r="BI25" s="45"/>
       <c r="BJ25" s="33"/>
-      <c r="BK25" s="46"/>
-      <c r="BL25" s="45"/>
-      <c r="BM25" s="46"/>
-      <c r="BN25" s="45"/>
-      <c r="BO25" s="46"/>
-      <c r="BP25" s="8">
-        <f>SUM(D25:BO25)</f>
-        <v>13</v>
-      </c>
+      <c r="BK25" s="33"/>
+      <c r="BL25" s="46"/>
+      <c r="BM25" s="45"/>
+      <c r="BN25" s="46"/>
+      <c r="BO25" s="45"/>
+      <c r="BP25" s="46"/>
       <c r="BQ25" s="8">
+        <f>SUM(D25:BP25)</f>
+        <v>16</v>
+      </c>
+      <c r="BR25" s="8">
         <v>0</v>
       </c>
-      <c r="BR25" s="10">
-        <f>C25-BP25-BQ25</f>
-        <v>-1</v>
+      <c r="BS25" s="10">
+        <f>C25-BQ25-BR25</f>
+        <v>-4</v>
       </c>
     </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="29"/>
       <c r="D26" s="34"/>
@@ -3737,19 +3792,20 @@
       <c r="BH26" s="44"/>
       <c r="BI26" s="45"/>
       <c r="BJ26" s="33"/>
-      <c r="BK26" s="44"/>
-      <c r="BL26" s="45"/>
-      <c r="BM26" s="44"/>
-      <c r="BN26" s="45"/>
-      <c r="BO26" s="44"/>
-      <c r="BR26" s="10"/>
+      <c r="BK26" s="33"/>
+      <c r="BL26" s="44"/>
+      <c r="BM26" s="45"/>
+      <c r="BN26" s="44"/>
+      <c r="BO26" s="45"/>
+      <c r="BP26" s="44"/>
+      <c r="BS26" s="10"/>
     </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="35"/>
@@ -3810,19 +3866,20 @@
       <c r="BH27" s="46"/>
       <c r="BI27" s="45"/>
       <c r="BJ27" s="33"/>
-      <c r="BK27" s="46"/>
-      <c r="BL27" s="45"/>
-      <c r="BM27" s="46"/>
-      <c r="BN27" s="45"/>
-      <c r="BO27" s="46"/>
-      <c r="BR27" s="10"/>
+      <c r="BK27" s="33"/>
+      <c r="BL27" s="46"/>
+      <c r="BM27" s="45"/>
+      <c r="BN27" s="46"/>
+      <c r="BO27" s="45"/>
+      <c r="BP27" s="46"/>
+      <c r="BS27" s="10"/>
     </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="C28" s="8">
         <v>4</v>
@@ -3888,29 +3945,30 @@
       <c r="BH28" s="46"/>
       <c r="BI28" s="45"/>
       <c r="BJ28" s="33"/>
-      <c r="BK28" s="46"/>
-      <c r="BL28" s="45"/>
-      <c r="BM28" s="46"/>
-      <c r="BN28" s="45"/>
-      <c r="BO28" s="46"/>
-      <c r="BP28" s="8">
-        <f>SUM(D28:BO28)</f>
+      <c r="BK28" s="33"/>
+      <c r="BL28" s="46"/>
+      <c r="BM28" s="45"/>
+      <c r="BN28" s="46"/>
+      <c r="BO28" s="45"/>
+      <c r="BP28" s="46"/>
+      <c r="BQ28" s="8">
+        <f>SUM(D28:BP28)</f>
         <v>1</v>
       </c>
-      <c r="BQ28" s="8">
+      <c r="BR28" s="8">
         <v>0</v>
       </c>
-      <c r="BR28" s="10">
-        <f>C28-BP28-BQ28</f>
+      <c r="BS28" s="10">
+        <f>C28-BQ28-BR28</f>
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C29" s="8">
         <v>10</v>
@@ -3978,24 +4036,25 @@
       <c r="BH29" s="46"/>
       <c r="BI29" s="45"/>
       <c r="BJ29" s="33"/>
-      <c r="BK29" s="46"/>
-      <c r="BL29" s="45"/>
-      <c r="BM29" s="46"/>
-      <c r="BN29" s="45"/>
-      <c r="BO29" s="46"/>
-      <c r="BP29" s="8">
-        <f>SUM(D29:BO29)</f>
+      <c r="BK29" s="33"/>
+      <c r="BL29" s="46"/>
+      <c r="BM29" s="45"/>
+      <c r="BN29" s="46"/>
+      <c r="BO29" s="45"/>
+      <c r="BP29" s="46"/>
+      <c r="BQ29" s="8">
+        <f>SUM(D29:BP29)</f>
         <v>12</v>
       </c>
-      <c r="BQ29" s="8">
+      <c r="BR29" s="8">
         <v>0</v>
       </c>
-      <c r="BR29" s="10">
-        <f>C29-BP29-BQ29</f>
+      <c r="BS29" s="10">
+        <f>C29-BQ29-BR29</f>
         <v>-2</v>
       </c>
     </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="15"/>
       <c r="D30" s="34"/>
@@ -4057,19 +4116,20 @@
       <c r="BH30" s="46"/>
       <c r="BI30" s="45"/>
       <c r="BJ30" s="33"/>
-      <c r="BK30" s="46"/>
-      <c r="BL30" s="45"/>
-      <c r="BM30" s="46"/>
-      <c r="BN30" s="45"/>
-      <c r="BO30" s="46"/>
-      <c r="BR30" s="10"/>
+      <c r="BK30" s="33"/>
+      <c r="BL30" s="46"/>
+      <c r="BM30" s="45"/>
+      <c r="BN30" s="46"/>
+      <c r="BO30" s="45"/>
+      <c r="BP30" s="46"/>
+      <c r="BS30" s="10"/>
     </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D31" s="34"/>
       <c r="E31" s="35"/>
@@ -4130,20 +4190,21 @@
       <c r="BH31" s="44"/>
       <c r="BI31" s="45"/>
       <c r="BJ31" s="33"/>
-      <c r="BK31" s="44"/>
-      <c r="BL31" s="45"/>
-      <c r="BM31" s="44"/>
-      <c r="BN31" s="45"/>
-      <c r="BO31" s="44"/>
-      <c r="BP31" s="28"/>
-      <c r="BR31" s="10"/>
+      <c r="BK31" s="33"/>
+      <c r="BL31" s="44"/>
+      <c r="BM31" s="45"/>
+      <c r="BN31" s="44"/>
+      <c r="BO31" s="45"/>
+      <c r="BP31" s="44"/>
+      <c r="BQ31" s="28"/>
+      <c r="BS31" s="10"/>
     </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="C32" s="8">
         <v>10</v>
@@ -4209,24 +4270,25 @@
       <c r="BH32" s="46"/>
       <c r="BI32" s="45"/>
       <c r="BJ32" s="33"/>
-      <c r="BK32" s="46"/>
-      <c r="BL32" s="45"/>
-      <c r="BM32" s="46"/>
-      <c r="BN32" s="45"/>
-      <c r="BO32" s="46"/>
-      <c r="BP32" s="8">
-        <f>SUM(D32:BO32)</f>
+      <c r="BK32" s="33"/>
+      <c r="BL32" s="46"/>
+      <c r="BM32" s="45"/>
+      <c r="BN32" s="46"/>
+      <c r="BO32" s="45"/>
+      <c r="BP32" s="46"/>
+      <c r="BQ32" s="8">
+        <f>SUM(D32:BP32)</f>
         <v>1</v>
       </c>
-      <c r="BQ32" s="8">
+      <c r="BR32" s="8">
         <v>0</v>
       </c>
-      <c r="BR32" s="10">
-        <f>C32-BP32-BQ32</f>
+      <c r="BS32" s="10">
+        <f>C32-BQ32-BR32</f>
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="29"/>
       <c r="D33" s="34"/>
@@ -4288,20 +4350,21 @@
       <c r="BH33" s="46"/>
       <c r="BI33" s="45"/>
       <c r="BJ33" s="33"/>
-      <c r="BK33" s="46"/>
-      <c r="BL33" s="45"/>
-      <c r="BM33" s="46"/>
-      <c r="BN33" s="45"/>
-      <c r="BO33" s="46"/>
-      <c r="BP33" s="28"/>
-      <c r="BR33" s="10"/>
+      <c r="BK33" s="33"/>
+      <c r="BL33" s="46"/>
+      <c r="BM33" s="45"/>
+      <c r="BN33" s="46"/>
+      <c r="BO33" s="45"/>
+      <c r="BP33" s="46"/>
+      <c r="BQ33" s="28"/>
+      <c r="BS33" s="10"/>
     </row>
-    <row r="34" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="55" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="56" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C34" s="17">
         <f>SUM(C39:C59)</f>
@@ -4366,21 +4429,22 @@
       <c r="BH34" s="67"/>
       <c r="BI34" s="69"/>
       <c r="BJ34" s="66"/>
-      <c r="BK34" s="67"/>
-      <c r="BL34" s="69"/>
-      <c r="BM34" s="67"/>
-      <c r="BN34" s="69"/>
-      <c r="BO34" s="67"/>
-      <c r="BP34" s="17"/>
-      <c r="BQ34" s="12"/>
-      <c r="BR34" s="13"/>
+      <c r="BK34" s="66"/>
+      <c r="BL34" s="67"/>
+      <c r="BM34" s="69"/>
+      <c r="BN34" s="67"/>
+      <c r="BO34" s="69"/>
+      <c r="BP34" s="67"/>
+      <c r="BQ34" s="17"/>
+      <c r="BR34" s="12"/>
+      <c r="BS34" s="13"/>
     </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="50" t="s">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="C35" s="8">
         <v>10</v>
@@ -4452,28 +4516,30 @@
       <c r="BH35" s="44"/>
       <c r="BI35" s="45"/>
       <c r="BJ35" s="33"/>
-      <c r="BK35" s="44"/>
-      <c r="BL35" s="45"/>
-      <c r="BM35" s="44"/>
-      <c r="BN35" s="45"/>
-      <c r="BO35" s="44"/>
-      <c r="BP35" s="8">
-        <f>SUM(D35:BO35)</f>
+      <c r="BK35" s="33"/>
+      <c r="BL35" s="44"/>
+      <c r="BM35" s="45"/>
+      <c r="BN35" s="44"/>
+      <c r="BO35" s="45"/>
+      <c r="BP35" s="44"/>
+      <c r="BQ35" s="8">
+        <f>SUM(D35:BP35)</f>
         <v>20</v>
       </c>
-      <c r="BQ35" s="8">
-        <v>20</v>
-      </c>
-      <c r="BR35" s="10">
+      <c r="BR35" s="8">
         <v>0</v>
       </c>
+      <c r="BS35" s="10">
+        <f>C35-BQ35-BR35</f>
+        <v>-10</v>
+      </c>
     </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D36" s="34"/>
       <c r="E36" s="35"/>
@@ -4538,23 +4604,27 @@
       <c r="BH36" s="44"/>
       <c r="BI36" s="45"/>
       <c r="BJ36" s="33"/>
-      <c r="BK36" s="44"/>
-      <c r="BL36" s="45"/>
-      <c r="BM36" s="44"/>
-      <c r="BN36" s="45"/>
-      <c r="BO36" s="44"/>
-      <c r="BP36" s="8">
-        <f>SUM(D36:BO36)</f>
-        <v>9</v>
-      </c>
+      <c r="BK36" s="33"/>
+      <c r="BL36" s="44"/>
+      <c r="BM36" s="45">
+        <v>3</v>
+      </c>
+      <c r="BN36" s="44"/>
+      <c r="BO36" s="45"/>
+      <c r="BP36" s="44"/>
       <c r="BQ36" s="8">
-        <v>20</v>
-      </c>
-      <c r="BR36" s="10">
+        <f>SUM(D36:BP36)</f>
+        <v>12</v>
+      </c>
+      <c r="BR36" s="8">
         <v>0</v>
       </c>
+      <c r="BS36" s="10">
+        <f>C36-BQ36-BR36</f>
+        <v>-12</v>
+      </c>
     </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A37" s="27"/>
       <c r="B37" s="74"/>
       <c r="D37" s="34"/>
@@ -4616,20 +4686,21 @@
       <c r="BH37" s="44"/>
       <c r="BI37" s="45"/>
       <c r="BJ37" s="33"/>
-      <c r="BK37" s="44"/>
-      <c r="BL37" s="45"/>
-      <c r="BM37" s="44"/>
-      <c r="BN37" s="45"/>
-      <c r="BO37" s="44"/>
-      <c r="BP37" s="28"/>
-      <c r="BR37" s="10"/>
+      <c r="BK37" s="33"/>
+      <c r="BL37" s="44"/>
+      <c r="BM37" s="45"/>
+      <c r="BN37" s="44"/>
+      <c r="BO37" s="45"/>
+      <c r="BP37" s="44"/>
+      <c r="BQ37" s="28"/>
+      <c r="BS37" s="10"/>
     </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D38" s="34"/>
       <c r="E38" s="35"/>
@@ -4690,20 +4761,21 @@
       <c r="BH38" s="46"/>
       <c r="BI38" s="45"/>
       <c r="BJ38" s="33"/>
-      <c r="BK38" s="46"/>
-      <c r="BL38" s="45"/>
-      <c r="BM38" s="46"/>
-      <c r="BN38" s="45"/>
-      <c r="BO38" s="46"/>
-      <c r="BP38" s="28"/>
-      <c r="BR38" s="10"/>
+      <c r="BK38" s="33"/>
+      <c r="BL38" s="46"/>
+      <c r="BM38" s="45"/>
+      <c r="BN38" s="46"/>
+      <c r="BO38" s="45"/>
+      <c r="BP38" s="46"/>
+      <c r="BQ38" s="28"/>
+      <c r="BS38" s="10"/>
     </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="C39" s="18">
         <v>20</v>
@@ -4769,30 +4841,30 @@
       <c r="BH39" s="44"/>
       <c r="BI39" s="45"/>
       <c r="BJ39" s="33"/>
-      <c r="BK39" s="44"/>
-      <c r="BL39" s="45"/>
-      <c r="BM39" s="44"/>
-      <c r="BN39" s="45"/>
-      <c r="BO39" s="44"/>
-      <c r="BP39" s="8">
-        <f>SUM(D39:BO39)</f>
+      <c r="BK39" s="33"/>
+      <c r="BL39" s="44"/>
+      <c r="BM39" s="45"/>
+      <c r="BN39" s="44"/>
+      <c r="BO39" s="45"/>
+      <c r="BP39" s="44"/>
+      <c r="BQ39" s="8">
+        <f>SUM(D39:BP39)</f>
         <v>2</v>
       </c>
-      <c r="BQ39" s="8">
-        <f>C39-BP39</f>
+      <c r="BR39" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS39" s="10">
+        <f>C39-BQ39-BR39</f>
         <v>18</v>
       </c>
-      <c r="BR39" s="10">
-        <f>C39-BP39-BQ39</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B40" s="57" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C40" s="8">
         <v>30</v>
@@ -4870,30 +4942,30 @@
       <c r="BH40" s="46"/>
       <c r="BI40" s="45"/>
       <c r="BJ40" s="33"/>
-      <c r="BK40" s="46"/>
-      <c r="BL40" s="45"/>
-      <c r="BM40" s="46"/>
-      <c r="BN40" s="45"/>
-      <c r="BO40" s="46"/>
-      <c r="BP40" s="8">
-        <f>SUM(D40:BO40)</f>
+      <c r="BK40" s="33"/>
+      <c r="BL40" s="46"/>
+      <c r="BM40" s="45"/>
+      <c r="BN40" s="46"/>
+      <c r="BO40" s="45"/>
+      <c r="BP40" s="46"/>
+      <c r="BQ40" s="8">
+        <f>SUM(D40:BP40)</f>
         <v>40</v>
       </c>
-      <c r="BQ40" s="8">
-        <f>C40-BP40</f>
+      <c r="BR40" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS40" s="10">
+        <f>C40-BQ40-BR40</f>
         <v>-10</v>
       </c>
-      <c r="BR40" s="10">
-        <f>C40-BP40-BQ40</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="C41" s="8">
         <v>4</v>
@@ -4961,30 +5033,30 @@
       <c r="BH41" s="46"/>
       <c r="BI41" s="45"/>
       <c r="BJ41" s="33"/>
-      <c r="BK41" s="46"/>
-      <c r="BL41" s="45"/>
-      <c r="BM41" s="46"/>
-      <c r="BN41" s="45"/>
-      <c r="BO41" s="46"/>
-      <c r="BP41" s="8">
-        <f>SUM(D41:BO41)</f>
+      <c r="BK41" s="33"/>
+      <c r="BL41" s="46"/>
+      <c r="BM41" s="45"/>
+      <c r="BN41" s="46"/>
+      <c r="BO41" s="45"/>
+      <c r="BP41" s="46"/>
+      <c r="BQ41" s="8">
+        <f>SUM(D41:BP41)</f>
         <v>1</v>
       </c>
-      <c r="BQ41" s="8">
-        <f>C41-BP41</f>
+      <c r="BR41" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS41" s="10">
+        <f>C41-BQ41-BR41</f>
         <v>3</v>
       </c>
-      <c r="BR41" s="10">
-        <f>C41-BP41-BQ41</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="35"/>
@@ -5049,25 +5121,25 @@
       <c r="BH42" s="46"/>
       <c r="BI42" s="45"/>
       <c r="BJ42" s="33"/>
-      <c r="BK42" s="46"/>
-      <c r="BL42" s="45"/>
-      <c r="BM42" s="46"/>
-      <c r="BN42" s="45"/>
-      <c r="BO42" s="46"/>
-      <c r="BP42" s="8">
-        <f>SUM(D42:BO42)</f>
+      <c r="BK42" s="33"/>
+      <c r="BL42" s="46"/>
+      <c r="BM42" s="45"/>
+      <c r="BN42" s="46"/>
+      <c r="BO42" s="45"/>
+      <c r="BP42" s="46"/>
+      <c r="BQ42" s="8">
+        <f>SUM(D42:BP42)</f>
         <v>6.5</v>
       </c>
-      <c r="BQ42" s="8">
-        <f>C42-BP42</f>
+      <c r="BR42" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS42" s="10">
+        <f>C42-BQ42-BR42</f>
         <v>-6.5</v>
       </c>
-      <c r="BR42" s="10">
-        <f>C42-BP42-BQ42</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="26"/>
       <c r="D43" s="34"/>
@@ -5129,20 +5201,21 @@
       <c r="BH43" s="46"/>
       <c r="BI43" s="45"/>
       <c r="BJ43" s="33"/>
-      <c r="BK43" s="46"/>
-      <c r="BL43" s="45"/>
-      <c r="BM43" s="46"/>
-      <c r="BN43" s="45"/>
-      <c r="BO43" s="46"/>
-      <c r="BP43" s="28"/>
-      <c r="BR43" s="10"/>
+      <c r="BK43" s="33"/>
+      <c r="BL43" s="46"/>
+      <c r="BM43" s="45"/>
+      <c r="BN43" s="46"/>
+      <c r="BO43" s="45"/>
+      <c r="BP43" s="46"/>
+      <c r="BQ43" s="28"/>
+      <c r="BS43" s="10"/>
     </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D44" s="34"/>
       <c r="E44" s="35"/>
@@ -5203,20 +5276,21 @@
       <c r="BH44" s="46"/>
       <c r="BI44" s="45"/>
       <c r="BJ44" s="33"/>
-      <c r="BK44" s="46"/>
-      <c r="BL44" s="45"/>
-      <c r="BM44" s="46"/>
-      <c r="BN44" s="45"/>
-      <c r="BO44" s="46"/>
-      <c r="BP44" s="28"/>
-      <c r="BR44" s="10"/>
+      <c r="BK44" s="33"/>
+      <c r="BL44" s="46"/>
+      <c r="BM44" s="45"/>
+      <c r="BN44" s="46"/>
+      <c r="BO44" s="45"/>
+      <c r="BP44" s="46"/>
+      <c r="BQ44" s="28"/>
+      <c r="BS44" s="10"/>
     </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B45" s="53" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C45" s="8">
         <v>5</v>
@@ -5294,30 +5368,30 @@
       <c r="BH45" s="46"/>
       <c r="BI45" s="45"/>
       <c r="BJ45" s="33"/>
-      <c r="BK45" s="46"/>
-      <c r="BL45" s="45"/>
-      <c r="BM45" s="46"/>
-      <c r="BN45" s="45"/>
-      <c r="BO45" s="46"/>
-      <c r="BP45" s="8">
-        <f>SUM(D45:BO45)</f>
+      <c r="BK45" s="33"/>
+      <c r="BL45" s="46"/>
+      <c r="BM45" s="45"/>
+      <c r="BN45" s="46"/>
+      <c r="BO45" s="45"/>
+      <c r="BP45" s="46"/>
+      <c r="BQ45" s="8">
+        <f>SUM(D45:BP45)</f>
         <v>20</v>
       </c>
-      <c r="BQ45" s="8">
-        <f>C45-BP45</f>
+      <c r="BR45" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS45" s="10">
+        <f>C45-BQ45-BR45</f>
         <v>-15</v>
       </c>
-      <c r="BR45" s="10">
-        <f>C45-BP45-BQ45</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B46" s="53" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="C46" s="8">
         <v>25</v>
@@ -5383,15 +5457,25 @@
       <c r="BH46" s="46"/>
       <c r="BI46" s="45"/>
       <c r="BJ46" s="33"/>
-      <c r="BK46" s="46"/>
-      <c r="BL46" s="45"/>
-      <c r="BM46" s="46"/>
-      <c r="BN46" s="45"/>
-      <c r="BO46" s="46"/>
-      <c r="BP46" s="28"/>
-      <c r="BR46" s="10"/>
+      <c r="BK46" s="33"/>
+      <c r="BL46" s="46"/>
+      <c r="BM46" s="45"/>
+      <c r="BN46" s="46"/>
+      <c r="BO46" s="45"/>
+      <c r="BP46" s="46"/>
+      <c r="BQ46" s="8">
+        <f>SUM(D46:BP46)</f>
+        <v>6</v>
+      </c>
+      <c r="BR46" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS46" s="10">
+        <f>C46-BQ46-BR46</f>
+        <v>19</v>
+      </c>
     </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="16"/>
       <c r="D47" s="34"/>
@@ -5453,20 +5537,21 @@
       <c r="BH47" s="46"/>
       <c r="BI47" s="45"/>
       <c r="BJ47" s="33"/>
-      <c r="BK47" s="46"/>
-      <c r="BL47" s="45"/>
-      <c r="BM47" s="46"/>
-      <c r="BN47" s="45"/>
-      <c r="BO47" s="46"/>
-      <c r="BP47" s="28"/>
-      <c r="BR47" s="10"/>
+      <c r="BK47" s="33"/>
+      <c r="BL47" s="46"/>
+      <c r="BM47" s="45"/>
+      <c r="BN47" s="46"/>
+      <c r="BO47" s="45"/>
+      <c r="BP47" s="46"/>
+      <c r="BQ47" s="28"/>
+      <c r="BS47" s="10"/>
     </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B48" s="58" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D48" s="34"/>
       <c r="E48" s="35"/>
@@ -5527,20 +5612,21 @@
       <c r="BH48" s="46"/>
       <c r="BI48" s="45"/>
       <c r="BJ48" s="33"/>
-      <c r="BK48" s="46"/>
-      <c r="BL48" s="45"/>
-      <c r="BM48" s="46"/>
-      <c r="BN48" s="45"/>
-      <c r="BO48" s="46"/>
-      <c r="BP48" s="28"/>
-      <c r="BR48" s="10"/>
+      <c r="BK48" s="33"/>
+      <c r="BL48" s="46"/>
+      <c r="BM48" s="45"/>
+      <c r="BN48" s="46"/>
+      <c r="BO48" s="45"/>
+      <c r="BP48" s="46"/>
+      <c r="BQ48" s="28"/>
+      <c r="BS48" s="10"/>
     </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B49" s="53" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C49" s="28">
         <v>16</v>
@@ -5584,7 +5670,7 @@
       <c r="AL49" s="32"/>
       <c r="AM49" s="32"/>
       <c r="AN49" s="44"/>
-      <c r="AO49" s="79"/>
+      <c r="AO49" s="75"/>
       <c r="AP49" s="32">
         <v>2</v>
       </c>
@@ -5618,31 +5704,31 @@
       <c r="BH49" s="44"/>
       <c r="BI49" s="45"/>
       <c r="BJ49" s="44"/>
-      <c r="BK49" s="70"/>
-      <c r="BL49" s="45"/>
-      <c r="BM49" s="44"/>
-      <c r="BN49" s="45"/>
-      <c r="BO49" s="73"/>
-      <c r="BP49" s="8">
-        <f t="shared" ref="BP49:BP56" si="0">SUM(D49:BO49)</f>
+      <c r="BK49" s="75"/>
+      <c r="BL49" s="44"/>
+      <c r="BM49" s="45"/>
+      <c r="BN49" s="44"/>
+      <c r="BO49" s="45"/>
+      <c r="BP49" s="73"/>
+      <c r="BQ49" s="8">
+        <f t="shared" ref="BQ49:BQ56" si="0">SUM(D49:BP49)</f>
         <v>30</v>
       </c>
-      <c r="BQ49" s="8">
-        <f t="shared" ref="BQ49:BQ54" si="1">C49-BP49</f>
+      <c r="BR49" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS49" s="10">
+        <f t="shared" ref="BS49:BS54" si="1">C49-BQ49-BR49</f>
         <v>-14</v>
       </c>
-      <c r="BR49" s="10">
-        <f t="shared" ref="BR49:BR54" si="2">C49-BP49-BQ49</f>
-        <v>0</v>
-      </c>
-      <c r="BS49" s="71"/>
+      <c r="BT49" s="71"/>
     </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C50" s="8">
         <v>12</v>
@@ -5713,30 +5799,30 @@
       <c r="BH50" s="46"/>
       <c r="BI50" s="45"/>
       <c r="BJ50" s="33"/>
-      <c r="BK50" s="46"/>
-      <c r="BL50" s="45"/>
-      <c r="BM50" s="46"/>
-      <c r="BN50" s="45"/>
-      <c r="BO50" s="46"/>
-      <c r="BP50" s="8">
+      <c r="BK50" s="33"/>
+      <c r="BL50" s="46"/>
+      <c r="BM50" s="45"/>
+      <c r="BN50" s="46"/>
+      <c r="BO50" s="45"/>
+      <c r="BP50" s="46"/>
+      <c r="BQ50" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="BQ50" s="8">
+      <c r="BR50" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS50" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="BR50" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A51" s="27" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="C51" s="8">
         <v>6</v>
@@ -5806,30 +5892,30 @@
       <c r="BH51" s="46"/>
       <c r="BI51" s="45"/>
       <c r="BJ51" s="33"/>
-      <c r="BK51" s="46"/>
-      <c r="BL51" s="45"/>
-      <c r="BM51" s="46"/>
-      <c r="BN51" s="45"/>
-      <c r="BO51" s="46"/>
-      <c r="BP51" s="8">
+      <c r="BK51" s="33"/>
+      <c r="BL51" s="46"/>
+      <c r="BM51" s="45"/>
+      <c r="BN51" s="46"/>
+      <c r="BO51" s="45"/>
+      <c r="BP51" s="46"/>
+      <c r="BQ51" s="8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="BQ51" s="8">
+      <c r="BR51" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS51" s="10">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="BR51" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="52" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C52" s="8">
         <v>16</v>
@@ -5897,30 +5983,33 @@
       <c r="BH52" s="46"/>
       <c r="BI52" s="45"/>
       <c r="BJ52" s="33"/>
-      <c r="BK52" s="46"/>
-      <c r="BL52" s="45"/>
-      <c r="BM52" s="46"/>
-      <c r="BN52" s="45"/>
-      <c r="BO52" s="46"/>
-      <c r="BP52" s="8">
+      <c r="BK52" s="33"/>
+      <c r="BL52" s="46"/>
+      <c r="BM52" s="45"/>
+      <c r="BN52" s="46"/>
+      <c r="BO52" s="45"/>
+      <c r="BP52" s="46"/>
+      <c r="BQ52" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="BQ52" s="8">
+      <c r="BR52" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS52" s="10">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="BR52" s="10">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="53" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A53" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C53" s="8">
         <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A53" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>94</v>
       </c>
       <c r="D53" s="34"/>
       <c r="E53" s="35"/>
@@ -5989,30 +6078,33 @@
       <c r="BH53" s="46"/>
       <c r="BI53" s="45"/>
       <c r="BJ53" s="33"/>
-      <c r="BK53" s="46"/>
-      <c r="BL53" s="45"/>
-      <c r="BM53" s="46"/>
-      <c r="BN53" s="45"/>
-      <c r="BO53" s="46"/>
-      <c r="BP53" s="8">
+      <c r="BK53" s="33"/>
+      <c r="BL53" s="46"/>
+      <c r="BM53" s="45"/>
+      <c r="BN53" s="46"/>
+      <c r="BO53" s="45"/>
+      <c r="BP53" s="46"/>
+      <c r="BQ53" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="BQ53" s="8">
+      <c r="BR53" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS53" s="10">
         <f t="shared" si="1"/>
         <v>-15</v>
       </c>
-      <c r="BR53" s="10">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="54" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A54" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="8">
         <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A54" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>97</v>
       </c>
       <c r="D54" s="34"/>
       <c r="E54" s="35"/>
@@ -6083,30 +6175,33 @@
       <c r="BH54" s="46"/>
       <c r="BI54" s="45"/>
       <c r="BJ54" s="33"/>
-      <c r="BK54" s="46"/>
-      <c r="BL54" s="45"/>
-      <c r="BM54" s="46"/>
-      <c r="BN54" s="45"/>
-      <c r="BO54" s="46"/>
-      <c r="BP54" s="8">
+      <c r="BK54" s="33"/>
+      <c r="BL54" s="46"/>
+      <c r="BM54" s="45"/>
+      <c r="BN54" s="46"/>
+      <c r="BO54" s="45"/>
+      <c r="BP54" s="46"/>
+      <c r="BQ54" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="BQ54" s="8">
+      <c r="BR54" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS54" s="10">
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
-      <c r="BR54" s="10">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="55" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A55" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="8">
         <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.3">
-      <c r="A55" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>100</v>
       </c>
       <c r="D55" s="34"/>
       <c r="E55" s="35"/>
@@ -6171,23 +6266,35 @@
       <c r="BH55" s="46"/>
       <c r="BI55" s="45"/>
       <c r="BJ55" s="33"/>
-      <c r="BK55" s="46"/>
-      <c r="BL55" s="45"/>
-      <c r="BM55" s="46"/>
-      <c r="BN55" s="45"/>
-      <c r="BO55" s="46"/>
-      <c r="BP55" s="8">
+      <c r="BK55" s="33"/>
+      <c r="BL55" s="46"/>
+      <c r="BM55" s="45"/>
+      <c r="BN55" s="46">
+        <v>6</v>
+      </c>
+      <c r="BO55" s="45"/>
+      <c r="BP55" s="46"/>
+      <c r="BQ55" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="BR55" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="BR55" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS55" s="10">
+        <f>C55-BQ55-BR55</f>
+        <v>-9</v>
+      </c>
     </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>102</v>
+        <v>90</v>
+      </c>
+      <c r="C56" s="8">
+        <v>0</v>
       </c>
       <c r="D56" s="34"/>
       <c r="E56" s="35"/>
@@ -6252,18 +6359,25 @@
       <c r="BH56" s="46"/>
       <c r="BI56" s="45"/>
       <c r="BJ56" s="33"/>
-      <c r="BK56" s="46"/>
-      <c r="BL56" s="45"/>
-      <c r="BM56" s="46"/>
-      <c r="BN56" s="45"/>
-      <c r="BO56" s="46"/>
-      <c r="BP56" s="8">
+      <c r="BK56" s="33"/>
+      <c r="BL56" s="46"/>
+      <c r="BM56" s="45"/>
+      <c r="BN56" s="46"/>
+      <c r="BO56" s="45"/>
+      <c r="BP56" s="46"/>
+      <c r="BQ56" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="BR56" s="10"/>
+      <c r="BR56" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS56" s="10">
+        <f t="shared" ref="BS56" si="2">C56-BQ56-BR56</f>
+        <v>-16</v>
+      </c>
     </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A57" s="27"/>
       <c r="B57" s="16"/>
       <c r="D57" s="34"/>
@@ -6325,20 +6439,21 @@
       <c r="BH57" s="46"/>
       <c r="BI57" s="45"/>
       <c r="BJ57" s="33"/>
-      <c r="BK57" s="46"/>
-      <c r="BL57" s="45"/>
-      <c r="BM57" s="46"/>
-      <c r="BN57" s="45"/>
-      <c r="BO57" s="46"/>
-      <c r="BP57" s="28"/>
-      <c r="BR57" s="10"/>
+      <c r="BK57" s="33"/>
+      <c r="BL57" s="46"/>
+      <c r="BM57" s="45"/>
+      <c r="BN57" s="46"/>
+      <c r="BO57" s="45"/>
+      <c r="BP57" s="46"/>
+      <c r="BQ57" s="28"/>
+      <c r="BS57" s="10"/>
     </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B58" s="51" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D58" s="34"/>
       <c r="E58" s="35"/>
@@ -6399,20 +6514,21 @@
       <c r="BH58" s="46"/>
       <c r="BI58" s="45"/>
       <c r="BJ58" s="33"/>
-      <c r="BK58" s="46"/>
-      <c r="BL58" s="45"/>
-      <c r="BM58" s="46"/>
-      <c r="BN58" s="45"/>
-      <c r="BO58" s="46"/>
-      <c r="BP58" s="28"/>
-      <c r="BR58" s="10"/>
+      <c r="BK58" s="33"/>
+      <c r="BL58" s="46"/>
+      <c r="BM58" s="45"/>
+      <c r="BN58" s="46"/>
+      <c r="BO58" s="45"/>
+      <c r="BP58" s="46"/>
+      <c r="BQ58" s="28"/>
+      <c r="BS58" s="10"/>
     </row>
-    <row r="59" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C59" s="8">
         <v>20</v>
@@ -6476,25 +6592,25 @@
       <c r="BH59" s="46"/>
       <c r="BI59" s="45"/>
       <c r="BJ59" s="33"/>
-      <c r="BK59" s="46"/>
-      <c r="BL59" s="45"/>
-      <c r="BM59" s="46"/>
-      <c r="BN59" s="45"/>
-      <c r="BO59" s="46"/>
-      <c r="BP59" s="8">
-        <f>SUM(D59:BO59)</f>
+      <c r="BK59" s="33"/>
+      <c r="BL59" s="46"/>
+      <c r="BM59" s="45"/>
+      <c r="BN59" s="46"/>
+      <c r="BO59" s="45"/>
+      <c r="BP59" s="46"/>
+      <c r="BQ59" s="8">
+        <f>SUM(D59:BP59)</f>
         <v>0</v>
       </c>
-      <c r="BQ59" s="8">
-        <f>C59-BP59</f>
+      <c r="BR59" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS59" s="10">
+        <f>C59-BQ59-BR59</f>
         <v>20</v>
       </c>
-      <c r="BR59" s="10">
-        <f>C59-BP59-BQ59</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="60" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="16"/>
       <c r="D60" s="34"/>
@@ -6556,20 +6672,21 @@
       <c r="BH60" s="46"/>
       <c r="BI60" s="45"/>
       <c r="BJ60" s="33"/>
-      <c r="BK60" s="46"/>
-      <c r="BL60" s="45"/>
-      <c r="BM60" s="46"/>
-      <c r="BN60" s="45"/>
-      <c r="BO60" s="46"/>
-      <c r="BP60" s="28"/>
-      <c r="BR60" s="10"/>
+      <c r="BK60" s="33"/>
+      <c r="BL60" s="46"/>
+      <c r="BM60" s="45"/>
+      <c r="BN60" s="46"/>
+      <c r="BO60" s="45"/>
+      <c r="BP60" s="46"/>
+      <c r="BQ60" s="28"/>
+      <c r="BS60" s="10"/>
     </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B61" s="51" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C61" s="8">
         <v>30</v>
@@ -6643,25 +6760,25 @@
       <c r="BH61" s="46"/>
       <c r="BI61" s="45"/>
       <c r="BJ61" s="33"/>
-      <c r="BK61" s="46"/>
-      <c r="BL61" s="45"/>
-      <c r="BM61" s="46"/>
-      <c r="BN61" s="45"/>
-      <c r="BO61" s="46"/>
-      <c r="BP61" s="8">
-        <f>SUM(D61:BO61)</f>
+      <c r="BK61" s="33"/>
+      <c r="BL61" s="46"/>
+      <c r="BM61" s="45"/>
+      <c r="BN61" s="46"/>
+      <c r="BO61" s="45"/>
+      <c r="BP61" s="46"/>
+      <c r="BQ61" s="8">
+        <f>SUM(D61:BP61)</f>
         <v>16</v>
       </c>
-      <c r="BQ61" s="8">
-        <f>C61-BP61</f>
+      <c r="BR61" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS61" s="10">
+        <f>C61-BQ61-BR61</f>
         <v>14</v>
       </c>
-      <c r="BR61" s="10">
-        <f>C61-BP61-BQ61</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="16"/>
       <c r="D62" s="34"/>
@@ -6723,15 +6840,16 @@
       <c r="BH62" s="46"/>
       <c r="BI62" s="45"/>
       <c r="BJ62" s="33"/>
-      <c r="BK62" s="46"/>
-      <c r="BL62" s="45"/>
-      <c r="BM62" s="46"/>
-      <c r="BN62" s="45"/>
-      <c r="BO62" s="46"/>
-      <c r="BP62" s="28"/>
-      <c r="BR62" s="10"/>
+      <c r="BK62" s="33"/>
+      <c r="BL62" s="46"/>
+      <c r="BM62" s="45"/>
+      <c r="BN62" s="46"/>
+      <c r="BO62" s="45"/>
+      <c r="BP62" s="46"/>
+      <c r="BQ62" s="28"/>
+      <c r="BS62" s="10"/>
     </row>
-    <row r="63" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
         <v>30</v>
       </c>
@@ -6798,20 +6916,21 @@
       <c r="BH63" s="67"/>
       <c r="BI63" s="69"/>
       <c r="BJ63" s="66"/>
-      <c r="BK63" s="67"/>
-      <c r="BL63" s="69"/>
-      <c r="BM63" s="67"/>
-      <c r="BN63" s="69"/>
-      <c r="BO63" s="67"/>
-      <c r="BP63" s="17"/>
-      <c r="BR63" s="13"/>
+      <c r="BK63" s="66"/>
+      <c r="BL63" s="67"/>
+      <c r="BM63" s="69"/>
+      <c r="BN63" s="67"/>
+      <c r="BO63" s="69"/>
+      <c r="BP63" s="67"/>
+      <c r="BQ63" s="17"/>
+      <c r="BS63" s="13"/>
     </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C64" s="8">
         <v>20</v>
@@ -6877,30 +6996,32 @@
       <c r="BH64" s="46"/>
       <c r="BI64" s="45"/>
       <c r="BJ64" s="33"/>
-      <c r="BK64" s="46"/>
-      <c r="BL64" s="45"/>
-      <c r="BM64" s="46"/>
-      <c r="BN64" s="45"/>
-      <c r="BO64" s="46"/>
-      <c r="BP64" s="8">
-        <f>SUM(D64:BO64)</f>
-        <v>1.5</v>
-      </c>
-      <c r="BQ64" s="31">
-        <f>C64-BP64</f>
-        <v>18.5</v>
-      </c>
-      <c r="BR64" s="10">
-        <f>C64-BP64-BQ64</f>
+      <c r="BK64" s="33"/>
+      <c r="BL64" s="46"/>
+      <c r="BM64" s="45">
+        <v>5</v>
+      </c>
+      <c r="BN64" s="46"/>
+      <c r="BO64" s="45"/>
+      <c r="BP64" s="46"/>
+      <c r="BQ64" s="8">
+        <f>SUM(D64:BP64)</f>
+        <v>6.5</v>
+      </c>
+      <c r="BR64" s="31">
         <v>0</v>
       </c>
+      <c r="BS64" s="10">
+        <f>C64-BQ64-BR64</f>
+        <v>13.5</v>
+      </c>
     </row>
-    <row r="65" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C65" s="8">
         <v>10</v>
@@ -6929,7 +7050,7 @@
         <v>8</v>
       </c>
       <c r="Y65" s="39">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z65" s="59">
         <v>3</v>
@@ -6970,29 +7091,30 @@
       <c r="BH65" s="46"/>
       <c r="BI65" s="45"/>
       <c r="BJ65" s="33"/>
-      <c r="BK65" s="46"/>
-      <c r="BL65" s="45"/>
-      <c r="BM65" s="46"/>
-      <c r="BN65" s="45"/>
-      <c r="BO65" s="46"/>
-      <c r="BP65" s="8">
-        <f>SUM(D65:BO65)</f>
-        <v>14</v>
-      </c>
+      <c r="BK65" s="33"/>
+      <c r="BL65" s="46"/>
+      <c r="BM65" s="45"/>
+      <c r="BN65" s="46"/>
+      <c r="BO65" s="45"/>
+      <c r="BP65" s="46"/>
       <c r="BQ65" s="8">
+        <f>SUM(D65:BP65)</f>
+        <v>16</v>
+      </c>
+      <c r="BR65" s="8">
         <v>0</v>
       </c>
-      <c r="BR65" s="10">
-        <f>C65-BP65-BQ65</f>
-        <v>-4</v>
+      <c r="BS65" s="10">
+        <f>C65-BQ65-BR65</f>
+        <v>-6</v>
       </c>
     </row>
-    <row r="66" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C66" s="8">
         <v>40</v>
@@ -7052,7 +7174,7 @@
       <c r="BD66" s="45"/>
       <c r="BE66" s="33"/>
       <c r="BF66" s="40">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="BG66" s="42">
         <v>8</v>
@@ -7061,28 +7183,38 @@
         <v>8</v>
       </c>
       <c r="BI66" s="42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BJ66" s="39"/>
-      <c r="BK66" s="46"/>
-      <c r="BL66" s="45"/>
-      <c r="BM66" s="46"/>
-      <c r="BN66" s="45"/>
-      <c r="BO66" s="46"/>
-      <c r="BP66" s="8">
-        <f>SUM(D66:BO66)</f>
-        <v>25</v>
+      <c r="BK66" s="39">
+        <v>6</v>
+      </c>
+      <c r="BL66" s="46">
+        <v>8</v>
+      </c>
+      <c r="BM66" s="45"/>
+      <c r="BN66" s="46">
+        <v>2</v>
+      </c>
+      <c r="BO66" s="45">
+        <v>9</v>
+      </c>
+      <c r="BP66" s="46">
+        <v>4</v>
       </c>
       <c r="BQ66" s="8">
-        <f>C66-BP66</f>
-        <v>15</v>
-      </c>
-      <c r="BR66" s="10">
-        <f>C66-BP66-BQ66</f>
+        <f>SUM(D66:BP66)</f>
+        <v>57</v>
+      </c>
+      <c r="BR66" s="8">
         <v>0</v>
       </c>
+      <c r="BS66" s="10">
+        <f>C66-BQ66-BR66</f>
+        <v>-17</v>
+      </c>
     </row>
-    <row r="67" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>35</v>
       </c>
@@ -7151,25 +7283,25 @@
       <c r="BH67" s="46"/>
       <c r="BI67" s="45"/>
       <c r="BJ67" s="39"/>
-      <c r="BK67" s="40"/>
-      <c r="BL67" s="45"/>
-      <c r="BM67" s="46"/>
-      <c r="BN67" s="45"/>
-      <c r="BO67" s="46"/>
-      <c r="BP67" s="8">
-        <f>SUM(D67:BO67)</f>
+      <c r="BK67" s="39"/>
+      <c r="BL67" s="40"/>
+      <c r="BM67" s="45"/>
+      <c r="BN67" s="46"/>
+      <c r="BO67" s="45"/>
+      <c r="BP67" s="46"/>
+      <c r="BQ67" s="8">
+        <f>SUM(D67:BP67)</f>
         <v>0</v>
       </c>
-      <c r="BQ67" s="8">
-        <f>C67-BP67</f>
+      <c r="BR67" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS67" s="10">
+        <f>C67-BQ67-BR67</f>
         <v>5</v>
       </c>
-      <c r="BR67" s="10">
-        <f>C67-BP67-BQ67</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="68" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="14"/>
       <c r="D68" s="34"/>
@@ -7231,17 +7363,18 @@
       <c r="BH68" s="46"/>
       <c r="BI68" s="45"/>
       <c r="BJ68" s="39"/>
-      <c r="BK68" s="40"/>
-      <c r="BL68" s="45"/>
-      <c r="BM68" s="46"/>
-      <c r="BN68" s="45"/>
-      <c r="BO68" s="46"/>
-      <c r="BR68" s="10"/>
+      <c r="BK68" s="39"/>
+      <c r="BL68" s="40"/>
+      <c r="BM68" s="45"/>
+      <c r="BN68" s="46"/>
+      <c r="BO68" s="45"/>
+      <c r="BP68" s="46"/>
+      <c r="BS68" s="10"/>
     </row>
-    <row r="69" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="14" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D69" s="34">
         <v>0.5</v>
@@ -7305,52 +7438,56 @@
       <c r="AK69" s="45"/>
       <c r="AL69" s="46"/>
       <c r="AM69" s="45"/>
-      <c r="AN69" s="81">
+      <c r="AN69" s="77">
         <v>0.5</v>
       </c>
-      <c r="AO69" s="79"/>
+      <c r="AO69" s="75"/>
       <c r="AP69" s="46"/>
       <c r="AQ69" s="45"/>
       <c r="AR69" s="46"/>
       <c r="AS69" s="45"/>
-      <c r="AT69" s="34">
+      <c r="AT69" s="77">
         <v>0.5</v>
       </c>
-      <c r="AU69" s="33"/>
+      <c r="AU69" s="75"/>
       <c r="AV69" s="46"/>
       <c r="AW69" s="45"/>
       <c r="AX69" s="46"/>
       <c r="AY69" s="45"/>
-      <c r="AZ69" s="33"/>
+      <c r="AZ69" s="33">
+        <v>0.5</v>
+      </c>
       <c r="BA69" s="46"/>
       <c r="BB69" s="45"/>
       <c r="BC69" s="46"/>
       <c r="BD69" s="45"/>
-      <c r="BE69" s="33"/>
+      <c r="BE69" s="33">
+        <v>0.5</v>
+      </c>
       <c r="BF69" s="46"/>
       <c r="BG69" s="45"/>
       <c r="BH69" s="46"/>
       <c r="BI69" s="45"/>
       <c r="BJ69" s="39"/>
-      <c r="BK69" s="40"/>
-      <c r="BL69" s="45"/>
-      <c r="BM69" s="46"/>
-      <c r="BN69" s="45"/>
-      <c r="BO69" s="46"/>
-      <c r="BP69" s="8">
-        <f>SUM(D69:BO69)</f>
-        <v>7.5</v>
-      </c>
+      <c r="BK69" s="39"/>
+      <c r="BL69" s="40"/>
+      <c r="BM69" s="45"/>
+      <c r="BN69" s="46"/>
+      <c r="BO69" s="45"/>
+      <c r="BP69" s="46"/>
       <c r="BQ69" s="8">
-        <f>C69-BP69</f>
-        <v>-7.5</v>
-      </c>
-      <c r="BR69" s="10">
-        <f>C69-BP69-BQ69</f>
+        <f>SUM(D69:BP69)</f>
+        <v>8.5</v>
+      </c>
+      <c r="BR69" s="8">
         <v>0</v>
       </c>
+      <c r="BS69" s="10">
+        <f>C69-BQ69-BR69</f>
+        <v>-8.5</v>
+      </c>
     </row>
-    <row r="70" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="D70" s="34"/>
       <c r="E70" s="35"/>
@@ -7407,18 +7544,21 @@
       <c r="BD70" s="45"/>
       <c r="BE70" s="33"/>
       <c r="BF70" s="46"/>
-      <c r="BG70" s="45"/>
+      <c r="BG70" s="45" t="s">
+        <v>92</v>
+      </c>
       <c r="BH70" s="46"/>
       <c r="BI70" s="45"/>
       <c r="BJ70" s="33"/>
-      <c r="BK70" s="46"/>
-      <c r="BL70" s="45"/>
-      <c r="BM70" s="46"/>
-      <c r="BN70" s="45"/>
-      <c r="BO70" s="46"/>
-      <c r="BR70" s="10"/>
+      <c r="BK70" s="33"/>
+      <c r="BL70" s="46"/>
+      <c r="BM70" s="45"/>
+      <c r="BN70" s="46"/>
+      <c r="BO70" s="45"/>
+      <c r="BP70" s="46"/>
+      <c r="BS70" s="10"/>
     </row>
-    <row r="71" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:71" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>37</v>
       </c>
@@ -7467,7 +7607,7 @@
       <c r="AL71" s="46"/>
       <c r="AM71" s="45"/>
       <c r="AN71" s="33"/>
-      <c r="AO71" s="79"/>
+      <c r="AO71" s="75"/>
       <c r="AP71" s="46"/>
       <c r="AQ71" s="45"/>
       <c r="AR71" s="46"/>
@@ -7489,27 +7629,27 @@
       <c r="BH71" s="46"/>
       <c r="BI71" s="45"/>
       <c r="BJ71" s="33"/>
-      <c r="BK71" s="46"/>
-      <c r="BL71" s="45"/>
-      <c r="BM71" s="46"/>
-      <c r="BN71" s="45"/>
-      <c r="BO71" s="46"/>
-      <c r="BP71" s="8">
-        <f>SUM(D71:BO71)</f>
+      <c r="BK71" s="33"/>
+      <c r="BL71" s="46"/>
+      <c r="BM71" s="45"/>
+      <c r="BN71" s="46"/>
+      <c r="BO71" s="45"/>
+      <c r="BP71" s="46"/>
+      <c r="BQ71" s="8">
+        <f>SUM(D71:BP71)</f>
         <v>6</v>
       </c>
-      <c r="BQ71" s="8">
-        <f>C71-BP71</f>
+      <c r="BR71" s="8">
+        <v>0</v>
+      </c>
+      <c r="BS71" s="10">
+        <f>C71-BQ71-BR71</f>
         <v>84</v>
       </c>
-      <c r="BR71" s="10">
-        <f>C71-BP71-BQ71</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="72" spans="1:70" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:71" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
-      <c r="C72" s="18"/>
+      <c r="C72" s="80"/>
       <c r="D72" s="34"/>
       <c r="E72" s="35"/>
       <c r="F72" s="59"/>
@@ -7542,456 +7682,214 @@
       <c r="AG72" s="33"/>
       <c r="AH72" s="59"/>
       <c r="AI72" s="33"/>
-      <c r="AJ72" s="46"/>
-      <c r="AK72" s="45"/>
-      <c r="AL72" s="46"/>
-      <c r="AM72" s="45"/>
-      <c r="AN72" s="33"/>
-      <c r="AO72" s="79"/>
-      <c r="AP72" s="46"/>
-      <c r="AQ72" s="45"/>
-      <c r="AR72" s="46"/>
-      <c r="AS72" s="45"/>
-      <c r="AT72" s="33"/>
-      <c r="AU72" s="33"/>
-      <c r="AV72" s="46"/>
-      <c r="AW72" s="45"/>
-      <c r="AX72" s="46"/>
-      <c r="AY72" s="45"/>
-      <c r="AZ72" s="33"/>
-      <c r="BA72" s="46"/>
-      <c r="BB72" s="45"/>
-      <c r="BC72" s="46"/>
-      <c r="BD72" s="45"/>
-      <c r="BE72" s="33"/>
-      <c r="BF72" s="46"/>
-      <c r="BG72" s="45"/>
-      <c r="BH72" s="46"/>
-      <c r="BI72" s="45"/>
-      <c r="BJ72" s="33"/>
-      <c r="BK72" s="46"/>
-      <c r="BL72" s="45"/>
-      <c r="BM72" s="46"/>
-      <c r="BN72" s="45"/>
-      <c r="BO72" s="46"/>
+      <c r="AJ72" s="79"/>
+      <c r="AK72" s="69"/>
+      <c r="AL72" s="67"/>
+      <c r="AM72" s="69"/>
+      <c r="AN72" s="66"/>
+      <c r="AO72" s="76"/>
+      <c r="AP72" s="67"/>
+      <c r="AQ72" s="69"/>
+      <c r="AR72" s="67"/>
+      <c r="AS72" s="69"/>
+      <c r="AT72" s="66"/>
+      <c r="AU72" s="66"/>
+      <c r="AV72" s="67"/>
+      <c r="AW72" s="69"/>
+      <c r="AX72" s="67"/>
+      <c r="AY72" s="69"/>
+      <c r="AZ72" s="66"/>
+      <c r="BA72" s="67"/>
+      <c r="BB72" s="69"/>
+      <c r="BC72" s="67"/>
+      <c r="BD72" s="69"/>
+      <c r="BE72" s="66"/>
+      <c r="BF72" s="67"/>
+      <c r="BG72" s="69"/>
+      <c r="BH72" s="67"/>
+      <c r="BI72" s="69"/>
+      <c r="BJ72" s="66"/>
+      <c r="BK72" s="66"/>
+      <c r="BL72" s="67"/>
+      <c r="BM72" s="69"/>
+      <c r="BN72" s="67"/>
+      <c r="BO72" s="69"/>
+      <c r="BP72" s="67"/>
+      <c r="BQ72" s="12"/>
+      <c r="BR72" s="12"/>
+      <c r="BS72" s="13"/>
     </row>
-    <row r="73" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A73" s="6"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="59"/>
-      <c r="G73" s="33"/>
-      <c r="H73" s="59"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="46"/>
-      <c r="K73" s="35"/>
-      <c r="L73" s="32"/>
-      <c r="M73" s="33"/>
-      <c r="N73" s="59"/>
-      <c r="O73" s="33"/>
-      <c r="P73" s="59"/>
-      <c r="Q73" s="33"/>
-      <c r="R73" s="59"/>
-      <c r="S73" s="33"/>
-      <c r="T73" s="59"/>
-      <c r="U73" s="33"/>
-      <c r="V73" s="59"/>
-      <c r="W73" s="33"/>
-      <c r="X73" s="59"/>
-      <c r="Y73" s="33"/>
-      <c r="Z73" s="59"/>
-      <c r="AA73" s="33"/>
-      <c r="AB73" s="59"/>
-      <c r="AC73" s="33"/>
-      <c r="AD73" s="59"/>
-      <c r="AE73" s="33"/>
-      <c r="AF73" s="59"/>
-      <c r="AG73" s="33"/>
-      <c r="AH73" s="59"/>
-      <c r="AI73" s="33"/>
-      <c r="AJ73" s="46"/>
-      <c r="AK73" s="45"/>
-      <c r="AL73" s="46"/>
-      <c r="AM73" s="45"/>
-      <c r="AN73" s="33"/>
-      <c r="AO73" s="79"/>
-      <c r="AP73" s="46"/>
-      <c r="AQ73" s="45"/>
-      <c r="AR73" s="46"/>
-      <c r="AS73" s="45"/>
-      <c r="AT73" s="33"/>
-      <c r="AU73" s="33"/>
-      <c r="AV73" s="46"/>
-      <c r="AW73" s="45"/>
-      <c r="AX73" s="46"/>
-      <c r="AY73" s="45"/>
-      <c r="AZ73" s="33"/>
-      <c r="BA73" s="46"/>
-      <c r="BB73" s="45"/>
-      <c r="BC73" s="46"/>
-      <c r="BD73" s="45"/>
-      <c r="BE73" s="33"/>
-      <c r="BF73" s="46"/>
-      <c r="BG73" s="45"/>
-      <c r="BH73" s="46"/>
-      <c r="BI73" s="45"/>
-      <c r="BJ73" s="33"/>
-      <c r="BK73" s="46"/>
-      <c r="BL73" s="45"/>
-      <c r="BM73" s="46"/>
-      <c r="BN73" s="45"/>
-      <c r="BO73" s="46"/>
-      <c r="BR73" s="10"/>
+    <row r="73" spans="1:71" x14ac:dyDescent="0.3">
+      <c r="A73" s="19"/>
+      <c r="B73" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" s="21">
+        <f>SUM(C5:C13)+SUM(C16:C33)+SUM(C35:C62)+SUM(C64:C72)</f>
+        <v>476</v>
+      </c>
+      <c r="D73" s="89">
+        <f>SUM(D4:E72)</f>
+        <v>12.5</v>
+      </c>
+      <c r="E73" s="83"/>
+      <c r="F73" s="81">
+        <f>SUM(F4:G72)</f>
+        <v>7.5</v>
+      </c>
+      <c r="G73" s="83"/>
+      <c r="H73" s="81">
+        <f>SUM(H4:I72)</f>
+        <v>4.5</v>
+      </c>
+      <c r="I73" s="83"/>
+      <c r="J73" s="81">
+        <f>SUM(J4:K72)</f>
+        <v>0</v>
+      </c>
+      <c r="K73" s="83"/>
+      <c r="L73" s="81">
+        <f>SUM(L4:M72)</f>
+        <v>18</v>
+      </c>
+      <c r="M73" s="83"/>
+      <c r="N73" s="81">
+        <f>SUM(N4:O72)</f>
+        <v>12.5</v>
+      </c>
+      <c r="O73" s="83"/>
+      <c r="P73" s="81">
+        <f>SUM(P4:Q72)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Q73" s="83"/>
+      <c r="R73" s="81">
+        <f>SUM(R4:S72)</f>
+        <v>7.5</v>
+      </c>
+      <c r="S73" s="83"/>
+      <c r="T73" s="81">
+        <f>SUM(T4:U72)</f>
+        <v>10.5</v>
+      </c>
+      <c r="U73" s="83"/>
+      <c r="V73" s="81">
+        <f>SUM(V4:W72)</f>
+        <v>9.5</v>
+      </c>
+      <c r="W73" s="83"/>
+      <c r="X73" s="81">
+        <f>SUM(X4:Y72)</f>
+        <v>13.5</v>
+      </c>
+      <c r="Y73" s="83"/>
+      <c r="Z73" s="81">
+        <f>SUM(Z4:AA72)</f>
+        <v>17.5</v>
+      </c>
+      <c r="AA73" s="83"/>
+      <c r="AB73" s="81">
+        <f>SUM(AB4:AC72)</f>
+        <v>19.5</v>
+      </c>
+      <c r="AC73" s="83"/>
+      <c r="AD73" s="81">
+        <f>SUM(AD4:AE72)</f>
+        <v>12.5</v>
+      </c>
+      <c r="AE73" s="83"/>
+      <c r="AF73" s="81">
+        <f>SUM(AF4:AG72)</f>
+        <v>16</v>
+      </c>
+      <c r="AG73" s="82"/>
+      <c r="AH73" s="81">
+        <f>SUM(AH4:AI72)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AI73" s="82"/>
+      <c r="AJ73" s="81">
+        <f>SUM(AJ4:AO72)</f>
+        <v>48</v>
+      </c>
+      <c r="AK73" s="82"/>
+      <c r="AL73" s="82"/>
+      <c r="AM73" s="82"/>
+      <c r="AN73" s="82"/>
+      <c r="AO73" s="83"/>
+      <c r="AP73" s="81">
+        <f>SUM(AP4:AU72)</f>
+        <v>44</v>
+      </c>
+      <c r="AQ73" s="82"/>
+      <c r="AR73" s="82"/>
+      <c r="AS73" s="82"/>
+      <c r="AT73" s="82"/>
+      <c r="AU73" s="83"/>
+      <c r="AV73" s="81">
+        <f>SUM(AV4:AZ72)</f>
+        <v>43.5</v>
+      </c>
+      <c r="AW73" s="82"/>
+      <c r="AX73" s="82"/>
+      <c r="AY73" s="82"/>
+      <c r="AZ73" s="83"/>
+      <c r="BA73" s="84">
+        <f>SUM(BA4:BE72)</f>
+        <v>40.5</v>
+      </c>
+      <c r="BB73" s="85"/>
+      <c r="BC73" s="85"/>
+      <c r="BD73" s="85"/>
+      <c r="BE73" s="86"/>
+      <c r="BF73" s="84">
+        <f>SUM(BF4:BJ72)</f>
+        <v>30</v>
+      </c>
+      <c r="BG73" s="85"/>
+      <c r="BH73" s="85"/>
+      <c r="BI73" s="85"/>
+      <c r="BJ73" s="86"/>
+      <c r="BK73" s="81">
+        <f>SUM(BK4:BP72)</f>
+        <v>43</v>
+      </c>
+      <c r="BL73" s="82"/>
+      <c r="BM73" s="82"/>
+      <c r="BN73" s="82"/>
+      <c r="BO73" s="82"/>
+      <c r="BP73" s="83"/>
+      <c r="BQ73" s="21">
+        <f>SUM(BQ4:BQ72)</f>
+        <v>424.5</v>
+      </c>
+      <c r="BR73" s="21">
+        <f>SUM(BR4:BR72)</f>
+        <v>-3</v>
+      </c>
+      <c r="BS73" s="22">
+        <f>SUM(BS4:BS72)</f>
+        <v>54.5</v>
+      </c>
     </row>
-    <row r="74" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A74" s="6"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="35"/>
-      <c r="F74" s="59"/>
-      <c r="G74" s="33"/>
-      <c r="H74" s="59"/>
-      <c r="I74" s="33"/>
-      <c r="J74" s="46"/>
-      <c r="K74" s="35"/>
-      <c r="L74" s="32"/>
-      <c r="M74" s="33"/>
-      <c r="N74" s="59"/>
-      <c r="O74" s="33"/>
-      <c r="P74" s="59"/>
-      <c r="Q74" s="33"/>
-      <c r="R74" s="59"/>
-      <c r="S74" s="33"/>
-      <c r="T74" s="59"/>
-      <c r="U74" s="33"/>
-      <c r="V74" s="59"/>
-      <c r="W74" s="33"/>
-      <c r="X74" s="59"/>
-      <c r="Y74" s="33"/>
-      <c r="Z74" s="59"/>
-      <c r="AA74" s="33"/>
-      <c r="AB74" s="59"/>
-      <c r="AC74" s="33"/>
-      <c r="AD74" s="59"/>
-      <c r="AE74" s="33"/>
-      <c r="AF74" s="59"/>
-      <c r="AG74" s="33"/>
-      <c r="AH74" s="59"/>
-      <c r="AI74" s="33"/>
-      <c r="AJ74" s="46"/>
-      <c r="AK74" s="45"/>
-      <c r="AL74" s="46"/>
-      <c r="AM74" s="45"/>
-      <c r="AN74" s="33"/>
-      <c r="AO74" s="79"/>
-      <c r="AP74" s="46"/>
-      <c r="AQ74" s="45"/>
-      <c r="AR74" s="46"/>
-      <c r="AS74" s="45"/>
-      <c r="AT74" s="33"/>
-      <c r="AU74" s="33"/>
-      <c r="AV74" s="46"/>
-      <c r="AW74" s="45"/>
-      <c r="AX74" s="46"/>
-      <c r="AY74" s="45"/>
-      <c r="AZ74" s="33"/>
-      <c r="BA74" s="46"/>
-      <c r="BB74" s="45"/>
-      <c r="BC74" s="46"/>
-      <c r="BD74" s="45"/>
-      <c r="BE74" s="33"/>
-      <c r="BF74" s="46"/>
-      <c r="BG74" s="45"/>
-      <c r="BH74" s="46"/>
-      <c r="BI74" s="45"/>
-      <c r="BJ74" s="33"/>
-      <c r="BK74" s="46"/>
-      <c r="BL74" s="45"/>
-      <c r="BM74" s="46"/>
-      <c r="BN74" s="45"/>
-      <c r="BO74" s="46"/>
-      <c r="BP74" s="8">
-        <f>SUM(D74:BO74)</f>
-        <v>0</v>
-      </c>
-      <c r="BQ74" s="8">
-        <f>C74-BP74</f>
-        <v>0</v>
-      </c>
-      <c r="BR74" s="10">
-        <f>C74-BP74-BQ74</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:70" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="11"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="63"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="65"/>
-      <c r="G75" s="66"/>
-      <c r="H75" s="65"/>
-      <c r="I75" s="66"/>
-      <c r="J75" s="67"/>
-      <c r="K75" s="35"/>
-      <c r="L75" s="65"/>
-      <c r="M75" s="66"/>
-      <c r="N75" s="65"/>
-      <c r="O75" s="66"/>
-      <c r="P75" s="65"/>
-      <c r="Q75" s="66"/>
-      <c r="R75" s="65"/>
-      <c r="S75" s="66"/>
-      <c r="T75" s="65"/>
-      <c r="U75" s="66"/>
-      <c r="V75" s="65"/>
-      <c r="W75" s="66"/>
-      <c r="X75" s="65"/>
-      <c r="Y75" s="66"/>
-      <c r="Z75" s="65"/>
-      <c r="AA75" s="66"/>
-      <c r="AB75" s="65"/>
-      <c r="AC75" s="66"/>
-      <c r="AD75" s="65"/>
-      <c r="AE75" s="66"/>
-      <c r="AF75" s="65"/>
-      <c r="AG75" s="66"/>
-      <c r="AH75" s="65"/>
-      <c r="AI75" s="66"/>
-      <c r="AJ75" s="67"/>
-      <c r="AK75" s="69"/>
-      <c r="AL75" s="67"/>
-      <c r="AM75" s="69"/>
-      <c r="AN75" s="66"/>
-      <c r="AO75" s="80"/>
-      <c r="AP75" s="67"/>
-      <c r="AQ75" s="69"/>
-      <c r="AR75" s="67"/>
-      <c r="AS75" s="69"/>
-      <c r="AT75" s="66"/>
-      <c r="AU75" s="83"/>
-      <c r="AV75" s="67"/>
-      <c r="AW75" s="69"/>
-      <c r="AX75" s="67"/>
-      <c r="AY75" s="69"/>
-      <c r="AZ75" s="66"/>
-      <c r="BA75" s="67"/>
-      <c r="BB75" s="69"/>
-      <c r="BC75" s="67"/>
-      <c r="BD75" s="69"/>
-      <c r="BE75" s="66"/>
-      <c r="BF75" s="67"/>
-      <c r="BG75" s="69"/>
-      <c r="BH75" s="67"/>
-      <c r="BI75" s="69"/>
-      <c r="BJ75" s="66"/>
-      <c r="BK75" s="67"/>
-      <c r="BL75" s="69"/>
-      <c r="BM75" s="67"/>
-      <c r="BN75" s="69"/>
-      <c r="BO75" s="67"/>
-      <c r="BP75" s="12"/>
-      <c r="BQ75" s="12"/>
-      <c r="BR75" s="13"/>
-    </row>
-    <row r="76" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="A76" s="19"/>
-      <c r="B76" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C76" s="21">
-        <f>SUM(C5:C13)+SUM(C16:C33)+SUM(C37:C62)+SUM(C64:C75)</f>
-        <v>466</v>
-      </c>
-      <c r="D76" s="101">
-        <f>SUM(D4:E75)</f>
-        <v>10.5</v>
-      </c>
-      <c r="E76" s="102"/>
-      <c r="F76" s="103">
-        <f>SUM(F4:G75)</f>
-        <v>7.5</v>
-      </c>
-      <c r="G76" s="102"/>
-      <c r="H76" s="103">
-        <f>SUM(H4:I75)</f>
-        <v>4.5</v>
-      </c>
-      <c r="I76" s="102"/>
-      <c r="J76" s="103">
-        <f>SUM(J4:K75)</f>
-        <v>0</v>
-      </c>
-      <c r="K76" s="102"/>
-      <c r="L76" s="103">
-        <f>SUM(L4:M75)</f>
-        <v>18</v>
-      </c>
-      <c r="M76" s="102"/>
-      <c r="N76" s="103">
-        <f>SUM(N4:O75)</f>
-        <v>11.5</v>
-      </c>
-      <c r="O76" s="102"/>
-      <c r="P76" s="103">
-        <f>SUM(P4:Q75)</f>
-        <v>11.5</v>
-      </c>
-      <c r="Q76" s="102"/>
-      <c r="R76" s="103">
-        <f>SUM(R4:S75)</f>
-        <v>4.5</v>
-      </c>
-      <c r="S76" s="102"/>
-      <c r="T76" s="103">
-        <f>SUM(T4:U75)</f>
-        <v>7.5</v>
-      </c>
-      <c r="U76" s="102"/>
-      <c r="V76" s="103">
-        <f>SUM(V4:W75)</f>
-        <v>9.5</v>
-      </c>
-      <c r="W76" s="102"/>
-      <c r="X76" s="103">
-        <f>SUM(X4:Y75)</f>
-        <v>11.5</v>
-      </c>
-      <c r="Y76" s="102"/>
-      <c r="Z76" s="103">
-        <f>SUM(Z4:AA75)</f>
-        <v>17.5</v>
-      </c>
-      <c r="AA76" s="102"/>
-      <c r="AB76" s="103">
-        <f>SUM(AB4:AC75)</f>
-        <v>19.5</v>
-      </c>
-      <c r="AC76" s="102"/>
-      <c r="AD76" s="103">
-        <f>SUM(AD4:AE75)</f>
-        <v>12.5</v>
-      </c>
-      <c r="AE76" s="102"/>
-      <c r="AF76" s="103">
-        <f>SUM(AF4:AG75)</f>
-        <v>16</v>
-      </c>
-      <c r="AG76" s="109"/>
-      <c r="AH76" s="103">
-        <f>SUM(AH4:AI75)</f>
-        <v>0.5</v>
-      </c>
-      <c r="AI76" s="109"/>
-      <c r="AJ76" s="103">
-        <f>SUM(AJ4:AO75)</f>
-        <v>48</v>
-      </c>
-      <c r="AK76" s="107"/>
-      <c r="AL76" s="107"/>
-      <c r="AM76" s="107"/>
-      <c r="AN76" s="108"/>
-      <c r="AO76" s="75"/>
-      <c r="AP76" s="103">
-        <f>SUM(AP4:AU75)</f>
-        <v>44</v>
-      </c>
-      <c r="AQ76" s="107"/>
-      <c r="AR76" s="107"/>
-      <c r="AS76" s="107"/>
-      <c r="AT76" s="108"/>
-      <c r="AU76" s="78"/>
-      <c r="AV76" s="103">
-        <f>SUM(AV4:AZ75)</f>
-        <v>43</v>
-      </c>
-      <c r="AW76" s="107"/>
-      <c r="AX76" s="107"/>
-      <c r="AY76" s="107"/>
-      <c r="AZ76" s="108"/>
-      <c r="BA76" s="103">
-        <f>SUM(BA4:BE75)</f>
-        <v>40</v>
-      </c>
-      <c r="BB76" s="107"/>
-      <c r="BC76" s="107"/>
-      <c r="BD76" s="107"/>
-      <c r="BE76" s="108"/>
-      <c r="BF76" s="103">
-        <f>SUM(BF4:BJ75)</f>
-        <v>27</v>
-      </c>
-      <c r="BG76" s="107"/>
-      <c r="BH76" s="107"/>
-      <c r="BI76" s="107"/>
-      <c r="BJ76" s="108"/>
-      <c r="BK76" s="103">
-        <f>SUM(BK4:BO75)</f>
-        <v>0</v>
-      </c>
-      <c r="BL76" s="107"/>
-      <c r="BM76" s="107"/>
-      <c r="BN76" s="107"/>
-      <c r="BO76" s="108"/>
-      <c r="BP76" s="21">
-        <f>SUM(BP4:BP75)</f>
-        <v>358.5</v>
-      </c>
-      <c r="BQ76" s="21">
-        <f>SUM(BQ4:BQ75)</f>
-        <v>152.5</v>
-      </c>
-      <c r="BR76" s="22">
-        <f>SUM(BR4:BR75)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="77" spans="1:70" x14ac:dyDescent="0.3">
-      <c r="I77" s="24"/>
+    <row r="74" spans="1:71" x14ac:dyDescent="0.3">
+      <c r="I74" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="AP76:AT76"/>
-    <mergeCell ref="AV76:AZ76"/>
-    <mergeCell ref="BA76:BE76"/>
-    <mergeCell ref="BF76:BJ76"/>
-    <mergeCell ref="BK76:BO76"/>
-    <mergeCell ref="AJ76:AN76"/>
-    <mergeCell ref="N76:O76"/>
-    <mergeCell ref="P76:Q76"/>
-    <mergeCell ref="R76:S76"/>
-    <mergeCell ref="T76:U76"/>
-    <mergeCell ref="V76:W76"/>
-    <mergeCell ref="X76:Y76"/>
-    <mergeCell ref="Z76:AA76"/>
-    <mergeCell ref="AB76:AC76"/>
-    <mergeCell ref="AD76:AE76"/>
-    <mergeCell ref="AF76:AG76"/>
-    <mergeCell ref="AH76:AI76"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AV3:AZ3"/>
+    <mergeCell ref="BK73:BP73"/>
+    <mergeCell ref="BK3:BP3"/>
+    <mergeCell ref="AO3:AT3"/>
+    <mergeCell ref="AU3:AZ3"/>
+    <mergeCell ref="AJ73:AO73"/>
+    <mergeCell ref="AP73:AU73"/>
     <mergeCell ref="BA3:BE3"/>
     <mergeCell ref="BF3:BJ3"/>
-    <mergeCell ref="BK3:BO3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="L76:M76"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D1:BO1"/>
-    <mergeCell ref="BR1:BR3"/>
-    <mergeCell ref="D2:BO2"/>
+    <mergeCell ref="D1:BP1"/>
+    <mergeCell ref="BS1:BS3"/>
+    <mergeCell ref="D2:BP2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
@@ -8003,8 +7901,33 @@
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="V3:W3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="H73:I73"/>
+    <mergeCell ref="J73:K73"/>
+    <mergeCell ref="L73:M73"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="N73:O73"/>
+    <mergeCell ref="P73:Q73"/>
+    <mergeCell ref="R73:S73"/>
+    <mergeCell ref="T73:U73"/>
+    <mergeCell ref="V73:W73"/>
+    <mergeCell ref="AH73:AI73"/>
+    <mergeCell ref="AV73:AZ73"/>
+    <mergeCell ref="BA73:BE73"/>
+    <mergeCell ref="BF73:BJ73"/>
+    <mergeCell ref="X73:Y73"/>
+    <mergeCell ref="Z73:AA73"/>
+    <mergeCell ref="AB73:AC73"/>
+    <mergeCell ref="AD73:AE73"/>
+    <mergeCell ref="AF73:AG73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="63" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="59" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>